<commit_message>
re generate files for judging after removing redundant sentences
</commit_message>
<xml_diff>
--- a/sentence_level/data/sentences/remove_single/2012_leap_day_tornado.xlsx
+++ b/sentence_level/data/sentences/remove_single/2012_leap_day_tornado.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="210">
   <si>
     <t>2012_leap_day_tornado</t>
   </si>
@@ -31,25 +31,496 @@
     <t>IEMA regional personnel were deployed to Harrisburg soon after the storms and representatives from the Illinois State Police, departments of Transportation, Central Management Services, Corrections, Public Health and Natural Resources, along with the American Red Cross, reported to the SEOC soon thereafter.</t>
   </si>
   <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>In northern Oklahoma, gusts of up to 80 mph flipped trailers and damaged homes near Cherokee.</t>
+  </si>
+  <si>
+    <t>Leap Day was not a good one for thousands of people in the Midwest and Southern United States as severe storms and tornadoes left a trail of destruction in Illinois, Missouri, Kansas, Arkansas, Oklahoma, Kentucky, and Tennessee.</t>
+  </si>
+  <si>
+    <t>Eldorado</t>
+  </si>
+  <si>
+    <t>They are Mary Osman, 75, of Harrisburg, Jaylynn Ferrell, 22, of Harrisburg, Lynda Hull, 74, of Galatia, Donna Rann, 61, of Eldorado, and Randy Rann, 64, of Eldorado.</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Many people are asking how they can help after a preliminary EF4 tornado hit Saline County, Illinois killing six people.</t>
+  </si>
+  <si>
+    <t>Quinn directed the Illinois Emergency Management Agency to activate the State Emergency Operations Center (SEOC) in Springfield.</t>
+  </si>
+  <si>
+    <t>At least 13 dead in storms working across Missouri, Illinois.</t>
+  </si>
+  <si>
+    <t>But none faced the wrath of Mother Nature like the southern Illinois town of Harrisburg.</t>
+  </si>
+  <si>
+    <t>From Tuesday night into Wednesday morning, at least 16 tornado sightings were reported from Nebraska and Kansas across southern Missouri to Illinois and Kentucky, according to the storm center, an arm of the National Weather Service.</t>
+  </si>
+  <si>
+    <t>Quinn says he's already talked to President Obama and that Illinois is banding together as a family to help Harrisburg recover and rebuild.</t>
+  </si>
+  <si>
+    <t>It is the deadliest state disaster in Illinois in nearly a decade.</t>
+  </si>
+  <si>
+    <t>Pulaski County, Illinois EMS Director Ken Kerley says wreckers and vehicles were blown from their location and crossing arms broke off and blew into a squad car.</t>
+  </si>
+  <si>
+    <t>David Serby in Perry County, Illinois says a few outbuildings were blown over with some tree damage.</t>
+  </si>
+  <si>
+    <t>The United Way of South Central Illinois, located at 1101 Broadway in Mt.</t>
+  </si>
+  <si>
+    <t>At least 10 people were killed in the southern Illinois town of Harrisburg after a storm leveled much of the community of 9,000 people.</t>
+  </si>
+  <si>
+    <t>The Southern Illinois Egyptian Health Department says if you are experiencing a power outage:  -Keep your freezer/refrigerator door closed to maintain temperatures.</t>
+  </si>
+  <si>
+    <t>Illinois Gov.</t>
+  </si>
+  <si>
+    <t>Pulaski County</t>
+  </si>
+  <si>
+    <t>No injuries have been reported in Pulaski County.</t>
+  </si>
+  <si>
+    <t>Cape Girardeau County</t>
+  </si>
+  <si>
+    <t>Team 1 (Rick Shanklin, Ken Ludington) - Harrisburg west toward Cape Girardeau County MO  Team 2 (Kelly Hooper, Shane Luecke) - Newburg IN West toward Harrisburg IL)  Team 3 (Christine Wielgos, Debbie Hooper) - Metropolis IL west toward Stoddard co. MO)  Note this may change as storms are in western Kentucky.</t>
+  </si>
+  <si>
+    <t>in Cape Girardeau County.</t>
+  </si>
+  <si>
+    <t>Saline County</t>
+  </si>
+  <si>
+    <t>At least 100 people have been injured in the Harrisburg area, according to the Saline County Sheriff's Office.</t>
+  </si>
+  <si>
+    <t>Crews with Ameren Illinois have issued a safety warning to all residents in and around Saline County.</t>
+  </si>
+  <si>
+    <t>The National Weather Service reports an EF4 tornado hit Saline County on the southwest side of Harrisburg, killing six people.</t>
+  </si>
+  <si>
+    <t>Four females and two males, all adults, were killed in Saline County.</t>
+  </si>
+  <si>
+    <t>Saline County Emergency Management asks people to stay off their cell phones if possible as heavy phone traffic is jamming the system.</t>
+  </si>
+  <si>
+    <t>Stoddard County</t>
+  </si>
+  <si>
+    <t>A total of eight patients from Stoddard County are being treated at Saint Francis Medical Center.</t>
+  </si>
+  <si>
+    <t>One man has died after the storms in Stoddard County.</t>
+  </si>
+  <si>
+    <t>Stoddard County Sheriff Carl Hefner says several mobile homes in the area are destroyed in Stoddard County.</t>
+  </si>
+  <si>
+    <t>The Stoddard County coroner says Mark Champlin, 50, of Puxico was killed.</t>
+  </si>
+  <si>
+    <t>Highway Patrol Trooper Clark Parrott says large trees are down along Route M in Stoddard County.</t>
+  </si>
+  <si>
+    <t>You can drive for miles in Stoddard County and never see damage, but a path left from the strong winds that did blow through, show the wreckage.</t>
+  </si>
+  <si>
+    <t>man was killed in Stoddard County.</t>
+  </si>
+  <si>
+    <t>Hefner says they started receiving calls around 4 a.m.  Dale Moreland with Stoddard County EMA says one mobile home was moved about 200 feet.</t>
+  </si>
+  <si>
+    <t>They are all storm related injuries from Stoddard County.</t>
+  </si>
+  <si>
+    <t>A second tornado in Stoddard County Wednesday morning started just east of Bell City to three miles southeast of Benton, Mo.</t>
+  </si>
+  <si>
+    <t>Midwest</t>
+  </si>
+  <si>
+    <t>Disaster in the Heartland - one year later  Disaster in the Heartland - one year later  The storm drove this plywood piece through the wall of a garage in Harrisburg,  Seven people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
+  </si>
+  <si>
+    <t>How you can help after the tornadoes  How you can help after the tornadoes  Eight people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
+  </si>
+  <si>
+    <t>Three people were killed in Tennessee after the same severe weather system that created massive damage across the Midwest moved through the state.</t>
+  </si>
+  <si>
+    <t>Midwest Tornadoes: News, Photos, and Video of the Destruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDATED: At Least 12 People Killed In Deadly Midwest Storms. </t>
+  </si>
+  <si>
+    <t>Eight people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
+  </si>
+  <si>
+    <t>FEMA</t>
+  </si>
+  <si>
+    <t>"On behalf of the U.S. Department of Homeland Security's Federal Emergency Management Agency (FEMA), I would like to express our deepest condolences to the families of those who were killed and injured by tornadoes that impacted Kansas, Missouri and Nebraska late last night and into this morning.</t>
+  </si>
+  <si>
+    <t>FEMA has been in constant contact with officials at the Kansas Department of Emergency Management (KDEM), Missouri State Emergency Management Agency (SEMA) and the Nebraska Emergency Management Agency (NEMA) since the severe weather hit.</t>
+  </si>
+  <si>
+    <t>FEMA Regional Administrator Beth Freeman released this statement.</t>
+  </si>
+  <si>
+    <t>Springfield</t>
+  </si>
+  <si>
+    <t>Buffalo is about 35 miles north of Springfield.</t>
+  </si>
+  <si>
+    <t>Regular agency reports have been on the local Hometown Radio News all day, in addition to the Springfield television and network coverage.</t>
+  </si>
+  <si>
+    <t>Associated Press</t>
+  </si>
+  <si>
+    <t>Associated Press photographer Mark Schiefelbein contributed to this report from Branson, Mo.</t>
+  </si>
+  <si>
+    <t>The Associated Press contributed to report.</t>
+  </si>
+  <si>
+    <t>JIM SALTER,Associated Press.</t>
+  </si>
+  <si>
+    <t>According to the Associated Press Darrell Osman says his mother, 75-year-old Mary Osman, was among the dead.</t>
+  </si>
+  <si>
+    <t>Ameren</t>
+  </si>
+  <si>
+    <t>Ameren hopes to have all power restored by the end of the day Friday.</t>
+  </si>
+  <si>
+    <t>Ameren reports 14,000 without power at the peak.</t>
+  </si>
+  <si>
+    <t>Ameren has open a customer service center in Harrisburg.</t>
+  </si>
+  <si>
+    <t>Metropolis</t>
+  </si>
+  <si>
+    <t>The tornado then crossed the Ohio River again and lifted around two miles northwest of Metropolis just east of the airport.</t>
+  </si>
+  <si>
+    <t>NWS</t>
+  </si>
+  <si>
+    <t>The NWS confirms preliminary reports of an EF2 tornado that went through McCracken and Ballard counties in Ky.  Reports are the tornado touched down just southwest of Mounds, Ill. and crossed over I-57 near exit 8.</t>
+  </si>
+  <si>
+    <t>NWS reports are a tornado touched down just southwest of Mounds, Ill. and crossed over I-57 near exit 8.</t>
+  </si>
+  <si>
+    <t>Further west, a house was destroyed on County Road 431 just north of Highway C.    According to NWS, numerous trees near the house were also uprooted.</t>
+  </si>
+  <si>
+    <t>An EF3 tornado was confirmed by the NWS.</t>
+  </si>
+  <si>
+    <t>NWS teams were in Stoddard and Cape Girardeau counties on Thursday surveying damage.</t>
+  </si>
+  <si>
+    <t>Mounds</t>
+  </si>
+  <si>
+    <t>Crystal Britt is just east of Mounds.</t>
+  </si>
+  <si>
+    <t>The school in Mounds also received damage.</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Michigan, Connecticut and Massachusetts on Wednesday were spared from tornados but visited by snowy weather — a shock after this winter’s consistently warm temperatures.</t>
+  </si>
+  <si>
+    <t>The National Weather Service issued overnight advisories of snow and rain in all three states, warning of an ice coating followed by freezing rain in Michigan, a “bit of snow” followed by “lots of rain” in Connecticut, and up to 10 inches of snow in Eastern Massachusetts.</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>In Missouri, one person was killed in a trailer park in the town of Buffalo, and at least three people were critically injured in the small eastern Kansas town of Harveyville.</t>
+  </si>
+  <si>
+    <t>In neighboring Kansas, the National Weather Service reported brief tornado touchdowns southwest of Hutchinson, and Gov.</t>
+  </si>
+  <si>
+    <t>One person was killed in Kansas.</t>
+  </si>
+  <si>
+    <t>Fire Department</t>
+  </si>
+  <si>
+    <t>First Responders and media are to report to the Ridgway Fire Department on West Main Street to sign in.</t>
+  </si>
+  <si>
+    <t>For those whose homes are damaged, officials are asking victims to sign up at the Fire Department to request lodging, tarpaulins, and other supplies.</t>
+  </si>
+  <si>
+    <t>Generators will be brought to the Oasis Tavern, just south of the Fire Department.</t>
+  </si>
+  <si>
+    <t>Food and drink is available at the Fire Department.</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Walmart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HARRISBURG -- The Leap Day tornado that devastated parts of Harrisburg Tuesday completely destroyed the strip shopping center south of the Walmart parking lot and caused "significant roof and water damage" to Walmart itself.  </t>
+  </si>
+  <si>
+    <t>SEOC</t>
+  </si>
+  <si>
+    <t>The governor says the SEOC will remain activated as long as necessary.</t>
+  </si>
+  <si>
+    <t>Ameren Illinois</t>
+  </si>
+  <si>
+    <t>Ameren Illinois representatives say more than 430 personnel were deployed to southern Illinois.</t>
+  </si>
+  <si>
+    <t>More than 400 people are working to restore power to Ameren Illinois customers.</t>
+  </si>
+  <si>
+    <t>People should not call 911 or the dispatch center to report power line outages, please contact Ameren Illinois direct.</t>
+  </si>
+  <si>
+    <t>As of 4:10 a.m. Thursday, Ameren Illinois reports outages in:  Copyright 2012 KFVS.</t>
+  </si>
+  <si>
+    <t>Ameren Illinois doesn't have a time of when power will be restored.</t>
+  </si>
+  <si>
+    <t>America</t>
+  </si>
+  <si>
+    <t>The tornado then crossed the Ohio River near the town of America, then across McCracken and Ballard Counties.</t>
+  </si>
+  <si>
+    <t>The tornado then crossed the Ohio River near the town of America, then across McCracken and Ballard counties.</t>
+  </si>
+  <si>
+    <t>Heartland</t>
+  </si>
+  <si>
+    <t>[More damage across the Heartland.]</t>
+  </si>
+  <si>
+    <t>Severe storms and tornadoes tear through the Heartland.</t>
+  </si>
+  <si>
+    <t>See pictures from across the Heartland after severe storms on Feb. 29, 2012.</t>
+  </si>
+  <si>
+    <t>See the National Weather Service storm damage reports from the tornadoes and severe storms that swept through the Heartland early Feb. 29.</t>
+  </si>
+  <si>
+    <t>Seven of those tornadoes were in the Heartland.</t>
+  </si>
+  <si>
+    <t>See more pictures from across the Heartland after severe storms on Feb. 29, 2012.</t>
+  </si>
+  <si>
+    <t>Five of those tornadoes were in the Heartland.</t>
+  </si>
+  <si>
+    <t>5 confirmed tornadoes in the Heartland.</t>
+  </si>
+  <si>
+    <t>Mo.</t>
+  </si>
+  <si>
+    <t>A Puxico, Mo.</t>
+  </si>
+  <si>
+    <t>The National Weather Service confirms preliminary reports of an EF2 in Marquand in Madison County, Mo.</t>
+  </si>
+  <si>
+    <t>Branson, Mo.</t>
+  </si>
+  <si>
+    <t>The school and a church sustained damage in Oak Ridge, Mo.</t>
+  </si>
+  <si>
+    <t>Storm shelters have been opened up for those in need in southern Ill. and southeast Mo.</t>
+  </si>
+  <si>
     <t>Ohio River</t>
   </si>
   <si>
-    <t>The tornado then crossed the Ohio River again and lifted around two miles northwest of Metropolis just east of the airport.</t>
-  </si>
-  <si>
-    <t>The tornado then crossed the Ohio River near the town of America, then across McCracken and Ballard Counties.</t>
-  </si>
-  <si>
-    <t>The tornado then crossed the Ohio River near the town of America, then across McCracken and Ballard counties.</t>
-  </si>
-  <si>
-    <t>Oklahoma</t>
-  </si>
-  <si>
-    <t>In northern Oklahoma, gusts of up to 80 mph flipped trailers and damaged homes near Cherokee.</t>
-  </si>
-  <si>
-    <t>Leap Day was not a good one for thousands of people in the Midwest and Southern United States as severe storms and tornadoes left a trail of destruction in Illinois, Missouri, Kansas, Arkansas, Oklahoma, Kentucky, and Tennessee.</t>
+    <t>Ridgway</t>
+  </si>
+  <si>
+    <t>Carly O'Keefe reports Ridgway's St. Joseph's catholic church leveled by storm.</t>
+  </si>
+  <si>
+    <t>Carly O'Keefe reports that there were 13 injuries in Ridgway.</t>
+  </si>
+  <si>
+    <t>The roads in Ridgway are closed to through traffic.</t>
+  </si>
+  <si>
+    <t>One with serious injuries and the rest minor injuries  She says Tin Shop Hardware Store in Ridgway crushed by wind.</t>
+  </si>
+  <si>
+    <t>A shelter is being set up at the Golden Circle Senior Center in Ridgway.</t>
+  </si>
+  <si>
+    <t>Town officials have established a curfew from 9 a.m. to 6 a.m. in Ridgway.</t>
+  </si>
+  <si>
+    <t>Heavy equipment that is brought into the area will be staged at the Seed Company, just west of Ridgway.</t>
+  </si>
+  <si>
+    <t>Cape Girardeau</t>
+  </si>
+  <si>
+    <t>Mark Champlin, 50, of Puxico was pronounced dead at 7:35 a.m. at Saint Francis Medical Center in Cape Girardeau.</t>
+  </si>
+  <si>
+    <t>He says there were residents ejected from a mobile home and two people airlifted to a hospital in Cape Girardeau.</t>
+  </si>
+  <si>
+    <t>Moreland says the victim was found in a nearby field and airlifted to a Cape Girardeau hospital and later died.</t>
+  </si>
+  <si>
+    <t>Ballard Counties</t>
+  </si>
+  <si>
+    <t>The National Weather Service confirms preliminary reports of an EF2 tornado that went through McCracken and Ballard Counties in Ky.</t>
+  </si>
+  <si>
+    <t>Marquand</t>
+  </si>
+  <si>
+    <t>The National Weather Service confirms preliminary reports of an EF1 in Marquand.</t>
+  </si>
+  <si>
+    <t>U.S.</t>
+  </si>
+  <si>
+    <t>Corey Mead, lead forecaster at the U.S. Storm Prediction Center in Norman, Okla., said a broad cold front was slamming into warm, humid air over much of the eastern half of the nation.</t>
+  </si>
+  <si>
+    <t>The National Weather Service’s U.S. map Wednesday was covered by colorful wintry and storm warnings:</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>A National Weather Service team has determined at least 1 of the strong storms that swept through Kentucky was an EF2 tornado packing winds of 125 miles per hour.</t>
+  </si>
+  <si>
+    <t>Tornado warnings and watches were posted for most of Kentucky and a large portion of Kentucky.</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>The tornadoes were spawned by a powerful storm system that blew down from the Rockies on Tuesday and was headed across the Ohio and Tennessee river valleys toward the Mid-Atlantic region.</t>
+  </si>
+  <si>
+    <t>Wal-Mart</t>
+  </si>
+  <si>
+    <t>He says the windows and doors have been blown out of the Wal-Mart in town.</t>
+  </si>
+  <si>
+    <t>Wal-Mart area severely damaged by tornado.</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Missouri Gov.</t>
+  </si>
+  <si>
+    <t>Two people were killed in southwest Missouri.</t>
+  </si>
+  <si>
+    <t>One man was killed outside Puxico, Missouri in the storms.</t>
+  </si>
+  <si>
+    <t>Waves of strong storms devastated small communities and damaged the country music resort town of Branson, Missouri.</t>
+  </si>
+  <si>
+    <t>Ky</t>
+  </si>
+  <si>
+    <t>Buffalo</t>
+  </si>
+  <si>
+    <t>Farther north, rescue crews waited for sunrise to begin searching a trailer park south of Buffalo where at least one person was killed after an apparent twister slammed the area.</t>
+  </si>
+  <si>
+    <t>National Weather Service</t>
+  </si>
+  <si>
+    <t>The National Weather Service is sending three teams to survey the damage.</t>
+  </si>
+  <si>
+    <t>Preliminary reports from the National Weather Service report large oak trees were found uprooted and damage to roofs was consistent with EF1 damage on the enhanced Fujita scale.</t>
+  </si>
+  <si>
+    <t>tornado, National Weather Service snow alerts and more Leap Year weather.</t>
+  </si>
+  <si>
+    <t>Some Leap Year babies woke up Wednesday to find their uncommon birthday plagued by school closings, National Weather Service snow alerts and even a tornado.</t>
+  </si>
+  <si>
+    <t>First Baptist Church</t>
+  </si>
+  <si>
+    <t>According to the sheriff's office, the shelter is open at the First Baptist Church at 204 North Main Street.</t>
+  </si>
+  <si>
+    <t>Stoddard County Coroner</t>
+  </si>
+  <si>
+    <t>Stoddard County Coroner Aaron Mathis has released the name of the man killed in Puxico Wednesday morning after a tornado moved through the area.</t>
+  </si>
+  <si>
+    <t>The Stoddard County Coroner confirms one person has died as a result of overnight storms.</t>
+  </si>
+  <si>
+    <t>Ill.</t>
   </si>
   <si>
     <t>Oak Ridge</t>
@@ -64,396 +535,24 @@
     <t>People are using the school in Oak Ridge as a staging area to head out to help those in the area.</t>
   </si>
   <si>
-    <t>The school and a church sustained damage in Oak Ridge, Mo.</t>
-  </si>
-  <si>
     <t>The Oak Ridge has damage to the roof and air conditioning unit.</t>
   </si>
   <si>
-    <t>Eldorado</t>
-  </si>
-  <si>
-    <t>They are Mary Osman, 75, of Harrisburg, Jaylynn Ferrell, 22, of Harrisburg, Lynda Hull, 74, of Galatia, Donna Rann, 61, of Eldorado, and Randy Rann, 64, of Eldorado.</t>
-  </si>
-  <si>
-    <t>Illinois</t>
-  </si>
-  <si>
-    <t>Many people are asking how they can help after a preliminary EF4 tornado hit Saline County, Illinois killing six people.</t>
-  </si>
-  <si>
-    <t>Quinn directed the Illinois Emergency Management Agency to activate the State Emergency Operations Center (SEOC) in Springfield.</t>
-  </si>
-  <si>
-    <t>At least 13 dead in storms working across Missouri, Illinois.</t>
-  </si>
-  <si>
-    <t>Ameren Illinois representatives say more than 430 personnel were deployed to southern Illinois.</t>
-  </si>
-  <si>
-    <t>But none faced the wrath of Mother Nature like the southern Illinois town of Harrisburg.</t>
-  </si>
-  <si>
-    <t>From Tuesday night into Wednesday morning, at least 16 tornado sightings were reported from Nebraska and Kansas across southern Missouri to Illinois and Kentucky, according to the storm center, an arm of the National Weather Service.</t>
-  </si>
-  <si>
-    <t>Quinn says he's already talked to President Obama and that Illinois is banding together as a family to help Harrisburg recover and rebuild.</t>
-  </si>
-  <si>
-    <t>It is the deadliest state disaster in Illinois in nearly a decade.</t>
-  </si>
-  <si>
-    <t>Pulaski County, Illinois EMS Director Ken Kerley says wreckers and vehicles were blown from their location and crossing arms broke off and blew into a squad car.</t>
-  </si>
-  <si>
-    <t>David Serby in Perry County, Illinois says a few outbuildings were blown over with some tree damage.</t>
-  </si>
-  <si>
-    <t>Crews with Ameren Illinois have issued a safety warning to all residents in and around Saline County.</t>
-  </si>
-  <si>
-    <t>More than 400 people are working to restore power to Ameren Illinois customers.</t>
-  </si>
-  <si>
-    <t>The United Way of South Central Illinois, located at 1101 Broadway in Mt.</t>
-  </si>
-  <si>
-    <t>People should not call 911 or the dispatch center to report power line outages, please contact Ameren Illinois direct.</t>
-  </si>
-  <si>
-    <t>At least 10 people were killed in the southern Illinois town of Harrisburg after a storm leveled much of the community of 9,000 people.</t>
-  </si>
-  <si>
-    <t>The Southern Illinois Egyptian Health Department says if you are experiencing a power outage:  -Keep your freezer/refrigerator door closed to maintain temperatures.</t>
-  </si>
-  <si>
-    <t>As of 4:10 a.m. Thursday, Ameren Illinois reports outages in:  Copyright 2012 KFVS.</t>
-  </si>
-  <si>
-    <t>Illinois Gov.</t>
-  </si>
-  <si>
-    <t>Ameren Illinois doesn't have a time of when power will be restored.</t>
-  </si>
-  <si>
-    <t>Pulaski County</t>
-  </si>
-  <si>
-    <t>No injuries have been reported in Pulaski County.</t>
-  </si>
-  <si>
-    <t>Cape Girardeau County</t>
-  </si>
-  <si>
-    <t>Team 1 (Rick Shanklin, Ken Ludington) - Harrisburg west toward Cape Girardeau County MO  Team 2 (Kelly Hooper, Shane Luecke) - Newburg IN West toward Harrisburg IL)  Team 3 (Christine Wielgos, Debbie Hooper) - Metropolis IL west toward Stoddard co. MO)  Note this may change as storms are in western Kentucky.</t>
-  </si>
-  <si>
-    <t>in Cape Girardeau County.</t>
-  </si>
-  <si>
-    <t>Midwest</t>
-  </si>
-  <si>
-    <t>Disaster in the Heartland - one year later  Disaster in the Heartland - one year later  The storm drove this plywood piece through the wall of a garage in Harrisburg,  Seven people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
-  </si>
-  <si>
-    <t>How you can help after the tornadoes  How you can help after the tornadoes  Eight people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
-  </si>
-  <si>
-    <t>Three people were killed in Tennessee after the same severe weather system that created massive damage across the Midwest moved through the state.</t>
-  </si>
-  <si>
-    <t>Midwest Tornadoes: News, Photos, and Video of the Destruction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDATED: At Least 12 People Killed In Deadly Midwest Storms. </t>
-  </si>
-  <si>
-    <t>Eight people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
-  </si>
-  <si>
-    <t>Fire Department</t>
-  </si>
-  <si>
-    <t>First Responders and media are to report to the Ridgway Fire Department on West Main Street to sign in.</t>
-  </si>
-  <si>
-    <t>For those whose homes are damaged, officials are asking victims to sign up at the Fire Department to request lodging, tarpaulins, and other supplies.</t>
-  </si>
-  <si>
-    <t>Generators will be brought to the Oasis Tavern, just south of the Fire Department.</t>
-  </si>
-  <si>
-    <t>Food and drink is available at the Fire Department.</t>
-  </si>
-  <si>
-    <t>Springfield</t>
-  </si>
-  <si>
-    <t>Buffalo is about 35 miles north of Springfield.</t>
-  </si>
-  <si>
-    <t>Regular agency reports have been on the local Hometown Radio News all day, in addition to the Springfield television and network coverage.</t>
-  </si>
-  <si>
-    <t>Associated Press</t>
-  </si>
-  <si>
-    <t>Associated Press photographer Mark Schiefelbein contributed to this report from Branson, Mo.</t>
-  </si>
-  <si>
-    <t>The Associated Press contributed to report.</t>
-  </si>
-  <si>
-    <t>JIM SALTER,Associated Press.</t>
-  </si>
-  <si>
-    <t>According to the Associated Press Darrell Osman says his mother, 75-year-old Mary Osman, was among the dead.</t>
-  </si>
-  <si>
-    <t>Ameren</t>
-  </si>
-  <si>
-    <t>Ameren hopes to have all power restored by the end of the day Friday.</t>
-  </si>
-  <si>
-    <t>Ameren reports 14,000 without power at the peak.</t>
-  </si>
-  <si>
-    <t>Ameren has open a customer service center in Harrisburg.</t>
-  </si>
-  <si>
-    <t>Metropolis</t>
-  </si>
-  <si>
-    <t>NWS</t>
-  </si>
-  <si>
-    <t>The NWS confirms preliminary reports of an EF2 tornado that went through McCracken and Ballard counties in Ky.  Reports are the tornado touched down just southwest of Mounds, Ill. and crossed over I-57 near exit 8.</t>
-  </si>
-  <si>
-    <t>NWS reports are a tornado touched down just southwest of Mounds, Ill. and crossed over I-57 near exit 8.</t>
-  </si>
-  <si>
-    <t>Further west, a house was destroyed on County Road 431 just north of Highway C.    According to NWS, numerous trees near the house were also uprooted.</t>
-  </si>
-  <si>
-    <t>An EF3 tornado was confirmed by the NWS.</t>
-  </si>
-  <si>
-    <t>NWS teams were in Stoddard and Cape Girardeau counties on Thursday surveying damage.</t>
-  </si>
-  <si>
-    <t>Mounds</t>
-  </si>
-  <si>
-    <t>Crystal Britt is just east of Mounds.</t>
-  </si>
-  <si>
-    <t>The school in Mounds also received damage.</t>
-  </si>
-  <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>Michigan, Connecticut and Massachusetts on Wednesday were spared from tornados but visited by snowy weather — a shock after this winter’s consistently warm temperatures.</t>
-  </si>
-  <si>
-    <t>The National Weather Service issued overnight advisories of snow and rain in all three states, warning of an ice coating followed by freezing rain in Michigan, a “bit of snow” followed by “lots of rain” in Connecticut, and up to 10 inches of snow in Eastern Massachusetts.</t>
-  </si>
-  <si>
-    <t>Kansas</t>
-  </si>
-  <si>
-    <t>FEMA has been in constant contact with officials at the Kansas Department of Emergency Management (KDEM), Missouri State Emergency Management Agency (SEMA) and the Nebraska Emergency Management Agency (NEMA) since the severe weather hit.</t>
-  </si>
-  <si>
-    <t>In Missouri, one person was killed in a trailer park in the town of Buffalo, and at least three people were critically injured in the small eastern Kansas town of Harveyville.</t>
-  </si>
-  <si>
-    <t>"On behalf of the U.S. Department of Homeland Security's Federal Emergency Management Agency (FEMA), I would like to express our deepest condolences to the families of those who were killed and injured by tornadoes that impacted Kansas, Missouri and Nebraska late last night and into this morning.</t>
-  </si>
-  <si>
-    <t>In neighboring Kansas, the National Weather Service reported brief tornado touchdowns southwest of Hutchinson, and Gov.</t>
-  </si>
-  <si>
-    <t>One person was killed in Kansas.</t>
-  </si>
-  <si>
-    <t>FEMA</t>
-  </si>
-  <si>
-    <t>FEMA Regional Administrator Beth Freeman released this statement.</t>
-  </si>
-  <si>
-    <t>Saline County</t>
-  </si>
-  <si>
-    <t>At least 100 people have been injured in the Harrisburg area, according to the Saline County Sheriff's Office.</t>
-  </si>
-  <si>
-    <t>The National Weather Service reports an EF4 tornado hit Saline County on the southwest side of Harrisburg, killing six people.</t>
-  </si>
-  <si>
-    <t>Four females and two males, all adults, were killed in Saline County.</t>
-  </si>
-  <si>
-    <t>Saline County Emergency Management asks people to stay off their cell phones if possible as heavy phone traffic is jamming the system.</t>
-  </si>
-  <si>
-    <t>Connecticut</t>
-  </si>
-  <si>
-    <t>Walmart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HARRISBURG -- The Leap Day tornado that devastated parts of Harrisburg Tuesday completely destroyed the strip shopping center south of the Walmart parking lot and caused "significant roof and water damage" to Walmart itself.  </t>
-  </si>
-  <si>
-    <t>SEOC</t>
-  </si>
-  <si>
-    <t>The governor says the SEOC will remain activated as long as necessary.</t>
-  </si>
-  <si>
-    <t>Ameren Illinois</t>
-  </si>
-  <si>
-    <t>America</t>
-  </si>
-  <si>
-    <t>U.S.</t>
-  </si>
-  <si>
-    <t>Corey Mead, lead forecaster at the U.S. Storm Prediction Center in Norman, Okla., said a broad cold front was slamming into warm, humid air over much of the eastern half of the nation.</t>
-  </si>
-  <si>
-    <t>The National Weather Service’s U.S. map Wednesday was covered by colorful wintry and storm warnings:</t>
-  </si>
-  <si>
     <t>Bell City</t>
   </si>
   <si>
     <t>It started early Wednesday morning just west of Asherville to two miles west of Bell City.</t>
   </si>
   <si>
-    <t>A second tornado in Stoddard County Wednesday morning started just east of Bell City to three miles southeast of Benton, Mo.</t>
-  </si>
-  <si>
-    <t>Stoddard County</t>
-  </si>
-  <si>
-    <t>A total of eight patients from Stoddard County are being treated at Saint Francis Medical Center.</t>
-  </si>
-  <si>
-    <t>One man has died after the storms in Stoddard County.</t>
-  </si>
-  <si>
-    <t>Stoddard County Coroner Aaron Mathis has released the name of the man killed in Puxico Wednesday morning after a tornado moved through the area.</t>
-  </si>
-  <si>
-    <t>Stoddard County Sheriff Carl Hefner says several mobile homes in the area are destroyed in Stoddard County.</t>
-  </si>
-  <si>
-    <t>The Stoddard County coroner says Mark Champlin, 50, of Puxico was killed.</t>
-  </si>
-  <si>
-    <t>Highway Patrol Trooper Clark Parrott says large trees are down along Route M in Stoddard County.</t>
-  </si>
-  <si>
-    <t>You can drive for miles in Stoddard County and never see damage, but a path left from the strong winds that did blow through, show the wreckage.</t>
-  </si>
-  <si>
-    <t>man was killed in Stoddard County.</t>
-  </si>
-  <si>
-    <t>Hefner says they started receiving calls around 4 a.m.  Dale Moreland with Stoddard County EMA says one mobile home was moved about 200 feet.</t>
-  </si>
-  <si>
-    <t>They are all storm related injuries from Stoddard County.</t>
-  </si>
-  <si>
-    <t>The Stoddard County Coroner confirms one person has died as a result of overnight storms.</t>
-  </si>
-  <si>
-    <t>Ridgway</t>
-  </si>
-  <si>
-    <t>Carly O'Keefe reports Ridgway's St. Joseph's catholic church leveled by storm.</t>
-  </si>
-  <si>
-    <t>Carly O'Keefe reports that there were 13 injuries in Ridgway.</t>
-  </si>
-  <si>
-    <t>The roads in Ridgway are closed to through traffic.</t>
-  </si>
-  <si>
-    <t>One with serious injuries and the rest minor injuries  She says Tin Shop Hardware Store in Ridgway crushed by wind.</t>
-  </si>
-  <si>
-    <t>A shelter is being set up at the Golden Circle Senior Center in Ridgway.</t>
-  </si>
-  <si>
-    <t>Town officials have established a curfew from 9 a.m. to 6 a.m. in Ridgway.</t>
-  </si>
-  <si>
-    <t>Heavy equipment that is brought into the area will be staged at the Seed Company, just west of Ridgway.</t>
-  </si>
-  <si>
-    <t>Cape Girardeau</t>
-  </si>
-  <si>
-    <t>Mark Champlin, 50, of Puxico was pronounced dead at 7:35 a.m. at Saint Francis Medical Center in Cape Girardeau.</t>
-  </si>
-  <si>
-    <t>He says there were residents ejected from a mobile home and two people airlifted to a hospital in Cape Girardeau.</t>
-  </si>
-  <si>
-    <t>Moreland says the victim was found in a nearby field and airlifted to a Cape Girardeau hospital and later died.</t>
-  </si>
-  <si>
-    <t>Ballard Counties</t>
-  </si>
-  <si>
-    <t>The National Weather Service confirms preliminary reports of an EF2 tornado that went through McCracken and Ballard Counties in Ky.</t>
-  </si>
-  <si>
-    <t>Marquand</t>
-  </si>
-  <si>
-    <t>The National Weather Service confirms preliminary reports of an EF1 in Marquand.</t>
-  </si>
-  <si>
-    <t>The National Weather Service confirms preliminary reports of an EF2 in Marquand in Madison County, Mo.</t>
-  </si>
-  <si>
-    <t>Heartland</t>
-  </si>
-  <si>
-    <t>[More damage across the Heartland.]</t>
-  </si>
-  <si>
-    <t>Severe storms and tornadoes tear through the Heartland.</t>
+    <t>Heartland News</t>
+  </si>
+  <si>
+    <t>Heartland News reporter Carly O'Keefe reports grain bins in fields and more damage in Gallatin County.</t>
   </si>
   <si>
     <t>Moreland told Heartland News Wednesday morning that there is extensive damage everywhere, and power lines down across several miles.</t>
   </si>
   <si>
-    <t>See pictures from across the Heartland after severe storms on Feb. 29, 2012.</t>
-  </si>
-  <si>
-    <t>See the National Weather Service storm damage reports from the tornadoes and severe storms that swept through the Heartland early Feb. 29.</t>
-  </si>
-  <si>
-    <t>Seven of those tornadoes were in the Heartland.</t>
-  </si>
-  <si>
-    <t>Heartland News reporter Carly O'Keefe reports grain bins in fields and more damage in Gallatin County.</t>
-  </si>
-  <si>
-    <t>See more pictures from across the Heartland after severe storms on Feb. 29, 2012.</t>
-  </si>
-  <si>
     <t>Emergency Manager Dale Moreland tells Heartland News it looks like the mobile home  "exploded."</t>
   </si>
   <si>
@@ -463,78 +562,39 @@
     <t>The mayor of Harrisburg tells Heartland News that this is a horrific event.</t>
   </si>
   <si>
-    <t>Five of those tornadoes were in the Heartland.</t>
-  </si>
-  <si>
-    <t>5 confirmed tornadoes in the Heartland.</t>
-  </si>
-  <si>
-    <t>Kentucky</t>
-  </si>
-  <si>
-    <t>A National Weather Service team has determined at least 1 of the strong storms that swept through Kentucky was an EF2 tornado packing winds of 125 miles per hour.</t>
-  </si>
-  <si>
-    <t>Tornado warnings and watches were posted for most of Kentucky and a large portion of Kentucky.</t>
-  </si>
-  <si>
-    <t>Wal-Mart</t>
-  </si>
-  <si>
-    <t>He says the windows and doors have been blown out of the Wal-Mart in town.</t>
-  </si>
-  <si>
-    <t>Wal-Mart area severely damaged by tornado.</t>
-  </si>
-  <si>
-    <t>Nebraska</t>
-  </si>
-  <si>
-    <t>Missouri</t>
-  </si>
-  <si>
-    <t>Missouri Gov.</t>
-  </si>
-  <si>
-    <t>Two people were killed in southwest Missouri.</t>
-  </si>
-  <si>
-    <t>One man was killed outside Puxico, Missouri in the storms.</t>
-  </si>
-  <si>
-    <t>Waves of strong storms devastated small communities and damaged the country music resort town of Branson, Missouri.</t>
-  </si>
-  <si>
-    <t>Ky</t>
-  </si>
-  <si>
-    <t>Buffalo</t>
-  </si>
-  <si>
-    <t>Farther north, rescue crews waited for sunrise to begin searching a trailer park south of Buffalo where at least one person was killed after an apparent twister slammed the area.</t>
-  </si>
-  <si>
-    <t>National Weather Service</t>
-  </si>
-  <si>
-    <t>The National Weather Service is sending three teams to survey the damage.</t>
-  </si>
-  <si>
-    <t>Preliminary reports from the National Weather Service report large oak trees were found uprooted and damage to roofs was consistent with EF1 damage on the enhanced Fujita scale.</t>
-  </si>
-  <si>
-    <t>tornado, National Weather Service snow alerts and more Leap Year weather.</t>
-  </si>
-  <si>
-    <t>Some Leap Year babies woke up Wednesday to find their uncommon birthday plagued by school closings, National Weather Service snow alerts and even a tornado.</t>
+    <t>Mo</t>
+  </si>
+  <si>
+    <t>Moreland says crews are working on County Road 249 and County Road 271 is blocked.</t>
+  </si>
+  <si>
+    <t>Emergency Manager Dale Moreland says there will be a shelter opening at 3 p.m. Wednesday at Kinder Chapel that is on K Highway.</t>
+  </si>
+  <si>
+    <t>Windows are blown out," Moore said.</t>
+  </si>
+  <si>
+    <t>Residents of Clay County in northeastern Arkansas reported hail the size of golf balls, while half dollar-sized hail was reported in Mountain Home.</t>
+  </si>
+  <si>
+    <t>More than 30 people were reported hurt, mostly with cuts and bruises.</t>
+  </si>
+  <si>
+    <t>John Moore, owner of the damaged Cakes-n-Creams '50s Diner, said the tornado seemed to target the city's main strip, moving down the entertainment district, right through the convention center, across a lake and into a housing division.</t>
+  </si>
+  <si>
+    <t>Jennifer Verhaalen, a long-term resident at the Hillbilly Inn Motel in downtown Branson, said she saw a white funnel cloud followed by a wall of rain as the storm closed in on the town around 1 a.m.  She said she retreated to a back bedroom with her husband as the storm slammed into two other hotel buildings tearing the roof off one.</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>The system also skirted northern Arkansas, bringing gusts of up to 60 mph in the northwest.</t>
   </si>
   <si>
     <t>Puxico</t>
   </si>
   <si>
-    <t>A Puxico, Mo.</t>
-  </si>
-  <si>
     <t>The damage is along County Roads 266 and 257 east of Puxico and tracked to the northeast to the Leora area.</t>
   </si>
   <si>
@@ -542,66 +602,6 @@
   </si>
   <si>
     <t>No major damage is reported in Puxico city limits.</t>
-  </si>
-  <si>
-    <t>Stoddard County Coroner</t>
-  </si>
-  <si>
-    <t>Ill.</t>
-  </si>
-  <si>
-    <t>Storm shelters have been opened up for those in need in southern Ill. and southeast Mo.</t>
-  </si>
-  <si>
-    <t>Tennessee</t>
-  </si>
-  <si>
-    <t>The tornadoes were spawned by a powerful storm system that blew down from the Rockies on Tuesday and was headed across the Ohio and Tennessee river valleys toward the Mid-Atlantic region.</t>
-  </si>
-  <si>
-    <t>Mo.</t>
-  </si>
-  <si>
-    <t>Branson, Mo.</t>
-  </si>
-  <si>
-    <t>Heartland News</t>
-  </si>
-  <si>
-    <t>Mo</t>
-  </si>
-  <si>
-    <t>Moreland says crews are working on County Road 249 and County Road 271 is blocked.</t>
-  </si>
-  <si>
-    <t>Emergency Manager Dale Moreland says there will be a shelter opening at 3 p.m. Wednesday at Kinder Chapel that is on K Highway.</t>
-  </si>
-  <si>
-    <t>Windows are blown out," Moore said.</t>
-  </si>
-  <si>
-    <t>Residents of Clay County in northeastern Arkansas reported hail the size of golf balls, while half dollar-sized hail was reported in Mountain Home.</t>
-  </si>
-  <si>
-    <t>More than 30 people were reported hurt, mostly with cuts and bruises.</t>
-  </si>
-  <si>
-    <t>John Moore, owner of the damaged Cakes-n-Creams '50s Diner, said the tornado seemed to target the city's main strip, moving down the entertainment district, right through the convention center, across a lake and into a housing division.</t>
-  </si>
-  <si>
-    <t>Jennifer Verhaalen, a long-term resident at the Hillbilly Inn Motel in downtown Branson, said she saw a white funnel cloud followed by a wall of rain as the storm closed in on the town around 1 a.m.  She said she retreated to a back bedroom with her husband as the storm slammed into two other hotel buildings tearing the roof off one.</t>
-  </si>
-  <si>
-    <t>Arkansas</t>
-  </si>
-  <si>
-    <t>The system also skirted northern Arkansas, bringing gusts of up to 60 mph in the northwest.</t>
-  </si>
-  <si>
-    <t>First Baptist Church</t>
-  </si>
-  <si>
-    <t>According to the sheriff's office, the shelter is open at the First Baptist Church at 204 North Main Street.</t>
   </si>
   <si>
     <t>Harrisburg</t>
@@ -975,7 +975,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C285"/>
+  <dimension ref="A1:C253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1041,10 +1041,10 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1052,10 +1052,10 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1063,10 +1063,10 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1074,7 +1074,7 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
@@ -1096,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
@@ -1107,7 +1107,7 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
@@ -1118,10 +1118,10 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1129,10 +1129,10 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1140,10 +1140,10 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
         <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1151,10 +1151,10 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1162,10 +1162,10 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
         <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1173,10 +1173,10 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1184,10 +1184,10 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1195,10 +1195,10 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1206,10 +1206,10 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1217,10 +1217,10 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1228,10 +1228,10 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1239,10 +1239,10 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1250,10 +1250,10 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1261,7 +1261,7 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
         <v>30</v>
@@ -1272,7 +1272,7 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
         <v>31</v>
@@ -1283,7 +1283,7 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
         <v>32</v>
@@ -1294,10 +1294,10 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1305,10 +1305,10 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1316,10 +1316,10 @@
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1327,7 +1327,7 @@
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
         <v>36</v>
@@ -1338,7 +1338,7 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C33" t="s">
         <v>37</v>
@@ -1349,10 +1349,10 @@
         <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1360,10 +1360,10 @@
         <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1371,10 +1371,10 @@
         <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1382,10 +1382,10 @@
         <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1393,10 +1393,10 @@
         <v>0</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1404,7 +1404,7 @@
         <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C39" t="s">
         <v>43</v>
@@ -1415,7 +1415,7 @@
         <v>0</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C40" t="s">
         <v>44</v>
@@ -1426,10 +1426,10 @@
         <v>0</v>
       </c>
       <c r="B41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" t="s">
         <v>45</v>
-      </c>
-      <c r="C41" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1437,7 +1437,7 @@
         <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C42" t="s">
         <v>47</v>
@@ -1448,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
         <v>48</v>
@@ -1459,10 +1459,10 @@
         <v>0</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1470,10 +1470,10 @@
         <v>0</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1481,7 +1481,7 @@
         <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C46" t="s">
         <v>50</v>
@@ -1492,7 +1492,7 @@
         <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
         <v>51</v>
@@ -1503,10 +1503,10 @@
         <v>0</v>
       </c>
       <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" t="s">
         <v>52</v>
-      </c>
-      <c r="C48" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1514,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C49" t="s">
         <v>54</v>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C50" t="s">
         <v>55</v>
@@ -1536,7 +1536,7 @@
         <v>0</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C51" t="s">
         <v>56</v>
@@ -1550,7 +1550,7 @@
         <v>57</v>
       </c>
       <c r="C52" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1638,7 +1638,7 @@
         <v>65</v>
       </c>
       <c r="C60" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1649,7 +1649,7 @@
         <v>65</v>
       </c>
       <c r="C61" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1657,10 +1657,10 @@
         <v>0</v>
       </c>
       <c r="B62" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C62" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1668,10 +1668,10 @@
         <v>0</v>
       </c>
       <c r="B63" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C63" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1679,10 +1679,10 @@
         <v>0</v>
       </c>
       <c r="B64" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C64" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1690,10 +1690,10 @@
         <v>0</v>
       </c>
       <c r="B65" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C65" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1701,10 +1701,10 @@
         <v>0</v>
       </c>
       <c r="B66" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C66" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1712,10 +1712,10 @@
         <v>0</v>
       </c>
       <c r="B67" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C67" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1723,10 +1723,10 @@
         <v>0</v>
       </c>
       <c r="B68" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C68" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1734,10 +1734,10 @@
         <v>0</v>
       </c>
       <c r="B69" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C69" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1745,10 +1745,10 @@
         <v>0</v>
       </c>
       <c r="B70" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C70" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1756,10 +1756,10 @@
         <v>0</v>
       </c>
       <c r="B71" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C71" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1767,10 +1767,10 @@
         <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C72" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1778,10 +1778,10 @@
         <v>0</v>
       </c>
       <c r="B73" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C73" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1789,10 +1789,10 @@
         <v>0</v>
       </c>
       <c r="B74" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C74" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1800,10 +1800,10 @@
         <v>0</v>
       </c>
       <c r="B75" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C75" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1811,10 +1811,10 @@
         <v>0</v>
       </c>
       <c r="B76" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C76" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1822,10 +1822,10 @@
         <v>0</v>
       </c>
       <c r="B77" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C77" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1833,10 +1833,10 @@
         <v>0</v>
       </c>
       <c r="B78" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C78" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1844,10 +1844,10 @@
         <v>0</v>
       </c>
       <c r="B79" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C79" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1855,10 +1855,10 @@
         <v>0</v>
       </c>
       <c r="B80" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C80" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1866,10 +1866,10 @@
         <v>0</v>
       </c>
       <c r="B81" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C81" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1877,10 +1877,10 @@
         <v>0</v>
       </c>
       <c r="B82" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C82" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1888,10 +1888,10 @@
         <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C83" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1899,10 +1899,10 @@
         <v>0</v>
       </c>
       <c r="B84" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C84" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1910,10 +1910,10 @@
         <v>0</v>
       </c>
       <c r="B85" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C85" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1921,10 +1921,10 @@
         <v>0</v>
       </c>
       <c r="B86" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="C86" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1932,10 +1932,10 @@
         <v>0</v>
       </c>
       <c r="B87" t="s">
+        <v>92</v>
+      </c>
+      <c r="C87" t="s">
         <v>82</v>
-      </c>
-      <c r="C87" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1943,10 +1943,10 @@
         <v>0</v>
       </c>
       <c r="B88" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C88" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1954,10 +1954,10 @@
         <v>0</v>
       </c>
       <c r="B89" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C89" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1965,10 +1965,10 @@
         <v>0</v>
       </c>
       <c r="B90" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C90" t="s">
-        <v>89</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1976,10 +1976,10 @@
         <v>0</v>
       </c>
       <c r="B91" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C91" t="s">
-        <v>91</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1987,10 +1987,10 @@
         <v>0</v>
       </c>
       <c r="B92" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C92" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1998,10 +1998,10 @@
         <v>0</v>
       </c>
       <c r="B93" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C93" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2009,10 +2009,10 @@
         <v>0</v>
       </c>
       <c r="B94" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C94" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2020,10 +2020,10 @@
         <v>0</v>
       </c>
       <c r="B95" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C95" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2031,10 +2031,10 @@
         <v>0</v>
       </c>
       <c r="B96" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C96" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2042,10 +2042,10 @@
         <v>0</v>
       </c>
       <c r="B97" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C97" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2053,10 +2053,10 @@
         <v>0</v>
       </c>
       <c r="B98" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C98" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2064,10 +2064,10 @@
         <v>0</v>
       </c>
       <c r="B99" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C99" t="s">
-        <v>97</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2075,10 +2075,10 @@
         <v>0</v>
       </c>
       <c r="B100" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C100" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2086,10 +2086,10 @@
         <v>0</v>
       </c>
       <c r="B101" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="C101" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2097,10 +2097,10 @@
         <v>0</v>
       </c>
       <c r="B102" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="C102" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2108,10 +2108,10 @@
         <v>0</v>
       </c>
       <c r="B103" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C103" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2119,10 +2119,10 @@
         <v>0</v>
       </c>
       <c r="B104" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C104" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2130,10 +2130,10 @@
         <v>0</v>
       </c>
       <c r="B105" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C105" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2141,10 +2141,10 @@
         <v>0</v>
       </c>
       <c r="B106" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C106" t="s">
-        <v>34</v>
+        <v>110</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2152,10 +2152,10 @@
         <v>0</v>
       </c>
       <c r="B107" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C107" t="s">
-        <v>37</v>
+        <v>111</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2163,10 +2163,10 @@
         <v>0</v>
       </c>
       <c r="B108" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C108" t="s">
-        <v>39</v>
+        <v>112</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2174,10 +2174,10 @@
         <v>0</v>
       </c>
       <c r="B109" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C109" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2185,10 +2185,10 @@
         <v>0</v>
       </c>
       <c r="B110" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C110" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2196,10 +2196,10 @@
         <v>0</v>
       </c>
       <c r="B111" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C111" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2207,10 +2207,10 @@
         <v>0</v>
       </c>
       <c r="B112" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="C112" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2218,10 +2218,10 @@
         <v>0</v>
       </c>
       <c r="B113" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="C113" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2229,10 +2229,10 @@
         <v>0</v>
       </c>
       <c r="B114" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="C114" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2240,10 +2240,10 @@
         <v>0</v>
       </c>
       <c r="B115" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="C115" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2251,10 +2251,10 @@
         <v>0</v>
       </c>
       <c r="B116" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="C116" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2262,10 +2262,10 @@
         <v>0</v>
       </c>
       <c r="B117" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C117" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2273,10 +2273,10 @@
         <v>0</v>
       </c>
       <c r="B118" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C118" t="s">
-        <v>110</v>
+        <v>45</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2284,10 +2284,10 @@
         <v>0</v>
       </c>
       <c r="B119" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="C119" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2295,10 +2295,10 @@
         <v>0</v>
       </c>
       <c r="B120" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="C120" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2306,10 +2306,10 @@
         <v>0</v>
       </c>
       <c r="B121" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="C121" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2317,10 +2317,10 @@
         <v>0</v>
       </c>
       <c r="B122" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="C122" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2328,10 +2328,10 @@
         <v>0</v>
       </c>
       <c r="B123" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="C123" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2339,10 +2339,10 @@
         <v>0</v>
       </c>
       <c r="B124" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="C124" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2350,10 +2350,10 @@
         <v>0</v>
       </c>
       <c r="B125" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="C125" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2361,10 +2361,10 @@
         <v>0</v>
       </c>
       <c r="B126" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="C126" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2372,10 +2372,10 @@
         <v>0</v>
       </c>
       <c r="B127" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="C127" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2383,10 +2383,10 @@
         <v>0</v>
       </c>
       <c r="B128" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="C128" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2394,10 +2394,10 @@
         <v>0</v>
       </c>
       <c r="B129" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C129" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2405,10 +2405,10 @@
         <v>0</v>
       </c>
       <c r="B130" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C130" t="s">
-        <v>122</v>
+        <v>76</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2416,10 +2416,10 @@
         <v>0</v>
       </c>
       <c r="B131" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C131" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2427,10 +2427,10 @@
         <v>0</v>
       </c>
       <c r="B132" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C132" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2438,10 +2438,10 @@
         <v>0</v>
       </c>
       <c r="B133" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C133" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2449,10 +2449,10 @@
         <v>0</v>
       </c>
       <c r="B134" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="C134" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2460,10 +2460,10 @@
         <v>0</v>
       </c>
       <c r="B135" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="C135" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2471,10 +2471,10 @@
         <v>0</v>
       </c>
       <c r="B136" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="C136" t="s">
-        <v>53</v>
+        <v>137</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2482,10 +2482,10 @@
         <v>0</v>
       </c>
       <c r="B137" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="C137" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2493,10 +2493,10 @@
         <v>0</v>
       </c>
       <c r="B138" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C138" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2504,10 +2504,10 @@
         <v>0</v>
       </c>
       <c r="B139" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C139" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2515,10 +2515,10 @@
         <v>0</v>
       </c>
       <c r="B140" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C140" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2526,10 +2526,10 @@
         <v>0</v>
       </c>
       <c r="B141" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="C141" t="s">
-        <v>131</v>
+        <v>15</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2537,10 +2537,10 @@
         <v>0</v>
       </c>
       <c r="B142" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="C142" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2548,10 +2548,10 @@
         <v>0</v>
       </c>
       <c r="B143" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="C143" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2559,10 +2559,10 @@
         <v>0</v>
       </c>
       <c r="B144" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="C144" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2570,10 +2570,10 @@
         <v>0</v>
       </c>
       <c r="B145" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C145" t="s">
-        <v>135</v>
+        <v>7</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2581,10 +2581,10 @@
         <v>0</v>
       </c>
       <c r="B146" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C146" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2592,10 +2592,10 @@
         <v>0</v>
       </c>
       <c r="B147" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C147" t="s">
-        <v>138</v>
+        <v>49</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2603,10 +2603,10 @@
         <v>0</v>
       </c>
       <c r="B148" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C148" t="s">
-        <v>139</v>
+        <v>7</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2614,10 +2614,10 @@
         <v>0</v>
       </c>
       <c r="B149" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="C149" t="s">
-        <v>46</v>
+        <v>147</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2625,10 +2625,10 @@
         <v>0</v>
       </c>
       <c r="B150" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="C150" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2636,10 +2636,10 @@
         <v>0</v>
       </c>
       <c r="B151" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="C151" t="s">
-        <v>141</v>
+        <v>15</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2647,10 +2647,10 @@
         <v>0</v>
       </c>
       <c r="B152" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="C152" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2658,10 +2658,10 @@
         <v>0</v>
       </c>
       <c r="B153" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="C153" t="s">
-        <v>142</v>
+        <v>55</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2669,10 +2669,10 @@
         <v>0</v>
       </c>
       <c r="B154" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C154" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2680,10 +2680,10 @@
         <v>0</v>
       </c>
       <c r="B155" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C155" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2691,10 +2691,10 @@
         <v>0</v>
       </c>
       <c r="B156" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C156" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2702,10 +2702,10 @@
         <v>0</v>
       </c>
       <c r="B157" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C157" t="s">
-        <v>146</v>
+        <v>84</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2713,10 +2713,10 @@
         <v>0</v>
       </c>
       <c r="B158" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C158" t="s">
-        <v>147</v>
+        <v>15</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2724,10 +2724,10 @@
         <v>0</v>
       </c>
       <c r="B159" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C159" t="s">
-        <v>148</v>
+        <v>54</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2735,10 +2735,10 @@
         <v>0</v>
       </c>
       <c r="B160" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C160" t="s">
-        <v>149</v>
+        <v>13</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2746,10 +2746,10 @@
         <v>0</v>
       </c>
       <c r="B161" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C161" t="s">
-        <v>150</v>
+        <v>7</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2757,10 +2757,10 @@
         <v>0</v>
       </c>
       <c r="B162" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C162" t="s">
-        <v>51</v>
+        <v>154</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2768,10 +2768,10 @@
         <v>0</v>
       </c>
       <c r="B163" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C163" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2779,10 +2779,10 @@
         <v>0</v>
       </c>
       <c r="B164" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C164" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2790,10 +2790,10 @@
         <v>0</v>
       </c>
       <c r="B165" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C165" t="s">
-        <v>153</v>
+        <v>72</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -2801,10 +2801,10 @@
         <v>0</v>
       </c>
       <c r="B166" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C166" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2812,10 +2812,10 @@
         <v>0</v>
       </c>
       <c r="B167" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C167" t="s">
-        <v>11</v>
+        <v>157</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2823,10 +2823,10 @@
         <v>0</v>
       </c>
       <c r="B168" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C168" t="s">
-        <v>155</v>
+        <v>84</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -2834,10 +2834,10 @@
         <v>0</v>
       </c>
       <c r="B169" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C169" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -2845,10 +2845,10 @@
         <v>0</v>
       </c>
       <c r="B170" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C170" t="s">
-        <v>26</v>
+        <v>140</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -2856,10 +2856,10 @@
         <v>0</v>
       </c>
       <c r="B171" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C171" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -2867,10 +2867,10 @@
         <v>0</v>
       </c>
       <c r="B172" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C172" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -2881,7 +2881,7 @@
         <v>158</v>
       </c>
       <c r="C173" t="s">
-        <v>159</v>
+        <v>32</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -2892,7 +2892,7 @@
         <v>158</v>
       </c>
       <c r="C174" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -2903,7 +2903,7 @@
         <v>158</v>
       </c>
       <c r="C175" t="s">
-        <v>161</v>
+        <v>82</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -2914,7 +2914,7 @@
         <v>158</v>
       </c>
       <c r="C176" t="s">
-        <v>84</v>
+        <v>137</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -2925,7 +2925,7 @@
         <v>158</v>
       </c>
       <c r="C177" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -2936,7 +2936,7 @@
         <v>158</v>
       </c>
       <c r="C178" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -2947,7 +2947,7 @@
         <v>158</v>
       </c>
       <c r="C179" t="s">
-        <v>23</v>
+        <v>142</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -2958,7 +2958,7 @@
         <v>158</v>
       </c>
       <c r="C180" t="s">
-        <v>11</v>
+        <v>160</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -2969,7 +2969,7 @@
         <v>158</v>
       </c>
       <c r="C181" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -2980,7 +2980,7 @@
         <v>158</v>
       </c>
       <c r="C182" t="s">
-        <v>83</v>
+        <v>162</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -2991,7 +2991,7 @@
         <v>163</v>
       </c>
       <c r="C183" t="s">
-        <v>133</v>
+        <v>3</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -3002,7 +3002,7 @@
         <v>163</v>
       </c>
       <c r="C184" t="s">
-        <v>71</v>
+        <v>164</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3010,10 +3010,10 @@
         <v>0</v>
       </c>
       <c r="B185" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C185" t="s">
-        <v>58</v>
+        <v>166</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3021,10 +3021,10 @@
         <v>0</v>
       </c>
       <c r="B186" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C186" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3032,10 +3032,10 @@
         <v>0</v>
       </c>
       <c r="B187" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C187" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3043,10 +3043,10 @@
         <v>0</v>
       </c>
       <c r="B188" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C188" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3054,10 +3054,10 @@
         <v>0</v>
       </c>
       <c r="B189" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C189" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -3065,10 +3065,10 @@
         <v>0</v>
       </c>
       <c r="B190" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C190" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3076,10 +3076,10 @@
         <v>0</v>
       </c>
       <c r="B191" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C191" t="s">
-        <v>26</v>
+        <v>171</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3087,10 +3087,10 @@
         <v>0</v>
       </c>
       <c r="B192" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C192" t="s">
-        <v>92</v>
+        <v>172</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -3098,10 +3098,10 @@
         <v>0</v>
       </c>
       <c r="B193" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C193" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3109,10 +3109,10 @@
         <v>0</v>
       </c>
       <c r="B194" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C194" t="s">
-        <v>81</v>
+        <v>2</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -3120,10 +3120,10 @@
         <v>0</v>
       </c>
       <c r="B195" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C195" t="s">
-        <v>135</v>
+        <v>173</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -3131,10 +3131,10 @@
         <v>0</v>
       </c>
       <c r="B196" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="C196" t="s">
-        <v>86</v>
+        <v>175</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -3142,10 +3142,10 @@
         <v>0</v>
       </c>
       <c r="B197" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="C197" t="s">
-        <v>167</v>
+        <v>45</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -3153,10 +3153,10 @@
         <v>0</v>
       </c>
       <c r="B198" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C198" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -3164,10 +3164,10 @@
         <v>0</v>
       </c>
       <c r="B199" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C199" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -3175,10 +3175,10 @@
         <v>0</v>
       </c>
       <c r="B200" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C200" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -3186,10 +3186,10 @@
         <v>0</v>
       </c>
       <c r="B201" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C201" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -3197,10 +3197,10 @@
         <v>0</v>
       </c>
       <c r="B202" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C202" t="s">
-        <v>111</v>
+        <v>181</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -3208,10 +3208,10 @@
         <v>0</v>
       </c>
       <c r="B203" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="C203" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -3219,10 +3219,10 @@
         <v>0</v>
       </c>
       <c r="B204" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="C204" t="s">
-        <v>129</v>
+        <v>184</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -3230,10 +3230,10 @@
         <v>0</v>
       </c>
       <c r="B205" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="C205" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -3241,10 +3241,10 @@
         <v>0</v>
       </c>
       <c r="B206" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="C206" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -3252,10 +3252,10 @@
         <v>0</v>
       </c>
       <c r="B207" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="C207" t="s">
-        <v>173</v>
+        <v>133</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -3263,10 +3263,10 @@
         <v>0</v>
       </c>
       <c r="B208" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="C208" t="s">
-        <v>174</v>
+        <v>99</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -3274,10 +3274,10 @@
         <v>0</v>
       </c>
       <c r="B209" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="C209" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -3285,10 +3285,10 @@
         <v>0</v>
       </c>
       <c r="B210" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C210" t="s">
-        <v>111</v>
+        <v>179</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -3296,10 +3296,10 @@
         <v>0</v>
       </c>
       <c r="B211" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C211" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -3307,10 +3307,10 @@
         <v>0</v>
       </c>
       <c r="B212" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C212" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -3318,10 +3318,10 @@
         <v>0</v>
       </c>
       <c r="B213" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C213" t="s">
-        <v>178</v>
+        <v>107</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -3329,10 +3329,10 @@
         <v>0</v>
       </c>
       <c r="B214" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C214" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -3340,10 +3340,10 @@
         <v>0</v>
       </c>
       <c r="B215" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C215" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -3351,10 +3351,10 @@
         <v>0</v>
       </c>
       <c r="B216" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C216" t="s">
-        <v>48</v>
+        <v>189</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -3362,10 +3362,10 @@
         <v>0</v>
       </c>
       <c r="B217" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="C217" t="s">
-        <v>11</v>
+        <v>186</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -3373,10 +3373,10 @@
         <v>0</v>
       </c>
       <c r="B218" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="C218" t="s">
-        <v>61</v>
+        <v>191</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -3384,10 +3384,10 @@
         <v>0</v>
       </c>
       <c r="B219" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="C219" t="s">
-        <v>172</v>
+        <v>7</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -3395,10 +3395,10 @@
         <v>0</v>
       </c>
       <c r="B220" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="C220" t="s">
-        <v>136</v>
+        <v>166</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -3406,10 +3406,10 @@
         <v>0</v>
       </c>
       <c r="B221" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="C221" t="s">
-        <v>182</v>
+        <v>116</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -3417,10 +3417,10 @@
         <v>0</v>
       </c>
       <c r="B222" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="C222" t="s">
-        <v>16</v>
+        <v>131</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -3428,10 +3428,10 @@
         <v>0</v>
       </c>
       <c r="B223" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="C223" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -3439,10 +3439,10 @@
         <v>0</v>
       </c>
       <c r="B224" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="C224" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -3450,10 +3450,10 @@
         <v>0</v>
       </c>
       <c r="B225" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="C225" t="s">
-        <v>144</v>
+        <v>193</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -3461,10 +3461,10 @@
         <v>0</v>
       </c>
       <c r="B226" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="C226" t="s">
-        <v>140</v>
+        <v>194</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -3472,10 +3472,10 @@
         <v>0</v>
       </c>
       <c r="B227" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="C227" t="s">
-        <v>146</v>
+        <v>195</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -3483,10 +3483,10 @@
         <v>0</v>
       </c>
       <c r="B228" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="C228" t="s">
-        <v>147</v>
+        <v>47</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -3494,10 +3494,10 @@
         <v>0</v>
       </c>
       <c r="B229" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="C229" t="s">
-        <v>148</v>
+        <v>197</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -3505,10 +3505,10 @@
         <v>0</v>
       </c>
       <c r="B230" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C230" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -3516,10 +3516,10 @@
         <v>0</v>
       </c>
       <c r="B231" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C231" t="s">
-        <v>186</v>
+        <v>68</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -3527,10 +3527,10 @@
         <v>0</v>
       </c>
       <c r="B232" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C232" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -3538,10 +3538,10 @@
         <v>0</v>
       </c>
       <c r="B233" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C233" t="s">
-        <v>72</v>
+        <v>199</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -3549,10 +3549,10 @@
         <v>0</v>
       </c>
       <c r="B234" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C234" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -3560,10 +3560,10 @@
         <v>0</v>
       </c>
       <c r="B235" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C235" t="s">
-        <v>188</v>
+        <v>94</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -3571,10 +3571,10 @@
         <v>0</v>
       </c>
       <c r="B236" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C236" t="s">
-        <v>131</v>
+        <v>201</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -3582,10 +3582,10 @@
         <v>0</v>
       </c>
       <c r="B237" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C237" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -3593,10 +3593,10 @@
         <v>0</v>
       </c>
       <c r="B238" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C238" t="s">
-        <v>71</v>
+        <v>181</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -3604,10 +3604,10 @@
         <v>0</v>
       </c>
       <c r="B239" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C239" t="s">
-        <v>77</v>
+        <v>202</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -3615,10 +3615,10 @@
         <v>0</v>
       </c>
       <c r="B240" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C240" t="s">
-        <v>172</v>
+        <v>27</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -3626,10 +3626,10 @@
         <v>0</v>
       </c>
       <c r="B241" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C241" t="s">
-        <v>182</v>
+        <v>30</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -3637,10 +3637,10 @@
         <v>0</v>
       </c>
       <c r="B242" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C242" t="s">
-        <v>32</v>
+        <v>203</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -3648,10 +3648,10 @@
         <v>0</v>
       </c>
       <c r="B243" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C243" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -3659,10 +3659,10 @@
         <v>0</v>
       </c>
       <c r="B244" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C244" t="s">
-        <v>189</v>
+        <v>4</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -3670,10 +3670,10 @@
         <v>0</v>
       </c>
       <c r="B245" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C245" t="s">
-        <v>146</v>
+        <v>204</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -3681,10 +3681,10 @@
         <v>0</v>
       </c>
       <c r="B246" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C246" t="s">
-        <v>140</v>
+        <v>3</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -3692,10 +3692,10 @@
         <v>0</v>
       </c>
       <c r="B247" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C247" t="s">
-        <v>178</v>
+        <v>14</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -3703,10 +3703,10 @@
         <v>0</v>
       </c>
       <c r="B248" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C248" t="s">
-        <v>117</v>
+        <v>32</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -3714,10 +3714,10 @@
         <v>0</v>
       </c>
       <c r="B249" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C249" t="s">
-        <v>107</v>
+        <v>205</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -3725,10 +3725,10 @@
         <v>0</v>
       </c>
       <c r="B250" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C250" t="s">
-        <v>138</v>
+        <v>206</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -3736,10 +3736,10 @@
         <v>0</v>
       </c>
       <c r="B251" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C251" t="s">
-        <v>25</v>
+        <v>207</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -3747,10 +3747,10 @@
         <v>0</v>
       </c>
       <c r="B252" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C252" t="s">
-        <v>136</v>
+        <v>208</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -3758,361 +3758,9 @@
         <v>0</v>
       </c>
       <c r="B253" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C253" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3">
-      <c r="A254" t="s">
-        <v>0</v>
-      </c>
-      <c r="B254" t="s">
-        <v>184</v>
-      </c>
-      <c r="C254" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3">
-      <c r="A255" t="s">
-        <v>0</v>
-      </c>
-      <c r="B255" t="s">
-        <v>192</v>
-      </c>
-      <c r="C255" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="256" spans="1:3">
-      <c r="A256" t="s">
-        <v>0</v>
-      </c>
-      <c r="B256" t="s">
-        <v>192</v>
-      </c>
-      <c r="C256" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3">
-      <c r="A257" t="s">
-        <v>0</v>
-      </c>
-      <c r="B257" t="s">
-        <v>192</v>
-      </c>
-      <c r="C257" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3">
-      <c r="A258" t="s">
-        <v>0</v>
-      </c>
-      <c r="B258" t="s">
-        <v>194</v>
-      </c>
-      <c r="C258" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3">
-      <c r="A259" t="s">
-        <v>0</v>
-      </c>
-      <c r="B259" t="s">
-        <v>194</v>
-      </c>
-      <c r="C259" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3">
-      <c r="A260" t="s">
-        <v>0</v>
-      </c>
-      <c r="B260" t="s">
-        <v>196</v>
-      </c>
-      <c r="C260" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="261" spans="1:3">
-      <c r="A261" t="s">
-        <v>0</v>
-      </c>
-      <c r="B261" t="s">
-        <v>196</v>
-      </c>
-      <c r="C261" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="262" spans="1:3">
-      <c r="A262" t="s">
-        <v>0</v>
-      </c>
-      <c r="B262" t="s">
-        <v>196</v>
-      </c>
-      <c r="C262" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="263" spans="1:3">
-      <c r="A263" t="s">
-        <v>0</v>
-      </c>
-      <c r="B263" t="s">
-        <v>196</v>
-      </c>
-      <c r="C263" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3">
-      <c r="A264" t="s">
-        <v>0</v>
-      </c>
-      <c r="B264" t="s">
-        <v>196</v>
-      </c>
-      <c r="C264" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="265" spans="1:3">
-      <c r="A265" t="s">
-        <v>0</v>
-      </c>
-      <c r="B265" t="s">
-        <v>196</v>
-      </c>
-      <c r="C265" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="266" spans="1:3">
-      <c r="A266" t="s">
-        <v>0</v>
-      </c>
-      <c r="B266" t="s">
-        <v>196</v>
-      </c>
-      <c r="C266" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3">
-      <c r="A267" t="s">
-        <v>0</v>
-      </c>
-      <c r="B267" t="s">
-        <v>196</v>
-      </c>
-      <c r="C267" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3">
-      <c r="A268" t="s">
-        <v>0</v>
-      </c>
-      <c r="B268" t="s">
-        <v>196</v>
-      </c>
-      <c r="C268" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="269" spans="1:3">
-      <c r="A269" t="s">
-        <v>0</v>
-      </c>
-      <c r="B269" t="s">
-        <v>196</v>
-      </c>
-      <c r="C269" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="270" spans="1:3">
-      <c r="A270" t="s">
-        <v>0</v>
-      </c>
-      <c r="B270" t="s">
-        <v>196</v>
-      </c>
-      <c r="C270" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="271" spans="1:3">
-      <c r="A271" t="s">
-        <v>0</v>
-      </c>
-      <c r="B271" t="s">
-        <v>196</v>
-      </c>
-      <c r="C271" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="272" spans="1:3">
-      <c r="A272" t="s">
-        <v>0</v>
-      </c>
-      <c r="B272" t="s">
-        <v>196</v>
-      </c>
-      <c r="C272" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="273" spans="1:3">
-      <c r="A273" t="s">
-        <v>0</v>
-      </c>
-      <c r="B273" t="s">
-        <v>196</v>
-      </c>
-      <c r="C273" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3">
-      <c r="A274" t="s">
-        <v>0</v>
-      </c>
-      <c r="B274" t="s">
-        <v>196</v>
-      </c>
-      <c r="C274" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3">
-      <c r="A275" t="s">
-        <v>0</v>
-      </c>
-      <c r="B275" t="s">
-        <v>196</v>
-      </c>
-      <c r="C275" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3">
-      <c r="A276" t="s">
-        <v>0</v>
-      </c>
-      <c r="B276" t="s">
-        <v>196</v>
-      </c>
-      <c r="C276" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3">
-      <c r="A277" t="s">
-        <v>0</v>
-      </c>
-      <c r="B277" t="s">
-        <v>196</v>
-      </c>
-      <c r="C277" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3">
-      <c r="A278" t="s">
-        <v>0</v>
-      </c>
-      <c r="B278" t="s">
-        <v>196</v>
-      </c>
-      <c r="C278" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3">
-      <c r="A279" t="s">
-        <v>0</v>
-      </c>
-      <c r="B279" t="s">
-        <v>196</v>
-      </c>
-      <c r="C279" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3">
-      <c r="A280" t="s">
-        <v>0</v>
-      </c>
-      <c r="B280" t="s">
-        <v>196</v>
-      </c>
-      <c r="C280" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3">
-      <c r="A281" t="s">
-        <v>0</v>
-      </c>
-      <c r="B281" t="s">
-        <v>196</v>
-      </c>
-      <c r="C281" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3">
-      <c r="A282" t="s">
-        <v>0</v>
-      </c>
-      <c r="B282" t="s">
-        <v>196</v>
-      </c>
-      <c r="C282" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="283" spans="1:3">
-      <c r="A283" t="s">
-        <v>0</v>
-      </c>
-      <c r="B283" t="s">
-        <v>196</v>
-      </c>
-      <c r="C283" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3">
-      <c r="A284" t="s">
-        <v>0</v>
-      </c>
-      <c r="B284" t="s">
-        <v>196</v>
-      </c>
-      <c r="C284" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="285" spans="1:3">
-      <c r="A285" t="s">
-        <v>0</v>
-      </c>
-      <c r="B285" t="s">
-        <v>196</v>
-      </c>
-      <c r="C285" t="s">
         <v>209</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update judgment and change the sentences to output of Stanford NER
</commit_message>
<xml_diff>
--- a/sentence_level/data/sentences/remove_single/2012_leap_day_tornado.xlsx
+++ b/sentence_level/data/sentences/remove_single/2012_leap_day_tornado.xlsx
@@ -14,30 +14,423 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="186">
   <si>
     <t>2012_leap_day_tornado</t>
   </si>
   <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>At least 13 dead in storms working across Missouri, Illinois.</t>
+  </si>
+  <si>
+    <t>At least 10 people were killed in the southern Illinois town of Harrisburg after a storm leveled much of the community of 9,000 people.</t>
+  </si>
+  <si>
+    <t>From Tuesday night into Wednesday morning, at least 16 tornado sightings were reported from Nebraska and Kansas across southern Missouri to Illinois and Kentucky, according to the storm center, an arm of the National Weather Service.</t>
+  </si>
+  <si>
+    <t>Many people are asking how they can help after a preliminary EF4 tornado hit Saline County, Illinois killing six people.</t>
+  </si>
+  <si>
+    <t>It is the deadliest state disaster in Illinois in nearly a decade.</t>
+  </si>
+  <si>
+    <t>Illinois Gov. Pat Quinn signed state disaster declaration at the podium at a 2 p.m. press conference in Harrisburg Wednesday.</t>
+  </si>
+  <si>
+    <t>Quinn says he's already talked to President Obama and that Illinois is banding together as a family to help Harrisburg recover and rebuild.</t>
+  </si>
+  <si>
+    <t>Ameren Illinois representatives say more than 430 personnel were deployed to southern Illinois.</t>
+  </si>
+  <si>
+    <t>David Serby in Perry County, Illinois says a few outbuildings were blown over with some tree damage.</t>
+  </si>
+  <si>
+    <t>Leap Day was not a good one for thousands of people in the Midwest and Southern United States as severe storms and tornadoes left a trail of destruction in Illinois, Missouri, Kansas, Arkansas, Oklahoma, Kentucky, and Tennessee.</t>
+  </si>
+  <si>
+    <t>But none faced the wrath of Mother Nature like the southern Illinois town of Harrisburg.</t>
+  </si>
+  <si>
+    <t>Metropolis</t>
+  </si>
+  <si>
+    <t>The tornado then crossed the Ohio River again and lifted around two miles northwest of Metropolis just east of the airport.</t>
+  </si>
+  <si>
+    <t>Ill.</t>
+  </si>
+  <si>
+    <t>Storm shelters have been opened up for those in need in southern Ill. and southeast Mo.</t>
+  </si>
+  <si>
+    <t>Reports are the tornado touched down just southwest of Mounds, Ill. and crossed over I-57 near exit 8.</t>
+  </si>
+  <si>
+    <t>NWS reports are a tornado touched down just southwest of Mounds, Ill. and crossed over I-57 near exit 8.</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>In Missouri, one person was killed in a trailer park in the town of Buffalo, and at least three people were critically injured in the small eastern Kansas town of Harveyville.</t>
+  </si>
+  <si>
+    <t>In neighboring Kansas, the National Weather Service reported brief tornado touchdowns southwest of Hutchinson, and Gov. Sam Brownback declared a state of emergency after an apparent tornado struck Harveyville.</t>
+  </si>
+  <si>
+    <t>One person was killed in Kansas.</t>
+  </si>
+  <si>
+    <t>"On behalf of the U.S. Department of Homeland Security's Federal Emergency Management Agency (FEMA), I would like to express our deepest condolences to the families of those who were killed and injured by tornadoes that impacted Kansas, Missouri and Nebraska late last night and into this morning.</t>
+  </si>
+  <si>
+    <t>Saline County</t>
+  </si>
+  <si>
+    <t>Crews with Ameren Illinois have issued a safety warning to all residents in and around Saline County.</t>
+  </si>
+  <si>
+    <t>The National Weather Service reports an EF4 tornado hit Saline County on the southwest side of Harrisburg, killing six people.</t>
+  </si>
+  <si>
+    <t>Four females and two males, all adults, were killed in Saline County.</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Michigan, Connecticut and Massachusetts on Wednesday were spared from tornados but visited by snowy weather — a shock after this winter’s consistently warm temperatures.</t>
+  </si>
+  <si>
+    <t>The National Weather Service issued overnight advisories of snow and rain in all three states, warning of an ice coating followed by freezing rain in Michigan, a “bit of snow” followed by “lots of rain” in Connecticut, and up to 10 inches of snow in Eastern Massachusetts.</t>
+  </si>
+  <si>
+    <t>SEOC</t>
+  </si>
+  <si>
+    <t>IEMA regional personnel were deployed to Harrisburg soon after the storms and representatives from the Illinois State Police, departments of Transportation, Central Management Services, Corrections, Public Health and Natural Resources, along with the American Red Cross, reported to the SEOC soon thereafter.</t>
+  </si>
+  <si>
+    <t>The governor says the SEOC will remain activated as long as necessary.</t>
+  </si>
+  <si>
+    <t>Ameren Illinois</t>
+  </si>
+  <si>
+    <t>More than 400 people are working to restore power to Ameren Illinois customers.</t>
+  </si>
+  <si>
+    <t>People should not call 911 or the dispatch center to report power line outages, please contact Ameren Illinois direct.</t>
+  </si>
+  <si>
+    <t>Ameren Illinois doesn't have a time of when power will be restored.</t>
+  </si>
+  <si>
+    <t>As of 4:10 a.m. Thursday, Ameren Illinois reports outages in:  Copyright 2012 KFVS.</t>
+  </si>
+  <si>
+    <t>Saint Francis Medical Center</t>
+  </si>
+  <si>
+    <t>A total of eight patients from Stoddard County are being treated at Saint Francis Medical Center.</t>
+  </si>
+  <si>
+    <t>Mark Champlin, 50, of Puxico was pronounced dead at 7:35 a.m. at Saint Francis Medical Center in Cape Girardeau.</t>
+  </si>
+  <si>
+    <t>Heartland</t>
+  </si>
+  <si>
+    <t>5 confirmed tornadoes in the Heartland.</t>
+  </si>
+  <si>
+    <t>See pictures from across the Heartland after severe storms on Feb. 29, 2012.</t>
+  </si>
+  <si>
+    <t>See more pictures from across the Heartland after severe storms on Feb. 29, 2012.</t>
+  </si>
+  <si>
+    <t>See the National Weather Service storm damage reports from the tornadoes and severe storms that swept through the Heartland early Feb. 29.</t>
+  </si>
+  <si>
+    <t>How you can help after the tornadoes  How you can help after the tornadoes  Eight people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
+  </si>
+  <si>
+    <t>Seven of those tornadoes were in the Heartland.</t>
+  </si>
+  <si>
+    <t>Eight people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
+  </si>
+  <si>
+    <t>Disaster in the Heartland - one year later  Disaster in the Heartland - one year later  The storm drove this plywood piece through the wall of a garage in Harrisburg,  Seven people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
+  </si>
+  <si>
+    <t>Five of those tornadoes were in the Heartland.</t>
+  </si>
+  <si>
+    <t>[More damage across the Heartland.]</t>
+  </si>
+  <si>
+    <t>Severe storms and tornadoes tear through the Heartland.</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>One man was killed outside Puxico, Missouri in the storms.</t>
+  </si>
+  <si>
+    <t>Two people were killed in southwest Missouri.</t>
+  </si>
+  <si>
+    <t>Missouri Gov. Jan Nixon has declared a state of emergency.</t>
+  </si>
+  <si>
+    <t>Waves of strong storms devastated small communities and damaged the country music resort town of Branson, Missouri.</t>
+  </si>
+  <si>
+    <t>Stoddard County Coroner</t>
+  </si>
+  <si>
+    <t>The Stoddard County Coroner confirms one person has died as a result of overnight storms.</t>
+  </si>
+  <si>
+    <t>Mo.</t>
+  </si>
+  <si>
+    <t>Branson, Mo. tornado, National Weather Service snow alerts and more Leap Year weather.</t>
+  </si>
+  <si>
+    <t>A Puxico, Mo. man was killed in Stoddard County.</t>
+  </si>
+  <si>
+    <t>The school and a church sustained damage in Oak Ridge, Mo. in Cape Girardeau County.</t>
+  </si>
+  <si>
+    <t>First Baptist Church</t>
+  </si>
+  <si>
+    <t>According to the sheriff's office, the shelter is open at the First Baptist Church at 204 North Main Street.</t>
+  </si>
+  <si>
+    <t>Donations may be made to the Red Cross at the First Baptist Church, The Salvation Army at 10 West Locust in Harrisburg or Christian Compassion Care Center at PO Box 422 in Harrisburg.</t>
+  </si>
+  <si>
+    <t>Pulaski County</t>
+  </si>
+  <si>
+    <t>Pulaski County, Illinois EMS Director Ken Kerley says wreckers and vehicles were blown from their location and crossing arms broke off and blew into a squad car.</t>
+  </si>
+  <si>
+    <t>No injuries have been reported in Pulaski County.</t>
+  </si>
+  <si>
+    <t>Cape Girardeau County</t>
+  </si>
+  <si>
+    <t>Team 1 (Rick Shanklin, Ken Ludington) - Harrisburg west toward Cape Girardeau County MO  Team 2 (Kelly Hooper, Shane Luecke) - Newburg IN West toward Harrisburg IL)  Team 3 (Christine Wielgos, Debbie Hooper) - Metropolis IL west toward Stoddard co.</t>
+  </si>
+  <si>
+    <t>Stoddard County</t>
+  </si>
+  <si>
+    <t>You can drive for miles in Stoddard County and never see damage, but a path left from the strong winds that did blow through, show the wreckage.</t>
+  </si>
+  <si>
+    <t>The Stoddard County coroner says Mark Champlin, 50, of Puxico was killed.</t>
+  </si>
+  <si>
+    <t>A second tornado in Stoddard County Wednesday morning started just east of Bell City to three miles southeast of Benton, Mo.</t>
+  </si>
+  <si>
+    <t>One man has died after the storms in Stoddard County.</t>
+  </si>
+  <si>
+    <t>They are all storm related injuries from Stoddard County.</t>
+  </si>
+  <si>
+    <t>Stoddard County Sheriff Carl Hefner says several mobile homes in the area are destroyed in Stoddard County.</t>
+  </si>
+  <si>
+    <t>Stoddard County Coroner Aaron Mathis has released the name of the man killed in Puxico Wednesday morning after a tornado moved through the area.</t>
+  </si>
+  <si>
+    <t>Highway Patrol Trooper Clark Parrott says large trees are down along Route M in Stoddard County.</t>
+  </si>
+  <si>
+    <t>NWS</t>
+  </si>
+  <si>
+    <t>The NWS confirms preliminary reports of an EF2 tornado that went through McCracken and Ballard counties in Ky.</t>
+  </si>
+  <si>
+    <t>NWS teams were in Stoddard and Cape Girardeau counties on Thursday surveying damage.</t>
+  </si>
+  <si>
+    <t>An EF3 tornado was confirmed by the NWS.</t>
+  </si>
+  <si>
+    <t>According to NWS, numerous trees near the house were also uprooted.</t>
+  </si>
+  <si>
+    <t>Oak Ridge</t>
+  </si>
+  <si>
+    <t>People are using the school in Oak Ridge as a staging area to head out to help those in the area.</t>
+  </si>
+  <si>
+    <t>The Red Cross is providing food and water to residents and emergency workers in Oak Ridge as they work on cleaning up from the storm damage.</t>
+  </si>
+  <si>
+    <t>According to Emergency Management, all roads are back open in the Oak Ridge area.</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>America</t>
+  </si>
+  <si>
+    <t>The tornado then crossed the Ohio River near the town of America, then across McCracken and Ballard counties.</t>
+  </si>
+  <si>
+    <t>The tornado then crossed the Ohio River near the town of America, then across McCracken and Ballard Counties.</t>
+  </si>
+  <si>
+    <t>U.S.</t>
+  </si>
+  <si>
+    <t>The National Weather Service’s U.S. map Wednesday was covered by colorful wintry and storm warnings:</t>
+  </si>
+  <si>
+    <t>Corey Mead, lead forecaster at the U.S. Storm Prediction Center in Norman, Okla., said a broad cold front was slamming into warm, humid air over much of the eastern half of the nation.</t>
+  </si>
+  <si>
+    <t>Mo</t>
+  </si>
+  <si>
+    <t>Associated Press photographer Mark Schiefelbein contributed to this report from Branson, Mo.</t>
+  </si>
+  <si>
+    <t>The National Weather Service confirms preliminary reports of an EF2 in Marquand in Madison County, Mo.</t>
+  </si>
+  <si>
+    <t>Buffalo</t>
+  </si>
+  <si>
+    <t>Farther north, rescue crews waited for sunrise to begin searching a trailer park south of Buffalo where at least one person was killed after an apparent twister slammed the area.</t>
+  </si>
+  <si>
+    <t>Buffalo is about 35 miles north of Springfield.</t>
+  </si>
+  <si>
+    <t>Heartland News</t>
+  </si>
+  <si>
+    <t>The mayor of Harrisburg tells Heartland News that this is a horrific event.</t>
+  </si>
+  <si>
+    <t>Emergency Manager Dale Moreland tells Heartland News it looks like the mobile home  "exploded."</t>
+  </si>
+  <si>
+    <t>Moreland told Heartland News Wednesday morning that there is extensive damage everywhere, and power lines down across several miles.</t>
+  </si>
+  <si>
+    <t>Her sister, Judie LaChance tells Heartland News that Sandy Hemby will be okay.</t>
+  </si>
+  <si>
+    <t>Heartland News reporter Carly O'Keefe reports grain bins in fields and more damage in Gallatin County.</t>
+  </si>
+  <si>
     <t>Red Cross</t>
   </si>
   <si>
-    <t>The Red Cross is providing food and water to residents and emergency workers in Oak Ridge as they work on cleaning up from the storm damage.</t>
-  </si>
-  <si>
-    <t>Donations may be made to the Red Cross at the First Baptist Church, The Salvation Army at 10 West Locust in Harrisburg or Christian Compassion Care Center at PO Box 422 in Harrisburg.</t>
-  </si>
-  <si>
-    <t>IEMA regional personnel were deployed to Harrisburg soon after the storms and representatives from the Illinois State Police, departments of Transportation, Central Management Services, Corrections, Public Health and Natural Resources, along with the American Red Cross, reported to the SEOC soon thereafter.</t>
-  </si>
-  <si>
     <t>Oklahoma</t>
   </si>
   <si>
     <t>In northern Oklahoma, gusts of up to 80 mph flipped trailers and damaged homes near Cherokee.</t>
   </si>
   <si>
-    <t>Leap Day was not a good one for thousands of people in the Midwest and Southern United States as severe storms and tornadoes left a trail of destruction in Illinois, Missouri, Kansas, Arkansas, Oklahoma, Kentucky, and Tennessee.</t>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>The system also skirted northern Arkansas, bringing gusts of up to 60 mph in the northwest.</t>
+  </si>
+  <si>
+    <t>Residents of Clay County in northeastern Arkansas reported hail the size of golf balls, while half dollar-sized hail was reported in Mountain Home.</t>
+  </si>
+  <si>
+    <t>Midwest</t>
+  </si>
+  <si>
+    <t>Three people were killed in Tennessee after the same severe weather system that created massive damage across the Midwest moved through the state.</t>
+  </si>
+  <si>
+    <t>Associated Press</t>
+  </si>
+  <si>
+    <t>JIM SALTER,Associated Press.</t>
+  </si>
+  <si>
+    <t>According to the Associated Press Darrell Osman says his mother, 75-year-old Mary Osman, was among the dead.</t>
+  </si>
+  <si>
+    <t>The Associated Press contributed to report.</t>
+  </si>
+  <si>
+    <t>Ameren</t>
+  </si>
+  <si>
+    <t>Ameren has open a customer service center in Harrisburg.</t>
+  </si>
+  <si>
+    <t>Ameren reports 14,000 without power at the peak.</t>
+  </si>
+  <si>
+    <t>Ameren hopes to have all power restored by the end of the day Friday.</t>
+  </si>
+  <si>
+    <t>Fire Department</t>
+  </si>
+  <si>
+    <t>Generators will be brought to the Oasis Tavern, just south of the Fire Department.</t>
+  </si>
+  <si>
+    <t>Food and drink is available at the Fire Department.</t>
+  </si>
+  <si>
+    <t>Ohio River</t>
+  </si>
+  <si>
+    <t>Ballard Counties</t>
+  </si>
+  <si>
+    <t>The National Weather Service confirms preliminary reports of an EF2 tornado that went through McCracken and Ballard Counties in Ky.</t>
+  </si>
+  <si>
+    <t>Marquand</t>
+  </si>
+  <si>
+    <t>The National Weather Service confirms preliminary reports of an EF1 in Marquand.</t>
+  </si>
+  <si>
+    <t>Ky</t>
+  </si>
+  <si>
+    <t>Puxico</t>
+  </si>
+  <si>
+    <t>The damage is along County Roads 266 and 257 east of Puxico and tracked to the northeast to the Leora area.</t>
+  </si>
+  <si>
+    <t>Johnnie Clark, the city manager in Puxico, says most of the damage is in the rural areas near town.</t>
+  </si>
+  <si>
+    <t>No major damage is reported in Puxico city limits.</t>
   </si>
   <si>
     <t>Eldorado</t>
@@ -46,406 +439,127 @@
     <t>They are Mary Osman, 75, of Harrisburg, Jaylynn Ferrell, 22, of Harrisburg, Lynda Hull, 74, of Galatia, Donna Rann, 61, of Eldorado, and Randy Rann, 64, of Eldorado.</t>
   </si>
   <si>
-    <t>Illinois</t>
-  </si>
-  <si>
-    <t>Many people are asking how they can help after a preliminary EF4 tornado hit Saline County, Illinois killing six people.</t>
-  </si>
-  <si>
-    <t>Quinn directed the Illinois Emergency Management Agency to activate the State Emergency Operations Center (SEOC) in Springfield.</t>
-  </si>
-  <si>
-    <t>At least 13 dead in storms working across Missouri, Illinois.</t>
-  </si>
-  <si>
-    <t>But none faced the wrath of Mother Nature like the southern Illinois town of Harrisburg.</t>
-  </si>
-  <si>
-    <t>From Tuesday night into Wednesday morning, at least 16 tornado sightings were reported from Nebraska and Kansas across southern Missouri to Illinois and Kentucky, according to the storm center, an arm of the National Weather Service.</t>
-  </si>
-  <si>
-    <t>Quinn says he's already talked to President Obama and that Illinois is banding together as a family to help Harrisburg recover and rebuild.</t>
-  </si>
-  <si>
-    <t>It is the deadliest state disaster in Illinois in nearly a decade.</t>
-  </si>
-  <si>
-    <t>Pulaski County, Illinois EMS Director Ken Kerley says wreckers and vehicles were blown from their location and crossing arms broke off and blew into a squad car.</t>
-  </si>
-  <si>
-    <t>David Serby in Perry County, Illinois says a few outbuildings were blown over with some tree damage.</t>
-  </si>
-  <si>
-    <t>The United Way of South Central Illinois, located at 1101 Broadway in Mt.</t>
-  </si>
-  <si>
-    <t>At least 10 people were killed in the southern Illinois town of Harrisburg after a storm leveled much of the community of 9,000 people.</t>
-  </si>
-  <si>
-    <t>The Southern Illinois Egyptian Health Department says if you are experiencing a power outage:  -Keep your freezer/refrigerator door closed to maintain temperatures.</t>
-  </si>
-  <si>
-    <t>Illinois Gov.</t>
-  </si>
-  <si>
-    <t>Pulaski County</t>
-  </si>
-  <si>
-    <t>No injuries have been reported in Pulaski County.</t>
-  </si>
-  <si>
-    <t>Cape Girardeau County</t>
-  </si>
-  <si>
-    <t>Team 1 (Rick Shanklin, Ken Ludington) - Harrisburg west toward Cape Girardeau County MO  Team 2 (Kelly Hooper, Shane Luecke) - Newburg IN West toward Harrisburg IL)  Team 3 (Christine Wielgos, Debbie Hooper) - Metropolis IL west toward Stoddard co. MO)  Note this may change as storms are in western Kentucky.</t>
-  </si>
-  <si>
-    <t>in Cape Girardeau County.</t>
-  </si>
-  <si>
-    <t>Saline County</t>
+    <t>FEMA</t>
+  </si>
+  <si>
+    <t>FEMA Regional Administrator Beth Freeman released this statement.</t>
+  </si>
+  <si>
+    <t>FEMA has been in constant contact with officials at the Kansas Department of Emergency Management (KDEM), Missouri State Emergency Management Agency (SEMA) and the Nebraska Emergency Management Agency (NEMA) since the severe weather hit.</t>
+  </si>
+  <si>
+    <t>Springfield</t>
+  </si>
+  <si>
+    <t>Regular agency reports have been on the local Hometown Radio News all day, in addition to the Springfield television and network coverage.</t>
+  </si>
+  <si>
+    <t>Earlier Wednesday, Gov. Quinn directed the Illinois Emergency Management Agency to activate the State Emergency Operations Center (SEOC) in Springfield.</t>
+  </si>
+  <si>
+    <t>Mounds</t>
+  </si>
+  <si>
+    <t>Harrisburg</t>
+  </si>
+  <si>
+    <t>It touched down around 4:51 a.m. one mile north of Carrier Mills and traveled ENE toward Harrisburg, touching down in Harrisburg at 4:56 a.m.</t>
+  </si>
+  <si>
+    <t>"This morning the city of Harrisburg suffered a horrific event," said Harrisburg mayor Eric Gregg.</t>
   </si>
   <si>
     <t>At least 100 people have been injured in the Harrisburg area, according to the Saline County Sheriff's Office.</t>
   </si>
   <si>
-    <t>Crews with Ameren Illinois have issued a safety warning to all residents in and around Saline County.</t>
-  </si>
-  <si>
-    <t>The National Weather Service reports an EF4 tornado hit Saline County on the southwest side of Harrisburg, killing six people.</t>
-  </si>
-  <si>
-    <t>Four females and two males, all adults, were killed in Saline County.</t>
-  </si>
-  <si>
-    <t>Saline County Emergency Management asks people to stay off their cell phones if possible as heavy phone traffic is jamming the system.</t>
-  </si>
-  <si>
-    <t>Stoddard County</t>
-  </si>
-  <si>
-    <t>A total of eight patients from Stoddard County are being treated at Saint Francis Medical Center.</t>
-  </si>
-  <si>
-    <t>One man has died after the storms in Stoddard County.</t>
-  </si>
-  <si>
-    <t>Stoddard County Sheriff Carl Hefner says several mobile homes in the area are destroyed in Stoddard County.</t>
-  </si>
-  <si>
-    <t>The Stoddard County coroner says Mark Champlin, 50, of Puxico was killed.</t>
-  </si>
-  <si>
-    <t>Highway Patrol Trooper Clark Parrott says large trees are down along Route M in Stoddard County.</t>
-  </si>
-  <si>
-    <t>You can drive for miles in Stoddard County and never see damage, but a path left from the strong winds that did blow through, show the wreckage.</t>
-  </si>
-  <si>
-    <t>man was killed in Stoddard County.</t>
-  </si>
-  <si>
-    <t>Hefner says they started receiving calls around 4 a.m.  Dale Moreland with Stoddard County EMA says one mobile home was moved about 200 feet.</t>
-  </si>
-  <si>
-    <t>They are all storm related injuries from Stoddard County.</t>
-  </si>
-  <si>
-    <t>A second tornado in Stoddard County Wednesday morning started just east of Bell City to three miles southeast of Benton, Mo.</t>
-  </si>
-  <si>
-    <t>Midwest</t>
-  </si>
-  <si>
-    <t>Disaster in the Heartland - one year later  Disaster in the Heartland - one year later  The storm drove this plywood piece through the wall of a garage in Harrisburg,  Seven people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
-  </si>
-  <si>
-    <t>How you can help after the tornadoes  How you can help after the tornadoes  Eight people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
-  </si>
-  <si>
-    <t>Three people were killed in Tennessee after the same severe weather system that created massive damage across the Midwest moved through the state.</t>
-  </si>
-  <si>
-    <t>Midwest Tornadoes: News, Photos, and Video of the Destruction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDATED: At Least 12 People Killed In Deadly Midwest Storms. </t>
-  </si>
-  <si>
-    <t>Eight people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
-  </si>
-  <si>
-    <t>FEMA</t>
-  </si>
-  <si>
-    <t>"On behalf of the U.S. Department of Homeland Security's Federal Emergency Management Agency (FEMA), I would like to express our deepest condolences to the families of those who were killed and injured by tornadoes that impacted Kansas, Missouri and Nebraska late last night and into this morning.</t>
-  </si>
-  <si>
-    <t>FEMA has been in constant contact with officials at the Kansas Department of Emergency Management (KDEM), Missouri State Emergency Management Agency (SEMA) and the Nebraska Emergency Management Agency (NEMA) since the severe weather hit.</t>
-  </si>
-  <si>
-    <t>FEMA Regional Administrator Beth Freeman released this statement.</t>
-  </si>
-  <si>
-    <t>Springfield</t>
-  </si>
-  <si>
-    <t>Buffalo is about 35 miles north of Springfield.</t>
-  </si>
-  <si>
-    <t>Regular agency reports have been on the local Hometown Radio News all day, in addition to the Springfield television and network coverage.</t>
-  </si>
-  <si>
-    <t>Associated Press</t>
-  </si>
-  <si>
-    <t>Associated Press photographer Mark Schiefelbein contributed to this report from Branson, Mo.</t>
-  </si>
-  <si>
-    <t>The Associated Press contributed to report.</t>
-  </si>
-  <si>
-    <t>JIM SALTER,Associated Press.</t>
-  </si>
-  <si>
-    <t>According to the Associated Press Darrell Osman says his mother, 75-year-old Mary Osman, was among the dead.</t>
-  </si>
-  <si>
-    <t>Ameren</t>
-  </si>
-  <si>
-    <t>Ameren hopes to have all power restored by the end of the day Friday.</t>
-  </si>
-  <si>
-    <t>Ameren reports 14,000 without power at the peak.</t>
-  </si>
-  <si>
-    <t>Ameren has open a customer service center in Harrisburg.</t>
-  </si>
-  <si>
-    <t>Metropolis</t>
-  </si>
-  <si>
-    <t>The tornado then crossed the Ohio River again and lifted around two miles northwest of Metropolis just east of the airport.</t>
-  </si>
-  <si>
-    <t>NWS</t>
-  </si>
-  <si>
-    <t>The NWS confirms preliminary reports of an EF2 tornado that went through McCracken and Ballard counties in Ky.  Reports are the tornado touched down just southwest of Mounds, Ill. and crossed over I-57 near exit 8.</t>
-  </si>
-  <si>
-    <t>NWS reports are a tornado touched down just southwest of Mounds, Ill. and crossed over I-57 near exit 8.</t>
-  </si>
-  <si>
-    <t>Further west, a house was destroyed on County Road 431 just north of Highway C.    According to NWS, numerous trees near the house were also uprooted.</t>
-  </si>
-  <si>
-    <t>An EF3 tornado was confirmed by the NWS.</t>
-  </si>
-  <si>
-    <t>NWS teams were in Stoddard and Cape Girardeau counties on Thursday surveying damage.</t>
-  </si>
-  <si>
-    <t>Mounds</t>
-  </si>
-  <si>
-    <t>Crystal Britt is just east of Mounds.</t>
-  </si>
-  <si>
-    <t>The school in Mounds also received damage.</t>
-  </si>
-  <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>Michigan, Connecticut and Massachusetts on Wednesday were spared from tornados but visited by snowy weather — a shock after this winter’s consistently warm temperatures.</t>
-  </si>
-  <si>
-    <t>The National Weather Service issued overnight advisories of snow and rain in all three states, warning of an ice coating followed by freezing rain in Michigan, a “bit of snow” followed by “lots of rain” in Connecticut, and up to 10 inches of snow in Eastern Massachusetts.</t>
-  </si>
-  <si>
-    <t>Kansas</t>
-  </si>
-  <si>
-    <t>In Missouri, one person was killed in a trailer park in the town of Buffalo, and at least three people were critically injured in the small eastern Kansas town of Harveyville.</t>
-  </si>
-  <si>
-    <t>In neighboring Kansas, the National Weather Service reported brief tornado touchdowns southwest of Hutchinson, and Gov.</t>
-  </si>
-  <si>
-    <t>One person was killed in Kansas.</t>
-  </si>
-  <si>
-    <t>Fire Department</t>
-  </si>
-  <si>
-    <t>First Responders and media are to report to the Ridgway Fire Department on West Main Street to sign in.</t>
-  </si>
-  <si>
-    <t>For those whose homes are damaged, officials are asking victims to sign up at the Fire Department to request lodging, tarpaulins, and other supplies.</t>
-  </si>
-  <si>
-    <t>Generators will be brought to the Oasis Tavern, just south of the Fire Department.</t>
-  </si>
-  <si>
-    <t>Food and drink is available at the Fire Department.</t>
-  </si>
-  <si>
-    <t>Connecticut</t>
+    <t>At least 300 houses have been damaged or destroyed with at least 25 businesses damaged or destroyed in the Harrisburg area, according to the sheriff's office.</t>
+  </si>
+  <si>
+    <t>Siteseers are asked to stay away from the City of Harrisburg.</t>
+  </si>
+  <si>
+    <t>The superintendent of schools in Harrisburg has canceled classes the rest of week.</t>
+  </si>
+  <si>
+    <t>Tyler Profilet reports a lot of damage in the Harrisburg area, including semi trucks tipped over.</t>
+  </si>
+  <si>
+    <t>Several roads are block off in Harrisburg.</t>
+  </si>
+  <si>
+    <t>All volunteers in Harrisburg must register at the SIC Foundation building on North Commercial St. starting at 7 a.m. on March 1.</t>
+  </si>
+  <si>
+    <t>Harrisburg Police Chief Bob Smith says Rural King and the SIC foundation building are set up as meeting areas for manpower and equipment.</t>
+  </si>
+  <si>
+    <t>The United Way of South Central Illinois, located at 1101 Broadway in Mt. Vernon (the Old Integra Bank Building) will serve as a drop off site for items for the tornado victims in Harrisburg, IL.</t>
+  </si>
+  <si>
+    <t>Smith says 24/7 law enforcement protection will be available in Harrisburg for as long as needed.</t>
+  </si>
+  <si>
+    <t>HARRISBURG -- The Leap Day tornado that devastated parts of Harrisburg Tuesday completely destroyed the strip shopping center south of the Walmart parking lot and caused "significant roof and water damage" to Walmart itself.</t>
   </si>
   <si>
     <t>Walmart</t>
   </si>
   <si>
-    <t xml:space="preserve">HARRISBURG -- The Leap Day tornado that devastated parts of Harrisburg Tuesday completely destroyed the strip shopping center south of the Walmart parking lot and caused "significant roof and water damage" to Walmart itself.  </t>
-  </si>
-  <si>
-    <t>SEOC</t>
-  </si>
-  <si>
-    <t>The governor says the SEOC will remain activated as long as necessary.</t>
-  </si>
-  <si>
-    <t>Ameren Illinois</t>
-  </si>
-  <si>
-    <t>Ameren Illinois representatives say more than 430 personnel were deployed to southern Illinois.</t>
-  </si>
-  <si>
-    <t>More than 400 people are working to restore power to Ameren Illinois customers.</t>
-  </si>
-  <si>
-    <t>People should not call 911 or the dispatch center to report power line outages, please contact Ameren Illinois direct.</t>
-  </si>
-  <si>
-    <t>As of 4:10 a.m. Thursday, Ameren Illinois reports outages in:  Copyright 2012 KFVS.</t>
-  </si>
-  <si>
-    <t>Ameren Illinois doesn't have a time of when power will be restored.</t>
-  </si>
-  <si>
-    <t>America</t>
-  </si>
-  <si>
-    <t>The tornado then crossed the Ohio River near the town of America, then across McCracken and Ballard Counties.</t>
-  </si>
-  <si>
-    <t>The tornado then crossed the Ohio River near the town of America, then across McCracken and Ballard counties.</t>
-  </si>
-  <si>
-    <t>Heartland</t>
-  </si>
-  <si>
-    <t>[More damage across the Heartland.]</t>
-  </si>
-  <si>
-    <t>Severe storms and tornadoes tear through the Heartland.</t>
-  </si>
-  <si>
-    <t>See pictures from across the Heartland after severe storms on Feb. 29, 2012.</t>
-  </si>
-  <si>
-    <t>See the National Weather Service storm damage reports from the tornadoes and severe storms that swept through the Heartland early Feb. 29.</t>
-  </si>
-  <si>
-    <t>Seven of those tornadoes were in the Heartland.</t>
-  </si>
-  <si>
-    <t>See more pictures from across the Heartland after severe storms on Feb. 29, 2012.</t>
-  </si>
-  <si>
-    <t>Five of those tornadoes were in the Heartland.</t>
-  </si>
-  <si>
-    <t>5 confirmed tornadoes in the Heartland.</t>
-  </si>
-  <si>
-    <t>Mo.</t>
-  </si>
-  <si>
-    <t>A Puxico, Mo.</t>
-  </si>
-  <si>
-    <t>The National Weather Service confirms preliminary reports of an EF2 in Marquand in Madison County, Mo.</t>
-  </si>
-  <si>
-    <t>Branson, Mo.</t>
-  </si>
-  <si>
-    <t>The school and a church sustained damage in Oak Ridge, Mo.</t>
-  </si>
-  <si>
-    <t>Storm shelters have been opened up for those in need in southern Ill. and southeast Mo.</t>
-  </si>
-  <si>
-    <t>Ohio River</t>
-  </si>
-  <si>
     <t>Ridgway</t>
   </si>
   <si>
-    <t>Carly O'Keefe reports Ridgway's St. Joseph's catholic church leveled by storm.</t>
-  </si>
-  <si>
-    <t>Carly O'Keefe reports that there were 13 injuries in Ridgway.</t>
+    <t>One with serious injuries and the rest minor injuries  She says Tin Shop Hardware Store in Ridgway crushed by wind.</t>
   </si>
   <si>
     <t>The roads in Ridgway are closed to through traffic.</t>
   </si>
   <si>
-    <t>One with serious injuries and the rest minor injuries  She says Tin Shop Hardware Store in Ridgway crushed by wind.</t>
-  </si>
-  <si>
-    <t>A shelter is being set up at the Golden Circle Senior Center in Ridgway.</t>
-  </si>
-  <si>
     <t>Town officials have established a curfew from 9 a.m. to 6 a.m. in Ridgway.</t>
   </si>
   <si>
-    <t>Heavy equipment that is brought into the area will be staged at the Seed Company, just west of Ridgway.</t>
-  </si>
-  <si>
     <t>Cape Girardeau</t>
   </si>
   <si>
-    <t>Mark Champlin, 50, of Puxico was pronounced dead at 7:35 a.m. at Saint Francis Medical Center in Cape Girardeau.</t>
-  </si>
-  <si>
     <t>He says there were residents ejected from a mobile home and two people airlifted to a hospital in Cape Girardeau.</t>
   </si>
   <si>
     <t>Moreland says the victim was found in a nearby field and airlifted to a Cape Girardeau hospital and later died.</t>
   </si>
   <si>
-    <t>Ballard Counties</t>
-  </si>
-  <si>
-    <t>The National Weather Service confirms preliminary reports of an EF2 tornado that went through McCracken and Ballard Counties in Ky.</t>
-  </si>
-  <si>
-    <t>Marquand</t>
-  </si>
-  <si>
-    <t>The National Weather Service confirms preliminary reports of an EF1 in Marquand.</t>
-  </si>
-  <si>
-    <t>U.S.</t>
-  </si>
-  <si>
-    <t>Corey Mead, lead forecaster at the U.S. Storm Prediction Center in Norman, Okla., said a broad cold front was slamming into warm, humid air over much of the eastern half of the nation.</t>
-  </si>
-  <si>
-    <t>The National Weather Service’s U.S. map Wednesday was covered by colorful wintry and storm warnings:</t>
-  </si>
-  <si>
     <t>Kentucky</t>
   </si>
   <si>
+    <t>Tornado warnings and watches were posted for most of Kentucky and a large portion of Kentucky.</t>
+  </si>
+  <si>
     <t>A National Weather Service team has determined at least 1 of the strong storms that swept through Kentucky was an EF2 tornado packing winds of 125 miles per hour.</t>
   </si>
   <si>
-    <t>Tornado warnings and watches were posted for most of Kentucky and a large portion of Kentucky.</t>
+    <t>MO)  Note this may change as storms are in western Kentucky.</t>
+  </si>
+  <si>
+    <t>Wal-Mart</t>
+  </si>
+  <si>
+    <t>He says the windows and doors have been blown out of the Wal-Mart in town.</t>
+  </si>
+  <si>
+    <t>Wal-Mart area severely damaged by tornado.</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>National Weather Service</t>
+  </si>
+  <si>
+    <t>Some Leap Year babies woke up Wednesday to find their uncommon birthday plagued by school closings, National Weather Service snow alerts and even a tornado.</t>
+  </si>
+  <si>
+    <t>Preliminary reports from the National Weather Service report large oak trees were found uprooted and damage to roofs was consistent with EF1 damage on the enhanced Fujita scale.</t>
+  </si>
+  <si>
+    <t>The National Weather Service is sending three teams to survey the damage.</t>
   </si>
   <si>
     <t>Tennessee</t>
@@ -454,196 +568,10 @@
     <t>The tornadoes were spawned by a powerful storm system that blew down from the Rockies on Tuesday and was headed across the Ohio and Tennessee river valleys toward the Mid-Atlantic region.</t>
   </si>
   <si>
-    <t>Wal-Mart</t>
-  </si>
-  <si>
-    <t>He says the windows and doors have been blown out of the Wal-Mart in town.</t>
-  </si>
-  <si>
-    <t>Wal-Mart area severely damaged by tornado.</t>
-  </si>
-  <si>
-    <t>Nebraska</t>
-  </si>
-  <si>
-    <t>Missouri</t>
-  </si>
-  <si>
-    <t>Missouri Gov.</t>
-  </si>
-  <si>
-    <t>Two people were killed in southwest Missouri.</t>
-  </si>
-  <si>
-    <t>One man was killed outside Puxico, Missouri in the storms.</t>
-  </si>
-  <si>
-    <t>Waves of strong storms devastated small communities and damaged the country music resort town of Branson, Missouri.</t>
-  </si>
-  <si>
-    <t>Ky</t>
-  </si>
-  <si>
-    <t>Buffalo</t>
-  </si>
-  <si>
-    <t>Farther north, rescue crews waited for sunrise to begin searching a trailer park south of Buffalo where at least one person was killed after an apparent twister slammed the area.</t>
-  </si>
-  <si>
-    <t>National Weather Service</t>
-  </si>
-  <si>
-    <t>The National Weather Service is sending three teams to survey the damage.</t>
-  </si>
-  <si>
-    <t>Preliminary reports from the National Weather Service report large oak trees were found uprooted and damage to roofs was consistent with EF1 damage on the enhanced Fujita scale.</t>
-  </si>
-  <si>
-    <t>tornado, National Weather Service snow alerts and more Leap Year weather.</t>
-  </si>
-  <si>
-    <t>Some Leap Year babies woke up Wednesday to find their uncommon birthday plagued by school closings, National Weather Service snow alerts and even a tornado.</t>
-  </si>
-  <si>
-    <t>First Baptist Church</t>
-  </si>
-  <si>
-    <t>According to the sheriff's office, the shelter is open at the First Baptist Church at 204 North Main Street.</t>
-  </si>
-  <si>
-    <t>Stoddard County Coroner</t>
-  </si>
-  <si>
-    <t>Stoddard County Coroner Aaron Mathis has released the name of the man killed in Puxico Wednesday morning after a tornado moved through the area.</t>
-  </si>
-  <si>
-    <t>The Stoddard County Coroner confirms one person has died as a result of overnight storms.</t>
-  </si>
-  <si>
-    <t>Ill.</t>
-  </si>
-  <si>
-    <t>Oak Ridge</t>
-  </si>
-  <si>
-    <t>According to Emergency Management, all roads are back open in the Oak Ridge area.</t>
-  </si>
-  <si>
-    <t>One man in Oak Ridge says it pulled the roof off his trailer and shifted it about five feet from the foundation.</t>
-  </si>
-  <si>
-    <t>People are using the school in Oak Ridge as a staging area to head out to help those in the area.</t>
-  </si>
-  <si>
-    <t>The Oak Ridge has damage to the roof and air conditioning unit.</t>
-  </si>
-  <si>
     <t>Bell City</t>
   </si>
   <si>
     <t>It started early Wednesday morning just west of Asherville to two miles west of Bell City.</t>
-  </si>
-  <si>
-    <t>Heartland News</t>
-  </si>
-  <si>
-    <t>Heartland News reporter Carly O'Keefe reports grain bins in fields and more damage in Gallatin County.</t>
-  </si>
-  <si>
-    <t>Moreland told Heartland News Wednesday morning that there is extensive damage everywhere, and power lines down across several miles.</t>
-  </si>
-  <si>
-    <t>Emergency Manager Dale Moreland tells Heartland News it looks like the mobile home  "exploded."</t>
-  </si>
-  <si>
-    <t>Her sister, Judie LaChance tells Heartland News that Sandy Hemby will be okay.</t>
-  </si>
-  <si>
-    <t>The mayor of Harrisburg tells Heartland News that this is a horrific event.</t>
-  </si>
-  <si>
-    <t>Mo</t>
-  </si>
-  <si>
-    <t>Moreland says crews are working on County Road 249 and County Road 271 is blocked.</t>
-  </si>
-  <si>
-    <t>Emergency Manager Dale Moreland says there will be a shelter opening at 3 p.m. Wednesday at Kinder Chapel that is on K Highway.</t>
-  </si>
-  <si>
-    <t>Windows are blown out," Moore said.</t>
-  </si>
-  <si>
-    <t>Residents of Clay County in northeastern Arkansas reported hail the size of golf balls, while half dollar-sized hail was reported in Mountain Home.</t>
-  </si>
-  <si>
-    <t>More than 30 people were reported hurt, mostly with cuts and bruises.</t>
-  </si>
-  <si>
-    <t>John Moore, owner of the damaged Cakes-n-Creams '50s Diner, said the tornado seemed to target the city's main strip, moving down the entertainment district, right through the convention center, across a lake and into a housing division.</t>
-  </si>
-  <si>
-    <t>Jennifer Verhaalen, a long-term resident at the Hillbilly Inn Motel in downtown Branson, said she saw a white funnel cloud followed by a wall of rain as the storm closed in on the town around 1 a.m.  She said she retreated to a back bedroom with her husband as the storm slammed into two other hotel buildings tearing the roof off one.</t>
-  </si>
-  <si>
-    <t>Arkansas</t>
-  </si>
-  <si>
-    <t>The system also skirted northern Arkansas, bringing gusts of up to 60 mph in the northwest.</t>
-  </si>
-  <si>
-    <t>Puxico</t>
-  </si>
-  <si>
-    <t>The damage is along County Roads 266 and 257 east of Puxico and tracked to the northeast to the Leora area.</t>
-  </si>
-  <si>
-    <t>Johnnie Clark, the city manager in Puxico, says most of the damage is in the rural areas near town.</t>
-  </si>
-  <si>
-    <t>No major damage is reported in Puxico city limits.</t>
-  </si>
-  <si>
-    <t>Harrisburg</t>
-  </si>
-  <si>
-    <t>The superintendent of schools in Harrisburg has canceled classes the rest of week.</t>
-  </si>
-  <si>
-    <t>Siteseers are asked to stay away from the City of Harrisburg.</t>
-  </si>
-  <si>
-    <t>The sheriff's office says the Harrisburg Medical Center is not admitting patients, but the emergency room is open and operational if anyone needs emergency care.</t>
-  </si>
-  <si>
-    <t>Harrisburg Police Chief Bob Smith says Rural King and the SIC foundation building are set up as meeting areas for manpower and equipment.</t>
-  </si>
-  <si>
-    <t>At least 300 houses have been damaged or destroyed with at least 25 businesses damaged or destroyed in the Harrisburg area, according to the sheriff's office.</t>
-  </si>
-  <si>
-    <t>"This morning the city of Harrisburg suffered a horrific event," said Harrisburg mayor Eric Gregg.</t>
-  </si>
-  <si>
-    <t>All volunteers in Harrisburg must register at the SIC Foundation building on North Commercial St. starting at 7 a.m. on March 1.</t>
-  </si>
-  <si>
-    <t>Pat Quinn signed state disaster declaration at the podium at a 2 p.m. press conference in Harrisburg Wednesday.</t>
-  </si>
-  <si>
-    <t>Smith says 24/7 law enforcement protection will be available in Harrisburg for as long as needed.</t>
-  </si>
-  <si>
-    <t>Several roads are block off in Harrisburg.</t>
-  </si>
-  <si>
-    <t>It touched down around 4:51 a.m. one mile north of Carrier Mills and traveled ENE toward Harrisburg, touching down in Harrisburg at 4:56 a.m.  That path of the tornado is more than seven miles long and about 250 yards wide.</t>
-  </si>
-  <si>
-    <t>Vernon (the Old Integra Bank Building) will serve as a drop off site for items for the tornado victims in Harrisburg, IL.</t>
-  </si>
-  <si>
-    <t>Tyler Profilet reports a lot of damage in the Harrisburg area, including semi trucks tipped over.</t>
   </si>
 </sst>
 </file>
@@ -975,7 +903,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C253"/>
+  <dimension ref="A1:C240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1019,10 +947,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1030,10 +958,10 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1041,10 +969,10 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1052,10 +980,10 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1063,10 +991,10 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1074,10 +1002,10 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1085,10 +1013,10 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1096,10 +1024,10 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1107,10 +1035,10 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1118,10 +1046,10 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1129,10 +1057,10 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1140,10 +1068,10 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1151,10 +1079,10 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1162,10 +1090,10 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1173,10 +1101,10 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1184,10 +1112,10 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1195,10 +1123,10 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1206,10 +1134,10 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1217,10 +1145,10 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1228,10 +1156,10 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1239,10 +1167,10 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1250,10 +1178,10 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1261,10 +1189,10 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1272,10 +1200,10 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1283,10 +1211,10 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1294,10 +1222,10 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1305,10 +1233,10 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1316,10 +1244,10 @@
         <v>0</v>
       </c>
       <c r="B31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" t="s">
         <v>29</v>
-      </c>
-      <c r="C31" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1327,10 +1255,10 @@
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1338,10 +1266,10 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1349,10 +1277,10 @@
         <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1360,10 +1288,10 @@
         <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1371,10 +1299,10 @@
         <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1382,10 +1310,10 @@
         <v>0</v>
       </c>
       <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" t="s">
         <v>35</v>
-      </c>
-      <c r="C37" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1393,10 +1321,10 @@
         <v>0</v>
       </c>
       <c r="B38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" t="s">
         <v>35</v>
-      </c>
-      <c r="C38" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1404,10 +1332,10 @@
         <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C39" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1415,10 +1343,10 @@
         <v>0</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1426,10 +1354,10 @@
         <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C41" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1437,10 +1365,10 @@
         <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1448,10 +1376,10 @@
         <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1459,10 +1387,10 @@
         <v>0</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1470,10 +1398,10 @@
         <v>0</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1481,10 +1409,10 @@
         <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1492,10 +1420,10 @@
         <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C47" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1503,10 +1431,10 @@
         <v>0</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C48" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1514,10 +1442,10 @@
         <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C49" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1525,10 +1453,10 @@
         <v>0</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1536,10 +1464,10 @@
         <v>0</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C51" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1547,10 +1475,10 @@
         <v>0</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C52" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1558,10 +1486,10 @@
         <v>0</v>
       </c>
       <c r="B53" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C53" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1569,10 +1497,10 @@
         <v>0</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C54" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1580,10 +1508,10 @@
         <v>0</v>
       </c>
       <c r="B55" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C55" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1591,10 +1519,10 @@
         <v>0</v>
       </c>
       <c r="B56" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C56" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1602,10 +1530,10 @@
         <v>0</v>
       </c>
       <c r="B57" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C57" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1613,10 +1541,10 @@
         <v>0</v>
       </c>
       <c r="B58" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C58" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1624,10 +1552,10 @@
         <v>0</v>
       </c>
       <c r="B59" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="C59" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1635,10 +1563,10 @@
         <v>0</v>
       </c>
       <c r="B60" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="C60" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1646,10 +1574,10 @@
         <v>0</v>
       </c>
       <c r="B61" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C61" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1657,10 +1585,10 @@
         <v>0</v>
       </c>
       <c r="B62" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C62" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1668,10 +1596,10 @@
         <v>0</v>
       </c>
       <c r="B63" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C63" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1679,10 +1607,10 @@
         <v>0</v>
       </c>
       <c r="B64" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C64" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1690,10 +1618,10 @@
         <v>0</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C65" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1701,10 +1629,10 @@
         <v>0</v>
       </c>
       <c r="B66" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C66" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1712,10 +1640,10 @@
         <v>0</v>
       </c>
       <c r="B67" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C67" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1723,10 +1651,10 @@
         <v>0</v>
       </c>
       <c r="B68" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C68" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1734,10 +1662,10 @@
         <v>0</v>
       </c>
       <c r="B69" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C69" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1745,10 +1673,10 @@
         <v>0</v>
       </c>
       <c r="B70" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C70" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1756,10 +1684,10 @@
         <v>0</v>
       </c>
       <c r="B71" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="C71" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1767,10 +1695,10 @@
         <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="C72" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1778,10 +1706,10 @@
         <v>0</v>
       </c>
       <c r="B73" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="C73" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1789,10 +1717,10 @@
         <v>0</v>
       </c>
       <c r="B74" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="C74" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1800,10 +1728,10 @@
         <v>0</v>
       </c>
       <c r="B75" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="C75" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1811,10 +1739,10 @@
         <v>0</v>
       </c>
       <c r="B76" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C76" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1822,10 +1750,10 @@
         <v>0</v>
       </c>
       <c r="B77" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C77" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1833,10 +1761,10 @@
         <v>0</v>
       </c>
       <c r="B78" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C78" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1844,10 +1772,10 @@
         <v>0</v>
       </c>
       <c r="B79" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C79" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1855,10 +1783,10 @@
         <v>0</v>
       </c>
       <c r="B80" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C80" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1866,10 +1794,10 @@
         <v>0</v>
       </c>
       <c r="B81" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C81" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1877,10 +1805,10 @@
         <v>0</v>
       </c>
       <c r="B82" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C82" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1888,10 +1816,10 @@
         <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C83" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1899,10 +1827,10 @@
         <v>0</v>
       </c>
       <c r="B84" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C84" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1910,10 +1838,10 @@
         <v>0</v>
       </c>
       <c r="B85" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C85" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1921,10 +1849,10 @@
         <v>0</v>
       </c>
       <c r="B86" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="C86" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1932,10 +1860,10 @@
         <v>0</v>
       </c>
       <c r="B87" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="C87" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1943,10 +1871,10 @@
         <v>0</v>
       </c>
       <c r="B88" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="C88" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1954,10 +1882,10 @@
         <v>0</v>
       </c>
       <c r="B89" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C89" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1965,10 +1893,10 @@
         <v>0</v>
       </c>
       <c r="B90" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C90" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1976,10 +1904,10 @@
         <v>0</v>
       </c>
       <c r="B91" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C91" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1987,10 +1915,10 @@
         <v>0</v>
       </c>
       <c r="B92" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="C92" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1998,10 +1926,10 @@
         <v>0</v>
       </c>
       <c r="B93" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="C93" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2009,10 +1937,10 @@
         <v>0</v>
       </c>
       <c r="B94" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C94" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2020,10 +1948,10 @@
         <v>0</v>
       </c>
       <c r="B95" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C95" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2031,10 +1959,10 @@
         <v>0</v>
       </c>
       <c r="B96" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C96" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2042,10 +1970,10 @@
         <v>0</v>
       </c>
       <c r="B97" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C97" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2053,10 +1981,10 @@
         <v>0</v>
       </c>
       <c r="B98" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="C98" t="s">
-        <v>104</v>
+        <v>18</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2064,10 +1992,10 @@
         <v>0</v>
       </c>
       <c r="B99" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="C99" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2075,10 +2003,10 @@
         <v>0</v>
       </c>
       <c r="B100" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="C100" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2086,10 +2014,10 @@
         <v>0</v>
       </c>
       <c r="B101" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="C101" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2097,10 +2025,10 @@
         <v>0</v>
       </c>
       <c r="B102" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="C102" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2108,10 +2036,10 @@
         <v>0</v>
       </c>
       <c r="B103" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="C103" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2119,10 +2047,10 @@
         <v>0</v>
       </c>
       <c r="B104" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="C104" t="s">
-        <v>109</v>
+        <v>30</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2130,10 +2058,10 @@
         <v>0</v>
       </c>
       <c r="B105" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C105" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2141,10 +2069,10 @@
         <v>0</v>
       </c>
       <c r="B106" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C106" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2152,10 +2080,10 @@
         <v>0</v>
       </c>
       <c r="B107" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C107" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2163,10 +2091,10 @@
         <v>0</v>
       </c>
       <c r="B108" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C108" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2174,10 +2102,10 @@
         <v>0</v>
       </c>
       <c r="B109" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C109" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2185,10 +2113,10 @@
         <v>0</v>
       </c>
       <c r="B110" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C110" t="s">
-        <v>114</v>
+        <v>16</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2196,10 +2124,10 @@
         <v>0</v>
       </c>
       <c r="B111" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C111" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2207,10 +2135,10 @@
         <v>0</v>
       </c>
       <c r="B112" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="C112" t="s">
-        <v>61</v>
+        <v>100</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2218,10 +2146,10 @@
         <v>0</v>
       </c>
       <c r="B113" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="C113" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2229,10 +2157,10 @@
         <v>0</v>
       </c>
       <c r="B114" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C114" t="s">
-        <v>117</v>
+        <v>20</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2240,10 +2168,10 @@
         <v>0</v>
       </c>
       <c r="B115" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C115" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2251,10 +2179,10 @@
         <v>0</v>
       </c>
       <c r="B116" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C116" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2262,10 +2190,10 @@
         <v>0</v>
       </c>
       <c r="B117" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C117" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2273,10 +2201,10 @@
         <v>0</v>
       </c>
       <c r="B118" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C118" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2284,10 +2212,10 @@
         <v>0</v>
       </c>
       <c r="B119" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="C119" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2295,10 +2223,10 @@
         <v>0</v>
       </c>
       <c r="B120" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="C120" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2306,10 +2234,10 @@
         <v>0</v>
       </c>
       <c r="B121" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="C121" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2317,10 +2245,10 @@
         <v>0</v>
       </c>
       <c r="B122" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C122" t="s">
-        <v>123</v>
+        <v>67</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2328,10 +2256,10 @@
         <v>0</v>
       </c>
       <c r="B123" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C123" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2339,10 +2267,10 @@
         <v>0</v>
       </c>
       <c r="B124" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C124" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2350,10 +2278,10 @@
         <v>0</v>
       </c>
       <c r="B125" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C125" t="s">
-        <v>126</v>
+        <v>11</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2361,10 +2289,10 @@
         <v>0</v>
       </c>
       <c r="B126" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C126" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2372,10 +2300,10 @@
         <v>0</v>
       </c>
       <c r="B127" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C127" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2383,10 +2311,10 @@
         <v>0</v>
       </c>
       <c r="B128" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C128" t="s">
-        <v>129</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2394,10 +2322,10 @@
         <v>0</v>
       </c>
       <c r="B129" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C129" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2405,10 +2333,10 @@
         <v>0</v>
       </c>
       <c r="B130" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="C130" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2416,10 +2344,10 @@
         <v>0</v>
       </c>
       <c r="B131" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="C131" t="s">
-        <v>131</v>
+        <v>50</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2427,10 +2355,10 @@
         <v>0</v>
       </c>
       <c r="B132" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="C132" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2438,10 +2366,10 @@
         <v>0</v>
       </c>
       <c r="B133" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="C133" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2449,10 +2377,10 @@
         <v>0</v>
       </c>
       <c r="B134" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="C134" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2460,10 +2388,10 @@
         <v>0</v>
       </c>
       <c r="B135" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="C135" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2471,10 +2399,10 @@
         <v>0</v>
       </c>
       <c r="B136" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="C136" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2482,10 +2410,10 @@
         <v>0</v>
       </c>
       <c r="B137" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="C137" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2493,10 +2421,10 @@
         <v>0</v>
       </c>
       <c r="B138" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="C138" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2504,10 +2432,10 @@
         <v>0</v>
       </c>
       <c r="B139" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="C139" t="s">
-        <v>54</v>
+        <v>123</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2515,10 +2443,10 @@
         <v>0</v>
       </c>
       <c r="B140" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="C140" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2526,10 +2454,10 @@
         <v>0</v>
       </c>
       <c r="B141" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="C141" t="s">
-        <v>15</v>
+        <v>125</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2537,10 +2465,10 @@
         <v>0</v>
       </c>
       <c r="B142" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="C142" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2548,10 +2476,10 @@
         <v>0</v>
       </c>
       <c r="B143" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="C143" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2559,10 +2487,10 @@
         <v>0</v>
       </c>
       <c r="B144" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C144" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2570,10 +2498,10 @@
         <v>0</v>
       </c>
       <c r="B145" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C145" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2581,10 +2509,10 @@
         <v>0</v>
       </c>
       <c r="B146" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="C146" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2592,10 +2520,10 @@
         <v>0</v>
       </c>
       <c r="B147" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="C147" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2603,10 +2531,10 @@
         <v>0</v>
       </c>
       <c r="B148" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="C148" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2614,10 +2542,10 @@
         <v>0</v>
       </c>
       <c r="B149" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="C149" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2625,10 +2553,10 @@
         <v>0</v>
       </c>
       <c r="B150" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="C150" t="s">
-        <v>148</v>
+        <v>100</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2636,10 +2564,10 @@
         <v>0</v>
       </c>
       <c r="B151" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="C151" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2647,10 +2575,10 @@
         <v>0</v>
       </c>
       <c r="B152" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="C152" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2658,10 +2586,10 @@
         <v>0</v>
       </c>
       <c r="B153" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="C153" t="s">
-        <v>55</v>
+        <v>131</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2669,10 +2597,10 @@
         <v>0</v>
       </c>
       <c r="B154" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C154" t="s">
-        <v>151</v>
+        <v>55</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2680,10 +2608,10 @@
         <v>0</v>
       </c>
       <c r="B155" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C155" t="s">
-        <v>152</v>
+        <v>55</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2691,10 +2619,10 @@
         <v>0</v>
       </c>
       <c r="B156" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C156" t="s">
-        <v>153</v>
+        <v>75</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2702,10 +2630,10 @@
         <v>0</v>
       </c>
       <c r="B157" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C157" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2713,10 +2641,10 @@
         <v>0</v>
       </c>
       <c r="B158" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C158" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2724,10 +2652,10 @@
         <v>0</v>
       </c>
       <c r="B159" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C159" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2735,10 +2663,10 @@
         <v>0</v>
       </c>
       <c r="B160" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C160" t="s">
-        <v>13</v>
+        <v>137</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2746,10 +2674,10 @@
         <v>0</v>
       </c>
       <c r="B161" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C161" t="s">
-        <v>7</v>
+        <v>138</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2757,10 +2685,10 @@
         <v>0</v>
       </c>
       <c r="B162" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C162" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2768,10 +2696,10 @@
         <v>0</v>
       </c>
       <c r="B163" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C163" t="s">
-        <v>55</v>
+        <v>140</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2779,10 +2707,10 @@
         <v>0</v>
       </c>
       <c r="B164" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="C164" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2790,10 +2718,10 @@
         <v>0</v>
       </c>
       <c r="B165" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="C165" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -2801,10 +2729,10 @@
         <v>0</v>
       </c>
       <c r="B166" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="C166" t="s">
-        <v>58</v>
+        <v>143</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2812,10 +2740,10 @@
         <v>0</v>
       </c>
       <c r="B167" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C167" t="s">
-        <v>157</v>
+        <v>103</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2823,10 +2751,10 @@
         <v>0</v>
       </c>
       <c r="B168" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C168" t="s">
-        <v>84</v>
+        <v>145</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -2834,10 +2762,10 @@
         <v>0</v>
       </c>
       <c r="B169" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="C169" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -2845,10 +2773,10 @@
         <v>0</v>
       </c>
       <c r="B170" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C170" t="s">
-        <v>140</v>
+        <v>17</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -2856,10 +2784,10 @@
         <v>0</v>
       </c>
       <c r="B171" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C171" t="s">
-        <v>117</v>
+        <v>18</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -2867,10 +2795,10 @@
         <v>0</v>
       </c>
       <c r="B172" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C172" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -2878,10 +2806,10 @@
         <v>0</v>
       </c>
       <c r="B173" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C173" t="s">
-        <v>32</v>
+        <v>123</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -2889,10 +2817,10 @@
         <v>0</v>
       </c>
       <c r="B174" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C174" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -2900,10 +2828,10 @@
         <v>0</v>
       </c>
       <c r="B175" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C175" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -2911,10 +2839,10 @@
         <v>0</v>
       </c>
       <c r="B176" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C176" t="s">
-        <v>137</v>
+        <v>26</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -2922,10 +2850,10 @@
         <v>0</v>
       </c>
       <c r="B177" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C177" t="s">
-        <v>85</v>
+        <v>149</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -2933,10 +2861,10 @@
         <v>0</v>
       </c>
       <c r="B178" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C178" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -2944,10 +2872,10 @@
         <v>0</v>
       </c>
       <c r="B179" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C179" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -2955,10 +2883,10 @@
         <v>0</v>
       </c>
       <c r="B180" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C180" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -2966,10 +2894,10 @@
         <v>0</v>
       </c>
       <c r="B181" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C181" t="s">
-        <v>161</v>
+        <v>7</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -2977,10 +2905,10 @@
         <v>0</v>
       </c>
       <c r="B182" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C182" t="s">
-        <v>162</v>
+        <v>8</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -2988,10 +2916,10 @@
         <v>0</v>
       </c>
       <c r="B183" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="C183" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -2999,10 +2927,10 @@
         <v>0</v>
       </c>
       <c r="B184" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="C184" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3010,10 +2938,10 @@
         <v>0</v>
       </c>
       <c r="B185" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C185" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3021,10 +2949,10 @@
         <v>0</v>
       </c>
       <c r="B186" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C186" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3032,10 +2960,10 @@
         <v>0</v>
       </c>
       <c r="B187" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="C187" t="s">
-        <v>72</v>
+        <v>152</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3043,10 +2971,10 @@
         <v>0</v>
       </c>
       <c r="B188" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="C188" t="s">
-        <v>120</v>
+        <v>153</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3054,10 +2982,10 @@
         <v>0</v>
       </c>
       <c r="B189" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="C189" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -3065,10 +2993,10 @@
         <v>0</v>
       </c>
       <c r="B190" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="C190" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3076,10 +3004,10 @@
         <v>0</v>
       </c>
       <c r="B191" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="C191" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3087,10 +3015,10 @@
         <v>0</v>
       </c>
       <c r="B192" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="C192" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -3098,10 +3026,10 @@
         <v>0</v>
       </c>
       <c r="B193" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="C193" t="s">
-        <v>119</v>
+        <v>157</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3109,10 +3037,10 @@
         <v>0</v>
       </c>
       <c r="B194" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="C194" t="s">
-        <v>2</v>
+        <v>158</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -3120,10 +3048,10 @@
         <v>0</v>
       </c>
       <c r="B195" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="C195" t="s">
-        <v>173</v>
+        <v>67</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -3131,10 +3059,10 @@
         <v>0</v>
       </c>
       <c r="B196" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="C196" t="s">
-        <v>175</v>
+        <v>67</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -3142,10 +3070,10 @@
         <v>0</v>
       </c>
       <c r="B197" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="C197" t="s">
-        <v>45</v>
+        <v>159</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -3153,10 +3081,10 @@
         <v>0</v>
       </c>
       <c r="B198" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="C198" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -3164,10 +3092,10 @@
         <v>0</v>
       </c>
       <c r="B199" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="C199" t="s">
-        <v>178</v>
+        <v>72</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -3175,10 +3103,10 @@
         <v>0</v>
       </c>
       <c r="B200" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="C200" t="s">
-        <v>179</v>
+        <v>72</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -3186,10 +3114,10 @@
         <v>0</v>
       </c>
       <c r="B201" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="C201" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -3197,10 +3125,10 @@
         <v>0</v>
       </c>
       <c r="B202" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="C202" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -3208,10 +3136,10 @@
         <v>0</v>
       </c>
       <c r="B203" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="C203" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -3219,10 +3147,10 @@
         <v>0</v>
       </c>
       <c r="B204" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="C204" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -3230,10 +3158,10 @@
         <v>0</v>
       </c>
       <c r="B205" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="C205" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -3241,10 +3169,10 @@
         <v>0</v>
       </c>
       <c r="B206" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="C206" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -3252,10 +3180,10 @@
         <v>0</v>
       </c>
       <c r="B207" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="C207" t="s">
-        <v>133</v>
+        <v>166</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -3263,10 +3191,10 @@
         <v>0</v>
       </c>
       <c r="B208" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="C208" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -3274,10 +3202,10 @@
         <v>0</v>
       </c>
       <c r="B209" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="C209" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -3285,10 +3213,10 @@
         <v>0</v>
       </c>
       <c r="B210" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="C210" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -3296,10 +3224,10 @@
         <v>0</v>
       </c>
       <c r="B211" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="C211" t="s">
-        <v>178</v>
+        <v>41</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -3307,10 +3235,10 @@
         <v>0</v>
       </c>
       <c r="B212" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C212" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -3318,10 +3246,10 @@
         <v>0</v>
       </c>
       <c r="B213" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C213" t="s">
-        <v>107</v>
+        <v>171</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -3329,10 +3257,10 @@
         <v>0</v>
       </c>
       <c r="B214" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C214" t="s">
-        <v>14</v>
+        <v>171</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -3340,10 +3268,10 @@
         <v>0</v>
       </c>
       <c r="B215" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C215" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -3351,10 +3279,10 @@
         <v>0</v>
       </c>
       <c r="B216" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C216" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -3362,10 +3290,10 @@
         <v>0</v>
       </c>
       <c r="B217" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="C217" t="s">
-        <v>186</v>
+        <v>11</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -3373,10 +3301,10 @@
         <v>0</v>
       </c>
       <c r="B218" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="C218" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -3384,10 +3312,10 @@
         <v>0</v>
       </c>
       <c r="B219" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="C219" t="s">
-        <v>7</v>
+        <v>176</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -3395,10 +3323,10 @@
         <v>0</v>
       </c>
       <c r="B220" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="C220" t="s">
-        <v>166</v>
+        <v>4</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -3406,10 +3334,10 @@
         <v>0</v>
       </c>
       <c r="B221" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="C221" t="s">
-        <v>116</v>
+        <v>23</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -3417,10 +3345,10 @@
         <v>0</v>
       </c>
       <c r="B222" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="C222" t="s">
-        <v>131</v>
+        <v>62</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -3428,10 +3356,10 @@
         <v>0</v>
       </c>
       <c r="B223" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="C223" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -3439,10 +3367,10 @@
         <v>0</v>
       </c>
       <c r="B224" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="C224" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -3450,10 +3378,10 @@
         <v>0</v>
       </c>
       <c r="B225" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="C225" t="s">
-        <v>193</v>
+        <v>96</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -3461,10 +3389,10 @@
         <v>0</v>
       </c>
       <c r="B226" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="C226" t="s">
-        <v>194</v>
+        <v>4</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -3472,10 +3400,10 @@
         <v>0</v>
       </c>
       <c r="B227" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="C227" t="s">
-        <v>195</v>
+        <v>21</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -3483,10 +3411,10 @@
         <v>0</v>
       </c>
       <c r="B228" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="C228" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -3494,10 +3422,10 @@
         <v>0</v>
       </c>
       <c r="B229" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="C229" t="s">
-        <v>197</v>
+        <v>26</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -3505,10 +3433,10 @@
         <v>0</v>
       </c>
       <c r="B230" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="C230" t="s">
-        <v>198</v>
+        <v>100</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -3516,10 +3444,10 @@
         <v>0</v>
       </c>
       <c r="B231" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="C231" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -3527,10 +3455,10 @@
         <v>0</v>
       </c>
       <c r="B232" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="C232" t="s">
-        <v>21</v>
+        <v>180</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -3538,10 +3466,10 @@
         <v>0</v>
       </c>
       <c r="B233" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="C233" t="s">
-        <v>199</v>
+        <v>172</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -3549,10 +3477,10 @@
         <v>0</v>
       </c>
       <c r="B234" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="C234" t="s">
-        <v>200</v>
+        <v>131</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -3560,10 +3488,10 @@
         <v>0</v>
       </c>
       <c r="B235" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="C235" t="s">
-        <v>94</v>
+        <v>181</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -3571,10 +3499,10 @@
         <v>0</v>
       </c>
       <c r="B236" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="C236" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -3582,10 +3510,10 @@
         <v>0</v>
       </c>
       <c r="B237" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="C237" t="s">
-        <v>9</v>
+        <v>117</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -3593,10 +3521,10 @@
         <v>0</v>
       </c>
       <c r="B238" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="C238" t="s">
-        <v>181</v>
+        <v>11</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -3604,10 +3532,10 @@
         <v>0</v>
       </c>
       <c r="B239" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="C239" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -3615,153 +3543,10 @@
         <v>0</v>
       </c>
       <c r="B240" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="C240" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3">
-      <c r="A241" t="s">
-        <v>0</v>
-      </c>
-      <c r="B241" t="s">
-        <v>196</v>
-      </c>
-      <c r="C241" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3">
-      <c r="A242" t="s">
-        <v>0</v>
-      </c>
-      <c r="B242" t="s">
-        <v>196</v>
-      </c>
-      <c r="C242" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3">
-      <c r="A243" t="s">
-        <v>0</v>
-      </c>
-      <c r="B243" t="s">
-        <v>196</v>
-      </c>
-      <c r="C243" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3">
-      <c r="A244" t="s">
-        <v>0</v>
-      </c>
-      <c r="B244" t="s">
-        <v>196</v>
-      </c>
-      <c r="C244" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3">
-      <c r="A245" t="s">
-        <v>0</v>
-      </c>
-      <c r="B245" t="s">
-        <v>196</v>
-      </c>
-      <c r="C245" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3">
-      <c r="A246" t="s">
-        <v>0</v>
-      </c>
-      <c r="B246" t="s">
-        <v>196</v>
-      </c>
-      <c r="C246" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3">
-      <c r="A247" t="s">
-        <v>0</v>
-      </c>
-      <c r="B247" t="s">
-        <v>196</v>
-      </c>
-      <c r="C247" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3">
-      <c r="A248" t="s">
-        <v>0</v>
-      </c>
-      <c r="B248" t="s">
-        <v>196</v>
-      </c>
-      <c r="C248" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3">
-      <c r="A249" t="s">
-        <v>0</v>
-      </c>
-      <c r="B249" t="s">
-        <v>196</v>
-      </c>
-      <c r="C249" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3">
-      <c r="A250" t="s">
-        <v>0</v>
-      </c>
-      <c r="B250" t="s">
-        <v>196</v>
-      </c>
-      <c r="C250" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3">
-      <c r="A251" t="s">
-        <v>0</v>
-      </c>
-      <c r="B251" t="s">
-        <v>196</v>
-      </c>
-      <c r="C251" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3">
-      <c r="A252" t="s">
-        <v>0</v>
-      </c>
-      <c r="B252" t="s">
-        <v>196</v>
-      </c>
-      <c r="C252" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3">
-      <c r="A253" t="s">
-        <v>0</v>
-      </c>
-      <c r="B253" t="s">
-        <v>196</v>
-      </c>
-      <c r="C253" t="s">
-        <v>209</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actually change to non-duplicate judge files
</commit_message>
<xml_diff>
--- a/sentence_level/data/sentences/remove_single/2012_leap_day_tornado.xlsx
+++ b/sentence_level/data/sentences/remove_single/2012_leap_day_tornado.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="181">
   <si>
     <t>2012_leap_day_tornado</t>
   </si>
@@ -22,390 +22,381 @@
     <t>Illinois</t>
   </si>
   <si>
+    <t>But none faced the wrath of Mother Nature like the southern Illinois town of Harrisburg.</t>
+  </si>
+  <si>
     <t>At least 13 dead in storms working across Missouri, Illinois.</t>
   </si>
   <si>
+    <t>Ameren Illinois representatives say more than 430 personnel were deployed to southern Illinois.</t>
+  </si>
+  <si>
+    <t>From Tuesday night into Wednesday morning, at least 16 tornado sightings were reported from Nebraska and Kansas across southern Missouri to Illinois and Kentucky, according to the storm center, an arm of the National Weather Service.</t>
+  </si>
+  <si>
+    <t>Quinn says he's already talked to President Obama and that Illinois is banding together as a family to help Harrisburg recover and rebuild.</t>
+  </si>
+  <si>
+    <t>It is the deadliest state disaster in Illinois in nearly a decade.</t>
+  </si>
+  <si>
+    <t>Many people are asking how they can help after a preliminary EF4 tornado hit Saline County, Illinois killing six people.</t>
+  </si>
+  <si>
+    <t>David Serby in Perry County, Illinois says a few outbuildings were blown over with some tree damage.</t>
+  </si>
+  <si>
     <t>At least 10 people were killed in the southern Illinois town of Harrisburg after a storm leveled much of the community of 9,000 people.</t>
   </si>
   <si>
-    <t>From Tuesday night into Wednesday morning, at least 16 tornado sightings were reported from Nebraska and Kansas across southern Missouri to Illinois and Kentucky, according to the storm center, an arm of the National Weather Service.</t>
-  </si>
-  <si>
-    <t>Many people are asking how they can help after a preliminary EF4 tornado hit Saline County, Illinois killing six people.</t>
-  </si>
-  <si>
-    <t>It is the deadliest state disaster in Illinois in nearly a decade.</t>
-  </si>
-  <si>
     <t>Illinois Gov. Pat Quinn signed state disaster declaration at the podium at a 2 p.m. press conference in Harrisburg Wednesday.</t>
   </si>
   <si>
-    <t>Quinn says he's already talked to President Obama and that Illinois is banding together as a family to help Harrisburg recover and rebuild.</t>
-  </si>
-  <si>
-    <t>Ameren Illinois representatives say more than 430 personnel were deployed to southern Illinois.</t>
-  </si>
-  <si>
-    <t>David Serby in Perry County, Illinois says a few outbuildings were blown over with some tree damage.</t>
-  </si>
-  <si>
     <t>Leap Day was not a good one for thousands of people in the Midwest and Southern United States as severe storms and tornadoes left a trail of destruction in Illinois, Missouri, Kansas, Arkansas, Oklahoma, Kentucky, and Tennessee.</t>
   </si>
   <si>
-    <t>But none faced the wrath of Mother Nature like the southern Illinois town of Harrisburg.</t>
-  </si>
-  <si>
-    <t>Metropolis</t>
+    <t>Ill.</t>
+  </si>
+  <si>
+    <t>Reports are the tornado touched down just southwest of Mounds, Ill. and crossed over I-57 near exit 8.</t>
+  </si>
+  <si>
+    <t>Storm shelters have been opened up for those in need in southern Ill. and southeast Mo.</t>
+  </si>
+  <si>
+    <t>NWS reports are a tornado touched down just southwest of Mounds, Ill. and crossed over I-57 near exit 8.</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>In Missouri, one person was killed in a trailer park in the town of Buffalo, and at least three people were critically injured in the small eastern Kansas town of Harveyville.</t>
+  </si>
+  <si>
+    <t>"On behalf of the U.S. Department of Homeland Security's Federal Emergency Management Agency (FEMA), I would like to express our deepest condolences to the families of those who were killed and injured by tornadoes that impacted Kansas, Missouri and Nebraska late last night and into this morning.</t>
+  </si>
+  <si>
+    <t>In neighboring Kansas, the National Weather Service reported brief tornado touchdowns southwest of Hutchinson, and Gov. Sam Brownback declared a state of emergency after an apparent tornado struck Harveyville.</t>
+  </si>
+  <si>
+    <t>One person was killed in Kansas.</t>
+  </si>
+  <si>
+    <t>Saline County</t>
+  </si>
+  <si>
+    <t>Crews with Ameren Illinois have issued a safety warning to all residents in and around Saline County.</t>
+  </si>
+  <si>
+    <t>The National Weather Service reports an EF4 tornado hit Saline County on the southwest side of Harrisburg, killing six people.</t>
+  </si>
+  <si>
+    <t>Four females and two males, all adults, were killed in Saline County.</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>The National Weather Service issued overnight advisories of snow and rain in all three states, warning of an ice coating followed by freezing rain in Michigan, a “bit of snow” followed by “lots of rain” in Connecticut, and up to 10 inches of snow in Eastern Massachusetts.</t>
+  </si>
+  <si>
+    <t>Michigan, Connecticut and Massachusetts on Wednesday were spared from tornados but visited by snowy weather — a shock after this winter’s consistently warm temperatures.</t>
+  </si>
+  <si>
+    <t>SEOC</t>
+  </si>
+  <si>
+    <t>The governor says the SEOC will remain activated as long as necessary.</t>
+  </si>
+  <si>
+    <t>IEMA regional personnel were deployed to Harrisburg soon after the storms and representatives from the Illinois State Police, departments of Transportation, Central Management Services, Corrections, Public Health and Natural Resources, along with the American Red Cross, reported to the SEOC soon thereafter.</t>
+  </si>
+  <si>
+    <t>Ameren Illinois</t>
+  </si>
+  <si>
+    <t>More than 400 people are working to restore power to Ameren Illinois customers.</t>
+  </si>
+  <si>
+    <t>People should not call 911 or the dispatch center to report power line outages, please contact Ameren Illinois direct.</t>
+  </si>
+  <si>
+    <t>As of 4:10 a.m. Thursday, Ameren Illinois reports outages in:  Copyright 2012 KFVS.</t>
+  </si>
+  <si>
+    <t>Ameren Illinois doesn't have a time of when power will be restored.</t>
+  </si>
+  <si>
+    <t>Saint Francis Medical Center</t>
+  </si>
+  <si>
+    <t>A total of eight patients from Stoddard County are being treated at Saint Francis Medical Center.</t>
+  </si>
+  <si>
+    <t>Mark Champlin, 50, of Puxico was pronounced dead at 7:35 a.m. at Saint Francis Medical Center in Cape Girardeau.</t>
+  </si>
+  <si>
+    <t>Heartland</t>
+  </si>
+  <si>
+    <t>[More damage across the Heartland.]</t>
+  </si>
+  <si>
+    <t>Disaster in the Heartland - one year later  Disaster in the Heartland - one year later  The storm drove this plywood piece through the wall of a garage in Harrisburg,  Seven people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
+  </si>
+  <si>
+    <t>See pictures from across the Heartland after severe storms on Feb. 29, 2012.</t>
+  </si>
+  <si>
+    <t>How you can help after the tornadoes  How you can help after the tornadoes  Eight people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
+  </si>
+  <si>
+    <t>See the National Weather Service storm damage reports from the tornadoes and severe storms that swept through the Heartland early Feb. 29.</t>
+  </si>
+  <si>
+    <t>Seven of those tornadoes were in the Heartland.</t>
+  </si>
+  <si>
+    <t>Severe storms and tornadoes tear through the Heartland.</t>
+  </si>
+  <si>
+    <t>See more pictures from across the Heartland after severe storms on Feb. 29, 2012.</t>
+  </si>
+  <si>
+    <t>Five of those tornadoes were in the Heartland.</t>
+  </si>
+  <si>
+    <t>5 confirmed tornadoes in the Heartland.</t>
+  </si>
+  <si>
+    <t>Eight people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Two people were killed in southwest Missouri.</t>
+  </si>
+  <si>
+    <t>Missouri Gov. Jan Nixon has declared a state of emergency.</t>
+  </si>
+  <si>
+    <t>One man was killed outside Puxico, Missouri in the storms.</t>
+  </si>
+  <si>
+    <t>Waves of strong storms devastated small communities and damaged the country music resort town of Branson, Missouri.</t>
+  </si>
+  <si>
+    <t>Mo.</t>
+  </si>
+  <si>
+    <t>The school and a church sustained damage in Oak Ridge, Mo. in Cape Girardeau County.</t>
+  </si>
+  <si>
+    <t>Branson, Mo. tornado, National Weather Service snow alerts and more Leap Year weather.</t>
+  </si>
+  <si>
+    <t>A Puxico, Mo. man was killed in Stoddard County.</t>
+  </si>
+  <si>
+    <t>First Baptist Church</t>
+  </si>
+  <si>
+    <t>Donations may be made to the Red Cross at the First Baptist Church, The Salvation Army at 10 West Locust in Harrisburg or Christian Compassion Care Center at PO Box 422 in Harrisburg.</t>
+  </si>
+  <si>
+    <t>According to the sheriff's office, the shelter is open at the First Baptist Church at 204 North Main Street.</t>
+  </si>
+  <si>
+    <t>Pulaski County</t>
+  </si>
+  <si>
+    <t>Pulaski County, Illinois EMS Director Ken Kerley says wreckers and vehicles were blown from their location and crossing arms broke off and blew into a squad car.</t>
+  </si>
+  <si>
+    <t>No injuries have been reported in Pulaski County.</t>
+  </si>
+  <si>
+    <t>Cape Girardeau County</t>
+  </si>
+  <si>
+    <t>Team 1 (Rick Shanklin, Ken Ludington) - Harrisburg west toward Cape Girardeau County MO  Team 2 (Kelly Hooper, Shane Luecke) - Newburg IN West toward Harrisburg IL)  Team 3 (Christine Wielgos, Debbie Hooper) - Metropolis IL west toward Stoddard co.</t>
+  </si>
+  <si>
+    <t>Stoddard County</t>
+  </si>
+  <si>
+    <t>One man has died after the storms in Stoddard County.</t>
+  </si>
+  <si>
+    <t>Stoddard County Coroner Aaron Mathis has released the name of the man killed in Puxico Wednesday morning after a tornado moved through the area.</t>
+  </si>
+  <si>
+    <t>Stoddard County Sheriff Carl Hefner says several mobile homes in the area are destroyed in Stoddard County.</t>
+  </si>
+  <si>
+    <t>The Stoddard County coroner says Mark Champlin, 50, of Puxico was killed.</t>
+  </si>
+  <si>
+    <t>Highway Patrol Trooper Clark Parrott says large trees are down along Route M in Stoddard County.</t>
+  </si>
+  <si>
+    <t>You can drive for miles in Stoddard County and never see damage, but a path left from the strong winds that did blow through, show the wreckage.</t>
+  </si>
+  <si>
+    <t>They are all storm related injuries from Stoddard County.</t>
+  </si>
+  <si>
+    <t>A second tornado in Stoddard County Wednesday morning started just east of Bell City to three miles southeast of Benton, Mo.</t>
+  </si>
+  <si>
+    <t>NWS</t>
+  </si>
+  <si>
+    <t>NWS teams were in Stoddard and Cape Girardeau counties on Thursday surveying damage.</t>
+  </si>
+  <si>
+    <t>According to NWS, numerous trees near the house were also uprooted.</t>
+  </si>
+  <si>
+    <t>An EF3 tornado was confirmed by the NWS.</t>
+  </si>
+  <si>
+    <t>The NWS confirms preliminary reports of an EF2 tornado that went through McCracken and Ballard counties in Ky.</t>
+  </si>
+  <si>
+    <t>Oak Ridge</t>
+  </si>
+  <si>
+    <t>The Red Cross is providing food and water to residents and emergency workers in Oak Ridge as they work on cleaning up from the storm damage.</t>
+  </si>
+  <si>
+    <t>According to Emergency Management, all roads are back open in the Oak Ridge area.</t>
+  </si>
+  <si>
+    <t>People are using the school in Oak Ridge as a staging area to head out to help those in the area.</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>America</t>
+  </si>
+  <si>
+    <t>The tornado then crossed the Ohio River near the town of America, then across McCracken and Ballard Counties.</t>
+  </si>
+  <si>
+    <t>The tornado then crossed the Ohio River near the town of America, then across McCracken and Ballard counties.</t>
+  </si>
+  <si>
+    <t>U.S.</t>
+  </si>
+  <si>
+    <t>Corey Mead, lead forecaster at the U.S. Storm Prediction Center in Norman, Okla., said a broad cold front was slamming into warm, humid air over much of the eastern half of the nation.</t>
+  </si>
+  <si>
+    <t>The National Weather Service’s U.S. map Wednesday was covered by colorful wintry and storm warnings:</t>
+  </si>
+  <si>
+    <t>Mo</t>
+  </si>
+  <si>
+    <t>Associated Press photographer Mark Schiefelbein contributed to this report from Branson, Mo.</t>
+  </si>
+  <si>
+    <t>The National Weather Service confirms preliminary reports of an EF2 in Marquand in Madison County, Mo.</t>
+  </si>
+  <si>
+    <t>Buffalo</t>
+  </si>
+  <si>
+    <t>Buffalo is about 35 miles north of Springfield.</t>
+  </si>
+  <si>
+    <t>Farther north, rescue crews waited for sunrise to begin searching a trailer park south of Buffalo where at least one person was killed after an apparent twister slammed the area.</t>
+  </si>
+  <si>
+    <t>Heartland News</t>
+  </si>
+  <si>
+    <t>Heartland News reporter Carly O'Keefe reports grain bins in fields and more damage in Gallatin County.</t>
+  </si>
+  <si>
+    <t>Emergency Manager Dale Moreland tells Heartland News it looks like the mobile home  "exploded."</t>
+  </si>
+  <si>
+    <t>Moreland told Heartland News Wednesday morning that there is extensive damage everywhere, and power lines down across several miles.</t>
+  </si>
+  <si>
+    <t>Her sister, Judie LaChance tells Heartland News that Sandy Hemby will be okay.</t>
+  </si>
+  <si>
+    <t>The mayor of Harrisburg tells Heartland News that this is a horrific event.</t>
+  </si>
+  <si>
+    <t>Red Cross</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>In northern Oklahoma, gusts of up to 80 mph flipped trailers and damaged homes near Cherokee.</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>Residents of Clay County in northeastern Arkansas reported hail the size of golf balls, while half dollar-sized hail was reported in Mountain Home.</t>
+  </si>
+  <si>
+    <t>The system also skirted northern Arkansas, bringing gusts of up to 60 mph in the northwest.</t>
+  </si>
+  <si>
+    <t>Midwest</t>
+  </si>
+  <si>
+    <t>Three people were killed in Tennessee after the same severe weather system that created massive damage across the Midwest moved through the state.</t>
+  </si>
+  <si>
+    <t>Associated Press</t>
+  </si>
+  <si>
+    <t>The Associated Press contributed to report.</t>
+  </si>
+  <si>
+    <t>JIM SALTER,Associated Press.</t>
+  </si>
+  <si>
+    <t>According to the Associated Press Darrell Osman says his mother, 75-year-old Mary Osman, was among the dead.</t>
+  </si>
+  <si>
+    <t>Ameren</t>
+  </si>
+  <si>
+    <t>Ameren reports 14,000 without power at the peak.</t>
+  </si>
+  <si>
+    <t>Ameren hopes to have all power restored by the end of the day Friday.</t>
+  </si>
+  <si>
+    <t>Ameren has open a customer service center in Harrisburg.</t>
+  </si>
+  <si>
+    <t>Fire Department</t>
+  </si>
+  <si>
+    <t>Generators will be brought to the Oasis Tavern, just south of the Fire Department.</t>
+  </si>
+  <si>
+    <t>Food and drink is available at the Fire Department.</t>
+  </si>
+  <si>
+    <t>Ohio River</t>
   </si>
   <si>
     <t>The tornado then crossed the Ohio River again and lifted around two miles northwest of Metropolis just east of the airport.</t>
   </si>
   <si>
-    <t>Ill.</t>
-  </si>
-  <si>
-    <t>Storm shelters have been opened up for those in need in southern Ill. and southeast Mo.</t>
-  </si>
-  <si>
-    <t>Reports are the tornado touched down just southwest of Mounds, Ill. and crossed over I-57 near exit 8.</t>
-  </si>
-  <si>
-    <t>NWS reports are a tornado touched down just southwest of Mounds, Ill. and crossed over I-57 near exit 8.</t>
-  </si>
-  <si>
-    <t>Kansas</t>
-  </si>
-  <si>
-    <t>In Missouri, one person was killed in a trailer park in the town of Buffalo, and at least three people were critically injured in the small eastern Kansas town of Harveyville.</t>
-  </si>
-  <si>
-    <t>In neighboring Kansas, the National Weather Service reported brief tornado touchdowns southwest of Hutchinson, and Gov. Sam Brownback declared a state of emergency after an apparent tornado struck Harveyville.</t>
-  </si>
-  <si>
-    <t>One person was killed in Kansas.</t>
-  </si>
-  <si>
-    <t>"On behalf of the U.S. Department of Homeland Security's Federal Emergency Management Agency (FEMA), I would like to express our deepest condolences to the families of those who were killed and injured by tornadoes that impacted Kansas, Missouri and Nebraska late last night and into this morning.</t>
-  </si>
-  <si>
-    <t>Saline County</t>
-  </si>
-  <si>
-    <t>Crews with Ameren Illinois have issued a safety warning to all residents in and around Saline County.</t>
-  </si>
-  <si>
-    <t>The National Weather Service reports an EF4 tornado hit Saline County on the southwest side of Harrisburg, killing six people.</t>
-  </si>
-  <si>
-    <t>Four females and two males, all adults, were killed in Saline County.</t>
-  </si>
-  <si>
-    <t>Connecticut</t>
-  </si>
-  <si>
-    <t>Michigan, Connecticut and Massachusetts on Wednesday were spared from tornados but visited by snowy weather — a shock after this winter’s consistently warm temperatures.</t>
-  </si>
-  <si>
-    <t>The National Weather Service issued overnight advisories of snow and rain in all three states, warning of an ice coating followed by freezing rain in Michigan, a “bit of snow” followed by “lots of rain” in Connecticut, and up to 10 inches of snow in Eastern Massachusetts.</t>
-  </si>
-  <si>
-    <t>SEOC</t>
-  </si>
-  <si>
-    <t>IEMA regional personnel were deployed to Harrisburg soon after the storms and representatives from the Illinois State Police, departments of Transportation, Central Management Services, Corrections, Public Health and Natural Resources, along with the American Red Cross, reported to the SEOC soon thereafter.</t>
-  </si>
-  <si>
-    <t>The governor says the SEOC will remain activated as long as necessary.</t>
-  </si>
-  <si>
-    <t>Ameren Illinois</t>
-  </si>
-  <si>
-    <t>More than 400 people are working to restore power to Ameren Illinois customers.</t>
-  </si>
-  <si>
-    <t>People should not call 911 or the dispatch center to report power line outages, please contact Ameren Illinois direct.</t>
-  </si>
-  <si>
-    <t>Ameren Illinois doesn't have a time of when power will be restored.</t>
-  </si>
-  <si>
-    <t>As of 4:10 a.m. Thursday, Ameren Illinois reports outages in:  Copyright 2012 KFVS.</t>
-  </si>
-  <si>
-    <t>Saint Francis Medical Center</t>
-  </si>
-  <si>
-    <t>A total of eight patients from Stoddard County are being treated at Saint Francis Medical Center.</t>
-  </si>
-  <si>
-    <t>Mark Champlin, 50, of Puxico was pronounced dead at 7:35 a.m. at Saint Francis Medical Center in Cape Girardeau.</t>
-  </si>
-  <si>
-    <t>Heartland</t>
-  </si>
-  <si>
-    <t>5 confirmed tornadoes in the Heartland.</t>
-  </si>
-  <si>
-    <t>See pictures from across the Heartland after severe storms on Feb. 29, 2012.</t>
-  </si>
-  <si>
-    <t>See more pictures from across the Heartland after severe storms on Feb. 29, 2012.</t>
-  </si>
-  <si>
-    <t>See the National Weather Service storm damage reports from the tornadoes and severe storms that swept through the Heartland early Feb. 29.</t>
-  </si>
-  <si>
-    <t>How you can help after the tornadoes  How you can help after the tornadoes  Eight people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
-  </si>
-  <si>
-    <t>Seven of those tornadoes were in the Heartland.</t>
-  </si>
-  <si>
-    <t>Eight people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
-  </si>
-  <si>
-    <t>Disaster in the Heartland - one year later  Disaster in the Heartland - one year later  The storm drove this plywood piece through the wall of a garage in Harrisburg,  Seven people across the Heartland, 13 across the nation have died after at least 35 tornadoes touched down in 24 hours in the Midwest.</t>
-  </si>
-  <si>
-    <t>Five of those tornadoes were in the Heartland.</t>
-  </si>
-  <si>
-    <t>[More damage across the Heartland.]</t>
-  </si>
-  <si>
-    <t>Severe storms and tornadoes tear through the Heartland.</t>
-  </si>
-  <si>
-    <t>Missouri</t>
-  </si>
-  <si>
-    <t>One man was killed outside Puxico, Missouri in the storms.</t>
-  </si>
-  <si>
-    <t>Two people were killed in southwest Missouri.</t>
-  </si>
-  <si>
-    <t>Missouri Gov. Jan Nixon has declared a state of emergency.</t>
-  </si>
-  <si>
-    <t>Waves of strong storms devastated small communities and damaged the country music resort town of Branson, Missouri.</t>
-  </si>
-  <si>
-    <t>Stoddard County Coroner</t>
-  </si>
-  <si>
-    <t>The Stoddard County Coroner confirms one person has died as a result of overnight storms.</t>
-  </si>
-  <si>
-    <t>Mo.</t>
-  </si>
-  <si>
-    <t>Branson, Mo. tornado, National Weather Service snow alerts and more Leap Year weather.</t>
-  </si>
-  <si>
-    <t>A Puxico, Mo. man was killed in Stoddard County.</t>
-  </si>
-  <si>
-    <t>The school and a church sustained damage in Oak Ridge, Mo. in Cape Girardeau County.</t>
-  </si>
-  <si>
-    <t>First Baptist Church</t>
-  </si>
-  <si>
-    <t>According to the sheriff's office, the shelter is open at the First Baptist Church at 204 North Main Street.</t>
-  </si>
-  <si>
-    <t>Donations may be made to the Red Cross at the First Baptist Church, The Salvation Army at 10 West Locust in Harrisburg or Christian Compassion Care Center at PO Box 422 in Harrisburg.</t>
-  </si>
-  <si>
-    <t>Pulaski County</t>
-  </si>
-  <si>
-    <t>Pulaski County, Illinois EMS Director Ken Kerley says wreckers and vehicles were blown from their location and crossing arms broke off and blew into a squad car.</t>
-  </si>
-  <si>
-    <t>No injuries have been reported in Pulaski County.</t>
-  </si>
-  <si>
-    <t>Cape Girardeau County</t>
-  </si>
-  <si>
-    <t>Team 1 (Rick Shanklin, Ken Ludington) - Harrisburg west toward Cape Girardeau County MO  Team 2 (Kelly Hooper, Shane Luecke) - Newburg IN West toward Harrisburg IL)  Team 3 (Christine Wielgos, Debbie Hooper) - Metropolis IL west toward Stoddard co.</t>
-  </si>
-  <si>
-    <t>Stoddard County</t>
-  </si>
-  <si>
-    <t>You can drive for miles in Stoddard County and never see damage, but a path left from the strong winds that did blow through, show the wreckage.</t>
-  </si>
-  <si>
-    <t>The Stoddard County coroner says Mark Champlin, 50, of Puxico was killed.</t>
-  </si>
-  <si>
-    <t>A second tornado in Stoddard County Wednesday morning started just east of Bell City to three miles southeast of Benton, Mo.</t>
-  </si>
-  <si>
-    <t>One man has died after the storms in Stoddard County.</t>
-  </si>
-  <si>
-    <t>They are all storm related injuries from Stoddard County.</t>
-  </si>
-  <si>
-    <t>Stoddard County Sheriff Carl Hefner says several mobile homes in the area are destroyed in Stoddard County.</t>
-  </si>
-  <si>
-    <t>Stoddard County Coroner Aaron Mathis has released the name of the man killed in Puxico Wednesday morning after a tornado moved through the area.</t>
-  </si>
-  <si>
-    <t>Highway Patrol Trooper Clark Parrott says large trees are down along Route M in Stoddard County.</t>
-  </si>
-  <si>
-    <t>NWS</t>
-  </si>
-  <si>
-    <t>The NWS confirms preliminary reports of an EF2 tornado that went through McCracken and Ballard counties in Ky.</t>
-  </si>
-  <si>
-    <t>NWS teams were in Stoddard and Cape Girardeau counties on Thursday surveying damage.</t>
-  </si>
-  <si>
-    <t>An EF3 tornado was confirmed by the NWS.</t>
-  </si>
-  <si>
-    <t>According to NWS, numerous trees near the house were also uprooted.</t>
-  </si>
-  <si>
-    <t>Oak Ridge</t>
-  </si>
-  <si>
-    <t>People are using the school in Oak Ridge as a staging area to head out to help those in the area.</t>
-  </si>
-  <si>
-    <t>The Red Cross is providing food and water to residents and emergency workers in Oak Ridge as they work on cleaning up from the storm damage.</t>
-  </si>
-  <si>
-    <t>According to Emergency Management, all roads are back open in the Oak Ridge area.</t>
-  </si>
-  <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>America</t>
-  </si>
-  <si>
-    <t>The tornado then crossed the Ohio River near the town of America, then across McCracken and Ballard counties.</t>
-  </si>
-  <si>
-    <t>The tornado then crossed the Ohio River near the town of America, then across McCracken and Ballard Counties.</t>
-  </si>
-  <si>
-    <t>U.S.</t>
-  </si>
-  <si>
-    <t>The National Weather Service’s U.S. map Wednesday was covered by colorful wintry and storm warnings:</t>
-  </si>
-  <si>
-    <t>Corey Mead, lead forecaster at the U.S. Storm Prediction Center in Norman, Okla., said a broad cold front was slamming into warm, humid air over much of the eastern half of the nation.</t>
-  </si>
-  <si>
-    <t>Mo</t>
-  </si>
-  <si>
-    <t>Associated Press photographer Mark Schiefelbein contributed to this report from Branson, Mo.</t>
-  </si>
-  <si>
-    <t>The National Weather Service confirms preliminary reports of an EF2 in Marquand in Madison County, Mo.</t>
-  </si>
-  <si>
-    <t>Buffalo</t>
-  </si>
-  <si>
-    <t>Farther north, rescue crews waited for sunrise to begin searching a trailer park south of Buffalo where at least one person was killed after an apparent twister slammed the area.</t>
-  </si>
-  <si>
-    <t>Buffalo is about 35 miles north of Springfield.</t>
-  </si>
-  <si>
-    <t>Heartland News</t>
-  </si>
-  <si>
-    <t>The mayor of Harrisburg tells Heartland News that this is a horrific event.</t>
-  </si>
-  <si>
-    <t>Emergency Manager Dale Moreland tells Heartland News it looks like the mobile home  "exploded."</t>
-  </si>
-  <si>
-    <t>Moreland told Heartland News Wednesday morning that there is extensive damage everywhere, and power lines down across several miles.</t>
-  </si>
-  <si>
-    <t>Her sister, Judie LaChance tells Heartland News that Sandy Hemby will be okay.</t>
-  </si>
-  <si>
-    <t>Heartland News reporter Carly O'Keefe reports grain bins in fields and more damage in Gallatin County.</t>
-  </si>
-  <si>
-    <t>Red Cross</t>
-  </si>
-  <si>
-    <t>Oklahoma</t>
-  </si>
-  <si>
-    <t>In northern Oklahoma, gusts of up to 80 mph flipped trailers and damaged homes near Cherokee.</t>
-  </si>
-  <si>
-    <t>Arkansas</t>
-  </si>
-  <si>
-    <t>The system also skirted northern Arkansas, bringing gusts of up to 60 mph in the northwest.</t>
-  </si>
-  <si>
-    <t>Residents of Clay County in northeastern Arkansas reported hail the size of golf balls, while half dollar-sized hail was reported in Mountain Home.</t>
-  </si>
-  <si>
-    <t>Midwest</t>
-  </si>
-  <si>
-    <t>Three people were killed in Tennessee after the same severe weather system that created massive damage across the Midwest moved through the state.</t>
-  </si>
-  <si>
-    <t>Associated Press</t>
-  </si>
-  <si>
-    <t>JIM SALTER,Associated Press.</t>
-  </si>
-  <si>
-    <t>According to the Associated Press Darrell Osman says his mother, 75-year-old Mary Osman, was among the dead.</t>
-  </si>
-  <si>
-    <t>The Associated Press contributed to report.</t>
-  </si>
-  <si>
-    <t>Ameren</t>
-  </si>
-  <si>
-    <t>Ameren has open a customer service center in Harrisburg.</t>
-  </si>
-  <si>
-    <t>Ameren reports 14,000 without power at the peak.</t>
-  </si>
-  <si>
-    <t>Ameren hopes to have all power restored by the end of the day Friday.</t>
-  </si>
-  <si>
-    <t>Fire Department</t>
-  </si>
-  <si>
-    <t>Generators will be brought to the Oasis Tavern, just south of the Fire Department.</t>
-  </si>
-  <si>
-    <t>Food and drink is available at the Fire Department.</t>
-  </si>
-  <si>
-    <t>Ohio River</t>
-  </si>
-  <si>
     <t>Ballard Counties</t>
   </si>
   <si>
@@ -433,87 +424,81 @@
     <t>No major damage is reported in Puxico city limits.</t>
   </si>
   <si>
-    <t>Eldorado</t>
+    <t>FEMA</t>
+  </si>
+  <si>
+    <t>FEMA has been in constant contact with officials at the Kansas Department of Emergency Management (KDEM), Missouri State Emergency Management Agency (SEMA) and the Nebraska Emergency Management Agency (NEMA) since the severe weather hit.</t>
+  </si>
+  <si>
+    <t>FEMA Regional Administrator Beth Freeman released this statement.</t>
+  </si>
+  <si>
+    <t>Springfield</t>
+  </si>
+  <si>
+    <t>Earlier Wednesday, Gov. Quinn directed the Illinois Emergency Management Agency to activate the State Emergency Operations Center (SEOC) in Springfield.</t>
+  </si>
+  <si>
+    <t>Regular agency reports have been on the local Hometown Radio News all day, in addition to the Springfield television and network coverage.</t>
+  </si>
+  <si>
+    <t>Mounds</t>
+  </si>
+  <si>
+    <t>Harrisburg</t>
+  </si>
+  <si>
+    <t>The superintendent of schools in Harrisburg has canceled classes the rest of week.</t>
+  </si>
+  <si>
+    <t>Siteseers are asked to stay away from the City of Harrisburg.</t>
+  </si>
+  <si>
+    <t>At least 100 people have been injured in the Harrisburg area, according to the Saline County Sheriff's Office.</t>
+  </si>
+  <si>
+    <t>Harrisburg Police Chief Bob Smith says Rural King and the SIC foundation building are set up as meeting areas for manpower and equipment.</t>
+  </si>
+  <si>
+    <t>At least 300 houses have been damaged or destroyed with at least 25 businesses damaged or destroyed in the Harrisburg area, according to the sheriff's office.</t>
   </si>
   <si>
     <t>They are Mary Osman, 75, of Harrisburg, Jaylynn Ferrell, 22, of Harrisburg, Lynda Hull, 74, of Galatia, Donna Rann, 61, of Eldorado, and Randy Rann, 64, of Eldorado.</t>
   </si>
   <si>
-    <t>FEMA</t>
-  </si>
-  <si>
-    <t>FEMA Regional Administrator Beth Freeman released this statement.</t>
-  </si>
-  <si>
-    <t>FEMA has been in constant contact with officials at the Kansas Department of Emergency Management (KDEM), Missouri State Emergency Management Agency (SEMA) and the Nebraska Emergency Management Agency (NEMA) since the severe weather hit.</t>
-  </si>
-  <si>
-    <t>Springfield</t>
-  </si>
-  <si>
-    <t>Regular agency reports have been on the local Hometown Radio News all day, in addition to the Springfield television and network coverage.</t>
-  </si>
-  <si>
-    <t>Earlier Wednesday, Gov. Quinn directed the Illinois Emergency Management Agency to activate the State Emergency Operations Center (SEOC) in Springfield.</t>
-  </si>
-  <si>
-    <t>Mounds</t>
-  </si>
-  <si>
-    <t>Harrisburg</t>
+    <t>"This morning the city of Harrisburg suffered a horrific event," said Harrisburg mayor Eric Gregg.</t>
+  </si>
+  <si>
+    <t>Tyler Profilet reports a lot of damage in the Harrisburg area, including semi trucks tipped over.</t>
   </si>
   <si>
     <t>It touched down around 4:51 a.m. one mile north of Carrier Mills and traveled ENE toward Harrisburg, touching down in Harrisburg at 4:56 a.m.</t>
   </si>
   <si>
-    <t>"This morning the city of Harrisburg suffered a horrific event," said Harrisburg mayor Eric Gregg.</t>
-  </si>
-  <si>
-    <t>At least 100 people have been injured in the Harrisburg area, according to the Saline County Sheriff's Office.</t>
-  </si>
-  <si>
-    <t>At least 300 houses have been damaged or destroyed with at least 25 businesses damaged or destroyed in the Harrisburg area, according to the sheriff's office.</t>
-  </si>
-  <si>
-    <t>Siteseers are asked to stay away from the City of Harrisburg.</t>
-  </si>
-  <si>
-    <t>The superintendent of schools in Harrisburg has canceled classes the rest of week.</t>
-  </si>
-  <si>
-    <t>Tyler Profilet reports a lot of damage in the Harrisburg area, including semi trucks tipped over.</t>
+    <t>All volunteers in Harrisburg must register at the SIC Foundation building on North Commercial St. starting at 7 a.m. on March 1.</t>
+  </si>
+  <si>
+    <t>The United Way of South Central Illinois, located at 1101 Broadway in Mt. Vernon (the Old Integra Bank Building) will serve as a drop off site for items for the tornado victims in Harrisburg, IL.</t>
+  </si>
+  <si>
+    <t>HARRISBURG -- The Leap Day tornado that devastated parts of Harrisburg Tuesday completely destroyed the strip shopping center south of the Walmart parking lot and caused "significant roof and water damage" to Walmart itself.</t>
+  </si>
+  <si>
+    <t>Smith says 24/7 law enforcement protection will be available in Harrisburg for as long as needed.</t>
   </si>
   <si>
     <t>Several roads are block off in Harrisburg.</t>
   </si>
   <si>
-    <t>All volunteers in Harrisburg must register at the SIC Foundation building on North Commercial St. starting at 7 a.m. on March 1.</t>
-  </si>
-  <si>
-    <t>Harrisburg Police Chief Bob Smith says Rural King and the SIC foundation building are set up as meeting areas for manpower and equipment.</t>
-  </si>
-  <si>
-    <t>The United Way of South Central Illinois, located at 1101 Broadway in Mt. Vernon (the Old Integra Bank Building) will serve as a drop off site for items for the tornado victims in Harrisburg, IL.</t>
-  </si>
-  <si>
-    <t>Smith says 24/7 law enforcement protection will be available in Harrisburg for as long as needed.</t>
-  </si>
-  <si>
-    <t>HARRISBURG -- The Leap Day tornado that devastated parts of Harrisburg Tuesday completely destroyed the strip shopping center south of the Walmart parking lot and caused "significant roof and water damage" to Walmart itself.</t>
-  </si>
-  <si>
-    <t>Walmart</t>
-  </si>
-  <si>
     <t>Ridgway</t>
   </si>
   <si>
+    <t>The roads in Ridgway are closed to through traffic.</t>
+  </si>
+  <si>
     <t>One with serious injuries and the rest minor injuries  She says Tin Shop Hardware Store in Ridgway crushed by wind.</t>
   </si>
   <si>
-    <t>The roads in Ridgway are closed to through traffic.</t>
-  </si>
-  <si>
     <t>Town officials have established a curfew from 9 a.m. to 6 a.m. in Ridgway.</t>
   </si>
   <si>
@@ -529,15 +514,15 @@
     <t>Kentucky</t>
   </si>
   <si>
+    <t>A National Weather Service team has determined at least 1 of the strong storms that swept through Kentucky was an EF2 tornado packing winds of 125 miles per hour.</t>
+  </si>
+  <si>
+    <t>MO)  Note this may change as storms are in western Kentucky.</t>
+  </si>
+  <si>
     <t>Tornado warnings and watches were posted for most of Kentucky and a large portion of Kentucky.</t>
   </si>
   <si>
-    <t>A National Weather Service team has determined at least 1 of the strong storms that swept through Kentucky was an EF2 tornado packing winds of 125 miles per hour.</t>
-  </si>
-  <si>
-    <t>MO)  Note this may change as storms are in western Kentucky.</t>
-  </si>
-  <si>
     <t>Wal-Mart</t>
   </si>
   <si>
@@ -553,13 +538,13 @@
     <t>National Weather Service</t>
   </si>
   <si>
+    <t>The National Weather Service is sending three teams to survey the damage.</t>
+  </si>
+  <si>
+    <t>Preliminary reports from the National Weather Service report large oak trees were found uprooted and damage to roofs was consistent with EF1 damage on the enhanced Fujita scale.</t>
+  </si>
+  <si>
     <t>Some Leap Year babies woke up Wednesday to find their uncommon birthday plagued by school closings, National Weather Service snow alerts and even a tornado.</t>
-  </si>
-  <si>
-    <t>Preliminary reports from the National Weather Service report large oak trees were found uprooted and damage to roofs was consistent with EF1 damage on the enhanced Fujita scale.</t>
-  </si>
-  <si>
-    <t>The National Weather Service is sending three teams to survey the damage.</t>
   </si>
   <si>
     <t>Tennessee</t>
@@ -903,7 +888,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C240"/>
+  <dimension ref="A1:C207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -961,7 +946,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -972,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -983,7 +968,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -994,7 +979,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1005,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1016,7 +1001,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1027,7 +1012,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1035,10 +1020,10 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1049,7 +1034,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1060,7 +1045,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1068,10 +1053,10 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1079,10 +1064,10 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1090,10 +1075,10 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1101,10 +1086,10 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1112,10 +1097,10 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1123,10 +1108,10 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1134,10 +1119,10 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1145,10 +1130,10 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1156,10 +1141,10 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1167,10 +1152,10 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1178,10 +1163,10 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1189,10 +1174,10 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1200,10 +1185,10 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1211,10 +1196,10 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1222,10 +1207,10 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1233,10 +1218,10 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1244,10 +1229,10 @@
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1255,10 +1240,10 @@
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1266,10 +1251,10 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1277,10 +1262,10 @@
         <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1288,10 +1273,10 @@
         <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1299,10 +1284,10 @@
         <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1310,10 +1295,10 @@
         <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1321,10 +1306,10 @@
         <v>0</v>
       </c>
       <c r="B38" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1332,10 +1317,10 @@
         <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1343,10 +1328,10 @@
         <v>0</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1354,10 +1339,10 @@
         <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1365,10 +1350,10 @@
         <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1376,10 +1361,10 @@
         <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1387,10 +1372,10 @@
         <v>0</v>
       </c>
       <c r="B44" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1398,10 +1383,10 @@
         <v>0</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C45" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1409,10 +1394,10 @@
         <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C46" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1420,10 +1405,10 @@
         <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C47" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1431,10 +1416,10 @@
         <v>0</v>
       </c>
       <c r="B48" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1442,10 +1427,10 @@
         <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1453,10 +1438,10 @@
         <v>0</v>
       </c>
       <c r="B50" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1464,10 +1449,10 @@
         <v>0</v>
       </c>
       <c r="B51" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C51" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1475,10 +1460,10 @@
         <v>0</v>
       </c>
       <c r="B52" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C52" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1486,10 +1471,10 @@
         <v>0</v>
       </c>
       <c r="B53" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1497,10 +1482,10 @@
         <v>0</v>
       </c>
       <c r="B54" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1508,10 +1493,10 @@
         <v>0</v>
       </c>
       <c r="B55" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C55" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1519,10 +1504,10 @@
         <v>0</v>
       </c>
       <c r="B56" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C56" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1530,10 +1515,10 @@
         <v>0</v>
       </c>
       <c r="B57" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C57" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1541,10 +1526,10 @@
         <v>0</v>
       </c>
       <c r="B58" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C58" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1552,10 +1537,10 @@
         <v>0</v>
       </c>
       <c r="B59" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C59" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1563,10 +1548,10 @@
         <v>0</v>
       </c>
       <c r="B60" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="C60" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1574,10 +1559,10 @@
         <v>0</v>
       </c>
       <c r="B61" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C61" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1585,10 +1570,10 @@
         <v>0</v>
       </c>
       <c r="B62" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C62" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1596,10 +1581,10 @@
         <v>0</v>
       </c>
       <c r="B63" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C63" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1607,10 +1592,10 @@
         <v>0</v>
       </c>
       <c r="B64" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C64" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1618,10 +1603,10 @@
         <v>0</v>
       </c>
       <c r="B65" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C65" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1629,10 +1614,10 @@
         <v>0</v>
       </c>
       <c r="B66" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C66" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1640,10 +1625,10 @@
         <v>0</v>
       </c>
       <c r="B67" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C67" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1651,10 +1636,10 @@
         <v>0</v>
       </c>
       <c r="B68" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C68" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1662,10 +1647,10 @@
         <v>0</v>
       </c>
       <c r="B69" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C69" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1673,10 +1658,10 @@
         <v>0</v>
       </c>
       <c r="B70" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C70" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1684,10 +1669,10 @@
         <v>0</v>
       </c>
       <c r="B71" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C71" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1695,10 +1680,10 @@
         <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C72" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1706,10 +1691,10 @@
         <v>0</v>
       </c>
       <c r="B73" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C73" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1717,10 +1702,10 @@
         <v>0</v>
       </c>
       <c r="B74" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C74" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1728,10 +1713,10 @@
         <v>0</v>
       </c>
       <c r="B75" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C75" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1739,10 +1724,10 @@
         <v>0</v>
       </c>
       <c r="B76" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C76" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1750,10 +1735,10 @@
         <v>0</v>
       </c>
       <c r="B77" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C77" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1761,10 +1746,10 @@
         <v>0</v>
       </c>
       <c r="B78" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C78" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1772,10 +1757,10 @@
         <v>0</v>
       </c>
       <c r="B79" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C79" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1783,10 +1768,10 @@
         <v>0</v>
       </c>
       <c r="B80" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C80" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1794,10 +1779,10 @@
         <v>0</v>
       </c>
       <c r="B81" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="C81" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1805,10 +1790,10 @@
         <v>0</v>
       </c>
       <c r="B82" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C82" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1816,10 +1801,10 @@
         <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C83" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1827,10 +1812,10 @@
         <v>0</v>
       </c>
       <c r="B84" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C84" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1838,10 +1823,10 @@
         <v>0</v>
       </c>
       <c r="B85" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C85" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1849,10 +1834,10 @@
         <v>0</v>
       </c>
       <c r="B86" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C86" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1860,10 +1845,10 @@
         <v>0</v>
       </c>
       <c r="B87" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="C87" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1871,10 +1856,10 @@
         <v>0</v>
       </c>
       <c r="B88" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="C88" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1882,10 +1867,10 @@
         <v>0</v>
       </c>
       <c r="B89" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="C89" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1893,10 +1878,10 @@
         <v>0</v>
       </c>
       <c r="B90" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="C90" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1904,10 +1889,10 @@
         <v>0</v>
       </c>
       <c r="B91" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="C91" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1915,10 +1900,10 @@
         <v>0</v>
       </c>
       <c r="B92" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="C92" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1926,10 +1911,10 @@
         <v>0</v>
       </c>
       <c r="B93" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="C93" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1937,10 +1922,10 @@
         <v>0</v>
       </c>
       <c r="B94" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C94" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1948,10 +1933,10 @@
         <v>0</v>
       </c>
       <c r="B95" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C95" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1959,10 +1944,10 @@
         <v>0</v>
       </c>
       <c r="B96" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C96" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1970,10 +1955,10 @@
         <v>0</v>
       </c>
       <c r="B97" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C97" t="s">
-        <v>86</v>
+        <v>18</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1981,10 +1966,10 @@
         <v>0</v>
       </c>
       <c r="B98" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="C98" t="s">
-        <v>18</v>
+        <v>101</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1992,10 +1977,10 @@
         <v>0</v>
       </c>
       <c r="B99" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C99" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2003,10 +1988,10 @@
         <v>0</v>
       </c>
       <c r="B100" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C100" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2014,10 +1999,10 @@
         <v>0</v>
       </c>
       <c r="B101" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C101" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2025,10 +2010,10 @@
         <v>0</v>
       </c>
       <c r="B102" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C102" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2036,10 +2021,10 @@
         <v>0</v>
       </c>
       <c r="B103" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="C103" t="s">
-        <v>29</v>
+        <v>84</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2047,10 +2032,10 @@
         <v>0</v>
       </c>
       <c r="B104" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="C104" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2058,10 +2043,10 @@
         <v>0</v>
       </c>
       <c r="B105" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C105" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2069,10 +2054,10 @@
         <v>0</v>
       </c>
       <c r="B106" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C106" t="s">
-        <v>94</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2080,10 +2065,10 @@
         <v>0</v>
       </c>
       <c r="B107" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="C107" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2091,10 +2076,10 @@
         <v>0</v>
       </c>
       <c r="B108" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="C108" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2102,10 +2087,10 @@
         <v>0</v>
       </c>
       <c r="B109" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="C109" t="s">
-        <v>99</v>
+        <v>12</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2113,10 +2098,10 @@
         <v>0</v>
       </c>
       <c r="B110" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="C110" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2124,10 +2109,10 @@
         <v>0</v>
       </c>
       <c r="B111" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="C111" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2135,10 +2120,10 @@
         <v>0</v>
       </c>
       <c r="B112" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="C112" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2146,10 +2131,10 @@
         <v>0</v>
       </c>
       <c r="B113" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="C113" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2157,10 +2142,10 @@
         <v>0</v>
       </c>
       <c r="B114" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="C114" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2168,10 +2153,10 @@
         <v>0</v>
       </c>
       <c r="B115" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="C115" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2179,10 +2164,10 @@
         <v>0</v>
       </c>
       <c r="B116" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="C116" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2190,10 +2175,10 @@
         <v>0</v>
       </c>
       <c r="B117" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="C117" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2201,10 +2186,10 @@
         <v>0</v>
       </c>
       <c r="B118" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="C118" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2212,10 +2197,10 @@
         <v>0</v>
       </c>
       <c r="B119" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="C119" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2223,10 +2208,10 @@
         <v>0</v>
       </c>
       <c r="B120" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="C120" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2234,10 +2219,10 @@
         <v>0</v>
       </c>
       <c r="B121" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="C121" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2245,10 +2230,10 @@
         <v>0</v>
       </c>
       <c r="B122" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="C122" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2256,10 +2241,10 @@
         <v>0</v>
       </c>
       <c r="B123" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="C123" t="s">
-        <v>89</v>
+        <v>124</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2267,10 +2252,10 @@
         <v>0</v>
       </c>
       <c r="B124" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="C124" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2278,10 +2263,10 @@
         <v>0</v>
       </c>
       <c r="B125" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="C125" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2289,10 +2274,10 @@
         <v>0</v>
       </c>
       <c r="B126" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="C126" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2300,10 +2285,10 @@
         <v>0</v>
       </c>
       <c r="B127" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="C127" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2311,10 +2296,10 @@
         <v>0</v>
       </c>
       <c r="B128" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="C128" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2322,10 +2307,10 @@
         <v>0</v>
       </c>
       <c r="B129" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="C129" t="s">
-        <v>47</v>
+        <v>130</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2333,10 +2318,10 @@
         <v>0</v>
       </c>
       <c r="B130" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="C130" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2344,10 +2329,10 @@
         <v>0</v>
       </c>
       <c r="B131" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="C131" t="s">
-        <v>50</v>
+        <v>128</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2355,10 +2340,10 @@
         <v>0</v>
       </c>
       <c r="B132" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="C132" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2366,10 +2351,10 @@
         <v>0</v>
       </c>
       <c r="B133" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="C133" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2377,10 +2362,10 @@
         <v>0</v>
       </c>
       <c r="B134" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="C134" t="s">
-        <v>119</v>
+        <v>39</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2388,10 +2373,10 @@
         <v>0</v>
       </c>
       <c r="B135" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="C135" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2399,10 +2384,10 @@
         <v>0</v>
       </c>
       <c r="B136" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="C136" t="s">
-        <v>120</v>
+        <v>73</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2410,10 +2395,10 @@
         <v>0</v>
       </c>
       <c r="B137" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="C137" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2421,10 +2406,10 @@
         <v>0</v>
       </c>
       <c r="B138" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C138" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2432,10 +2417,10 @@
         <v>0</v>
       </c>
       <c r="B139" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C139" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2443,10 +2428,10 @@
         <v>0</v>
       </c>
       <c r="B140" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="C140" t="s">
-        <v>124</v>
+        <v>19</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2454,10 +2439,10 @@
         <v>0</v>
       </c>
       <c r="B141" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="C141" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2465,10 +2450,10 @@
         <v>0</v>
       </c>
       <c r="B142" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="C142" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2476,10 +2461,10 @@
         <v>0</v>
       </c>
       <c r="B143" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="C143" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2487,10 +2472,10 @@
         <v>0</v>
       </c>
       <c r="B144" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="C144" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2498,10 +2483,10 @@
         <v>0</v>
       </c>
       <c r="B145" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="C145" t="s">
-        <v>14</v>
+        <v>141</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2509,10 +2494,10 @@
         <v>0</v>
       </c>
       <c r="B146" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="C146" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2520,10 +2505,10 @@
         <v>0</v>
       </c>
       <c r="B147" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="C147" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2531,10 +2516,10 @@
         <v>0</v>
       </c>
       <c r="B148" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="C148" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2542,10 +2527,10 @@
         <v>0</v>
       </c>
       <c r="B149" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="C149" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2553,10 +2538,10 @@
         <v>0</v>
       </c>
       <c r="B150" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="C150" t="s">
-        <v>100</v>
+        <v>145</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2564,10 +2549,10 @@
         <v>0</v>
       </c>
       <c r="B151" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="C151" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2575,10 +2560,10 @@
         <v>0</v>
       </c>
       <c r="B152" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C152" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2586,10 +2571,10 @@
         <v>0</v>
       </c>
       <c r="B153" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C153" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2597,10 +2582,10 @@
         <v>0</v>
       </c>
       <c r="B154" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="C154" t="s">
-        <v>55</v>
+        <v>147</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2608,10 +2593,10 @@
         <v>0</v>
       </c>
       <c r="B155" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="C155" t="s">
-        <v>55</v>
+        <v>148</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2619,10 +2604,10 @@
         <v>0</v>
       </c>
       <c r="B156" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="C156" t="s">
-        <v>75</v>
+        <v>149</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2630,10 +2615,10 @@
         <v>0</v>
       </c>
       <c r="B157" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="C157" t="s">
-        <v>136</v>
+        <v>105</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2641,10 +2626,10 @@
         <v>0</v>
       </c>
       <c r="B158" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="C158" t="s">
-        <v>80</v>
+        <v>150</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2652,10 +2637,10 @@
         <v>0</v>
       </c>
       <c r="B159" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="C159" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2663,10 +2648,10 @@
         <v>0</v>
       </c>
       <c r="B160" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="C160" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2674,10 +2659,10 @@
         <v>0</v>
       </c>
       <c r="B161" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="C161" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2685,10 +2670,10 @@
         <v>0</v>
       </c>
       <c r="B162" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C162" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2696,10 +2681,10 @@
         <v>0</v>
       </c>
       <c r="B163" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C163" t="s">
-        <v>140</v>
+        <v>6</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2707,10 +2692,10 @@
         <v>0</v>
       </c>
       <c r="B164" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C164" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2718,10 +2703,10 @@
         <v>0</v>
       </c>
       <c r="B165" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C165" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -2729,10 +2714,10 @@
         <v>0</v>
       </c>
       <c r="B166" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C166" t="s">
-        <v>143</v>
+        <v>62</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -2740,10 +2725,10 @@
         <v>0</v>
       </c>
       <c r="B167" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C167" t="s">
-        <v>103</v>
+        <v>155</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2751,10 +2736,10 @@
         <v>0</v>
       </c>
       <c r="B168" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C168" t="s">
-        <v>145</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -2762,10 +2747,10 @@
         <v>0</v>
       </c>
       <c r="B169" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C169" t="s">
-        <v>146</v>
+        <v>24</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -2773,10 +2758,10 @@
         <v>0</v>
       </c>
       <c r="B170" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C170" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -2784,10 +2769,10 @@
         <v>0</v>
       </c>
       <c r="B171" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C171" t="s">
-        <v>18</v>
+        <v>157</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -2795,10 +2780,10 @@
         <v>0</v>
       </c>
       <c r="B172" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C172" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -2806,10 +2791,10 @@
         <v>0</v>
       </c>
       <c r="B173" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C173" t="s">
-        <v>123</v>
+        <v>159</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -2817,10 +2802,10 @@
         <v>0</v>
       </c>
       <c r="B174" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C174" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -2828,10 +2813,10 @@
         <v>0</v>
       </c>
       <c r="B175" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C175" t="s">
-        <v>50</v>
+        <v>161</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -2839,10 +2824,10 @@
         <v>0</v>
       </c>
       <c r="B176" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="C176" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -2850,10 +2835,10 @@
         <v>0</v>
       </c>
       <c r="B177" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="C177" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -2861,10 +2846,10 @@
         <v>0</v>
       </c>
       <c r="B178" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="C178" t="s">
-        <v>149</v>
+        <v>39</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -2872,10 +2857,10 @@
         <v>0</v>
       </c>
       <c r="B179" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="C179" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -2883,10 +2868,10 @@
         <v>0</v>
       </c>
       <c r="B180" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="C180" t="s">
-        <v>140</v>
+        <v>5</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -2894,10 +2879,10 @@
         <v>0</v>
       </c>
       <c r="B181" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="C181" t="s">
-        <v>7</v>
+        <v>166</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -2905,10 +2890,10 @@
         <v>0</v>
       </c>
       <c r="B182" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="C182" t="s">
-        <v>8</v>
+        <v>167</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -2916,10 +2901,10 @@
         <v>0</v>
       </c>
       <c r="B183" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="C183" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -2927,10 +2912,10 @@
         <v>0</v>
       </c>
       <c r="B184" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="C184" t="s">
-        <v>150</v>
+        <v>12</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -2938,10 +2923,10 @@
         <v>0</v>
       </c>
       <c r="B185" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="C185" t="s">
-        <v>32</v>
+        <v>170</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -2949,10 +2934,10 @@
         <v>0</v>
       </c>
       <c r="B186" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="C186" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -2960,10 +2945,10 @@
         <v>0</v>
       </c>
       <c r="B187" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="C187" t="s">
-        <v>152</v>
+        <v>5</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -2971,10 +2956,10 @@
         <v>0</v>
       </c>
       <c r="B188" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="C188" t="s">
-        <v>153</v>
+        <v>19</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -2982,10 +2967,10 @@
         <v>0</v>
       </c>
       <c r="B189" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="C189" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -2993,10 +2978,10 @@
         <v>0</v>
       </c>
       <c r="B190" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="C190" t="s">
-        <v>154</v>
+        <v>59</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3004,10 +2989,10 @@
         <v>0</v>
       </c>
       <c r="B191" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="C191" t="s">
-        <v>155</v>
+        <v>96</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3015,10 +3000,10 @@
         <v>0</v>
       </c>
       <c r="B192" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="C192" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -3026,10 +3011,10 @@
         <v>0</v>
       </c>
       <c r="B193" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="C193" t="s">
-        <v>157</v>
+        <v>5</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3037,10 +3022,10 @@
         <v>0</v>
       </c>
       <c r="B194" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="C194" t="s">
-        <v>158</v>
+        <v>24</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -3048,10 +3033,10 @@
         <v>0</v>
       </c>
       <c r="B195" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="C195" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -3059,10 +3044,10 @@
         <v>0</v>
       </c>
       <c r="B196" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="C196" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -3070,10 +3055,10 @@
         <v>0</v>
       </c>
       <c r="B197" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="C197" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -3081,10 +3066,10 @@
         <v>0</v>
       </c>
       <c r="B198" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="C198" t="s">
-        <v>160</v>
+        <v>93</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -3092,10 +3077,10 @@
         <v>0</v>
       </c>
       <c r="B199" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="C199" t="s">
-        <v>72</v>
+        <v>166</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -3103,10 +3088,10 @@
         <v>0</v>
       </c>
       <c r="B200" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="C200" t="s">
-        <v>72</v>
+        <v>175</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -3114,10 +3099,10 @@
         <v>0</v>
       </c>
       <c r="B201" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="C201" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -3125,10 +3110,10 @@
         <v>0</v>
       </c>
       <c r="B202" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="C202" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -3136,10 +3121,10 @@
         <v>0</v>
       </c>
       <c r="B203" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="C203" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -3147,10 +3132,10 @@
         <v>0</v>
       </c>
       <c r="B204" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="C204" t="s">
-        <v>161</v>
+        <v>113</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -3158,10 +3143,10 @@
         <v>0</v>
       </c>
       <c r="B205" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="C205" t="s">
-        <v>164</v>
+        <v>12</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -3169,10 +3154,10 @@
         <v>0</v>
       </c>
       <c r="B206" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="C206" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -3180,373 +3165,10 @@
         <v>0</v>
       </c>
       <c r="B207" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="C207" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3">
-      <c r="A208" t="s">
-        <v>0</v>
-      </c>
-      <c r="B208" t="s">
-        <v>167</v>
-      </c>
-      <c r="C208" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3">
-      <c r="A209" t="s">
-        <v>0</v>
-      </c>
-      <c r="B209" t="s">
-        <v>167</v>
-      </c>
-      <c r="C209" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3">
-      <c r="A210" t="s">
-        <v>0</v>
-      </c>
-      <c r="B210" t="s">
-        <v>167</v>
-      </c>
-      <c r="C210" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3">
-      <c r="A211" t="s">
-        <v>0</v>
-      </c>
-      <c r="B211" t="s">
-        <v>167</v>
-      </c>
-      <c r="C211" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3">
-      <c r="A212" t="s">
-        <v>0</v>
-      </c>
-      <c r="B212" t="s">
-        <v>170</v>
-      </c>
-      <c r="C212" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3">
-      <c r="A213" t="s">
-        <v>0</v>
-      </c>
-      <c r="B213" t="s">
-        <v>170</v>
-      </c>
-      <c r="C213" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3">
-      <c r="A214" t="s">
-        <v>0</v>
-      </c>
-      <c r="B214" t="s">
-        <v>170</v>
-      </c>
-      <c r="C214" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3">
-      <c r="A215" t="s">
-        <v>0</v>
-      </c>
-      <c r="B215" t="s">
-        <v>170</v>
-      </c>
-      <c r="C215" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3">
-      <c r="A216" t="s">
-        <v>0</v>
-      </c>
-      <c r="B216" t="s">
-        <v>170</v>
-      </c>
-      <c r="C216" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3">
-      <c r="A217" t="s">
-        <v>0</v>
-      </c>
-      <c r="B217" t="s">
-        <v>170</v>
-      </c>
-      <c r="C217" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3">
-      <c r="A218" t="s">
-        <v>0</v>
-      </c>
-      <c r="B218" t="s">
-        <v>174</v>
-      </c>
-      <c r="C218" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3">
-      <c r="A219" t="s">
-        <v>0</v>
-      </c>
-      <c r="B219" t="s">
-        <v>174</v>
-      </c>
-      <c r="C219" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3">
-      <c r="A220" t="s">
-        <v>0</v>
-      </c>
-      <c r="B220" t="s">
-        <v>177</v>
-      </c>
-      <c r="C220" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3">
-      <c r="A221" t="s">
-        <v>0</v>
-      </c>
-      <c r="B221" t="s">
-        <v>177</v>
-      </c>
-      <c r="C221" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3">
-      <c r="A222" t="s">
-        <v>0</v>
-      </c>
-      <c r="B222" t="s">
-        <v>178</v>
-      </c>
-      <c r="C222" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3">
-      <c r="A223" t="s">
-        <v>0</v>
-      </c>
-      <c r="B223" t="s">
-        <v>178</v>
-      </c>
-      <c r="C223" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3">
-      <c r="A224" t="s">
-        <v>0</v>
-      </c>
-      <c r="B224" t="s">
-        <v>178</v>
-      </c>
-      <c r="C224" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3">
-      <c r="A225" t="s">
-        <v>0</v>
-      </c>
-      <c r="B225" t="s">
-        <v>178</v>
-      </c>
-      <c r="C225" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3">
-      <c r="A226" t="s">
-        <v>0</v>
-      </c>
-      <c r="B226" t="s">
-        <v>178</v>
-      </c>
-      <c r="C226" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3">
-      <c r="A227" t="s">
-        <v>0</v>
-      </c>
-      <c r="B227" t="s">
-        <v>178</v>
-      </c>
-      <c r="C227" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3">
-      <c r="A228" t="s">
-        <v>0</v>
-      </c>
-      <c r="B228" t="s">
-        <v>178</v>
-      </c>
-      <c r="C228" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3">
-      <c r="A229" t="s">
-        <v>0</v>
-      </c>
-      <c r="B229" t="s">
-        <v>178</v>
-      </c>
-      <c r="C229" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3">
-      <c r="A230" t="s">
-        <v>0</v>
-      </c>
-      <c r="B230" t="s">
-        <v>178</v>
-      </c>
-      <c r="C230" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3">
-      <c r="A231" t="s">
-        <v>0</v>
-      </c>
-      <c r="B231" t="s">
-        <v>178</v>
-      </c>
-      <c r="C231" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3">
-      <c r="A232" t="s">
-        <v>0</v>
-      </c>
-      <c r="B232" t="s">
-        <v>178</v>
-      </c>
-      <c r="C232" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3">
-      <c r="A233" t="s">
-        <v>0</v>
-      </c>
-      <c r="B233" t="s">
-        <v>178</v>
-      </c>
-      <c r="C233" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3">
-      <c r="A234" t="s">
-        <v>0</v>
-      </c>
-      <c r="B234" t="s">
-        <v>178</v>
-      </c>
-      <c r="C234" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3">
-      <c r="A235" t="s">
-        <v>0</v>
-      </c>
-      <c r="B235" t="s">
-        <v>178</v>
-      </c>
-      <c r="C235" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3">
-      <c r="A236" t="s">
-        <v>0</v>
-      </c>
-      <c r="B236" t="s">
-        <v>182</v>
-      </c>
-      <c r="C236" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3">
-      <c r="A237" t="s">
-        <v>0</v>
-      </c>
-      <c r="B237" t="s">
-        <v>182</v>
-      </c>
-      <c r="C237" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3">
-      <c r="A238" t="s">
-        <v>0</v>
-      </c>
-      <c r="B238" t="s">
-        <v>182</v>
-      </c>
-      <c r="C238" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3">
-      <c r="A239" t="s">
-        <v>0</v>
-      </c>
-      <c r="B239" t="s">
-        <v>184</v>
-      </c>
-      <c r="C239" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3">
-      <c r="A240" t="s">
-        <v>0</v>
-      </c>
-      <c r="B240" t="s">
-        <v>184</v>
-      </c>
-      <c r="C240" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>